<commit_message>
Update the code - Delete the InsertDB in comp_percentile_rank code
</commit_message>
<xml_diff>
--- a/input/comp_mrs_cat.xlsx
+++ b/input/comp_mrs_cat.xlsx
@@ -689,13 +689,13 @@
         <v>-1.16216567582168</v>
       </c>
       <c r="AE2" t="n">
-        <v>11.76416224525098</v>
+        <v>11.77990626116324</v>
       </c>
       <c r="AF2" t="n">
         <v>1.21525785660293</v>
       </c>
       <c r="AG2" t="n">
-        <v>9.386738712826366</v>
+        <v>9.402482728738628</v>
       </c>
     </row>
     <row r="3">
@@ -792,13 +792,13 @@
         <v>-2.479977037671318</v>
       </c>
       <c r="AE3" t="n">
-        <v>14.05583384716671</v>
+        <v>14.09549045834902</v>
       </c>
       <c r="AF3" t="n">
         <v>1.907476798064713</v>
       </c>
       <c r="AG3" t="n">
-        <v>9.668380011430678</v>
+        <v>9.708036622612987</v>
       </c>
     </row>
     <row r="4">
@@ -895,13 +895,13 @@
         <v>-1.234927003671412</v>
       </c>
       <c r="AE4" t="n">
-        <v>11.98641283502654</v>
+        <v>12.05507120829597</v>
       </c>
       <c r="AF4" t="n">
         <v>3.004803121989122</v>
       </c>
       <c r="AG4" t="n">
-        <v>7.746682709366008</v>
+        <v>7.81534108263544</v>
       </c>
     </row>
     <row r="5">
@@ -998,13 +998,13 @@
         <v>-1.468658039209249</v>
       </c>
       <c r="AE5" t="n">
-        <v>15.03230109234258</v>
+        <v>15.14395095318842</v>
       </c>
       <c r="AF5" t="n">
         <v>2.79833508502352</v>
       </c>
       <c r="AG5" t="n">
-        <v>10.76530796810981</v>
+        <v>10.87695782895565</v>
       </c>
     </row>
     <row r="6">
@@ -1101,13 +1101,13 @@
         <v>-0.9005002960522448</v>
       </c>
       <c r="AE6" t="n">
-        <v>11.35313086523678</v>
+        <v>11.41663563776412</v>
       </c>
       <c r="AF6" t="n">
         <v>1.398649254021426</v>
       </c>
       <c r="AG6" t="n">
-        <v>9.05398131516311</v>
+        <v>9.117486087690445</v>
       </c>
     </row>
     <row r="7">
@@ -1204,13 +1204,13 @@
         <v>-2.116910323168911</v>
       </c>
       <c r="AE7" t="n">
-        <v>11.45931372047049</v>
+        <v>11.5961704773125</v>
       </c>
       <c r="AF7" t="n">
         <v>2.713662913782229</v>
       </c>
       <c r="AG7" t="n">
-        <v>6.628740483519354</v>
+        <v>6.765597240361365</v>
       </c>
     </row>
     <row r="8">
@@ -1307,13 +1307,13 @@
         <v>-2.960680884375331</v>
       </c>
       <c r="AE8" t="n">
-        <v>11.41887266656564</v>
+        <v>11.52701059773078</v>
       </c>
       <c r="AF8" t="n">
         <v>3.149142237757889</v>
       </c>
       <c r="AG8" t="n">
-        <v>5.309049544432419</v>
+        <v>5.417187475597562</v>
       </c>
     </row>
     <row r="9">
@@ -1410,13 +1410,13 @@
         <v>-3.614753164174113</v>
       </c>
       <c r="AE9" t="n">
-        <v>11.74983015064569</v>
+        <v>11.96681525992708</v>
       </c>
       <c r="AF9" t="n">
         <v>3.276139743624471</v>
       </c>
       <c r="AG9" t="n">
-        <v>4.858937242847105</v>
+        <v>5.075922352128496</v>
       </c>
     </row>
     <row r="10">
@@ -1513,13 +1513,13 @@
         <v>-0.6538190124457182</v>
       </c>
       <c r="AE10" t="n">
-        <v>9.544879131168509</v>
+        <v>9.860478640744111</v>
       </c>
       <c r="AF10" t="n">
         <v>3.828349514488567</v>
       </c>
       <c r="AG10" t="n">
-        <v>5.062710604234224</v>
+        <v>5.378310113809826</v>
       </c>
     </row>
     <row r="11">
@@ -1616,13 +1616,13 @@
         <v>-2.101063399074429</v>
       </c>
       <c r="AE11" t="n">
-        <v>10.22504984930396</v>
+        <v>10.60976684966777</v>
       </c>
       <c r="AF11" t="n">
         <v>3.84770481406579</v>
       </c>
       <c r="AG11" t="n">
-        <v>4.276281636163737</v>
+        <v>4.660998636527554</v>
       </c>
     </row>
     <row r="12">
@@ -1719,13 +1719,13 @@
         <v>-1.51729773178816</v>
       </c>
       <c r="AE12" t="n">
-        <v>13.19869851427879</v>
+        <v>13.2386734764729</v>
       </c>
       <c r="AF12" t="n">
         <v>2.289331898834243</v>
       </c>
       <c r="AG12" t="n">
-        <v>9.392068883656387</v>
+        <v>9.432043845850497</v>
       </c>
     </row>
     <row r="13">
@@ -1822,13 +1822,13 @@
         <v>-0.8013112033540528</v>
       </c>
       <c r="AE13" t="n">
-        <v>11.82195185723116</v>
+        <v>11.88895917226999</v>
       </c>
       <c r="AF13" t="n">
         <v>1.034388269386078</v>
       </c>
       <c r="AG13" t="n">
-        <v>9.986252384491028</v>
+        <v>10.05325969952986</v>
       </c>
     </row>
     <row r="14">
@@ -1925,13 +1925,13 @@
         <v>-2.089801509041681</v>
       </c>
       <c r="AE14" t="n">
-        <v>9.830301088355027</v>
+        <v>10.16256479919443</v>
       </c>
       <c r="AF14" t="n">
         <v>3.641193771392695</v>
       </c>
       <c r="AG14" t="n">
-        <v>4.099305807920651</v>
+        <v>4.431569518760055</v>
       </c>
     </row>
     <row r="15">
@@ -2028,13 +2028,13 @@
         <v>-0.3942163585171082</v>
       </c>
       <c r="AE15" t="n">
-        <v>14.78919381101481</v>
+        <v>14.79637055232094</v>
       </c>
       <c r="AF15" t="n">
         <v>1.785537558360071</v>
       </c>
       <c r="AG15" t="n">
-        <v>12.60943989413764</v>
+        <v>12.61661663544376</v>
       </c>
     </row>
     <row r="16">
@@ -2131,13 +2131,13 @@
         <v>-1.681326404290318</v>
       </c>
       <c r="AE16" t="n">
-        <v>11.6778996737608</v>
+        <v>11.76908737648015</v>
       </c>
       <c r="AF16" t="n">
         <v>2.030937895387919</v>
       </c>
       <c r="AG16" t="n">
-        <v>7.96563537408256</v>
+        <v>8.056823076801912</v>
       </c>
     </row>
     <row r="17">
@@ -2234,13 +2234,13 @@
         <v>-1.871859727385615</v>
       </c>
       <c r="AE17" t="n">
-        <v>14.28436974279036</v>
+        <v>14.3740775733138</v>
       </c>
       <c r="AF17" t="n">
         <v>1.848962917049874</v>
       </c>
       <c r="AG17" t="n">
-        <v>10.56354709835487</v>
+        <v>10.65325492887831</v>
       </c>
     </row>
     <row r="18">
@@ -2337,13 +2337,13 @@
         <v>-2.722493136060427</v>
       </c>
       <c r="AE18" t="n">
-        <v>11.12051933584998</v>
+        <v>11.25392851252065</v>
       </c>
       <c r="AF18" t="n">
         <v>2.480869506725185</v>
       </c>
       <c r="AG18" t="n">
-        <v>5.917156693064372</v>
+        <v>6.050565869735037</v>
       </c>
     </row>
     <row r="19">
@@ -2440,13 +2440,13 @@
         <v>-1.496541490112216</v>
       </c>
       <c r="AE19" t="n">
-        <v>9.731040538300393</v>
+        <v>9.881465367855055</v>
       </c>
       <c r="AF19" t="n">
         <v>3.297158965890005</v>
       </c>
       <c r="AG19" t="n">
-        <v>4.937340082298172</v>
+        <v>5.087764911852834</v>
       </c>
     </row>
     <row r="20">
@@ -2543,13 +2543,13 @@
         <v>-1.698814710905883</v>
       </c>
       <c r="AE20" t="n">
-        <v>11.74798473668342</v>
+        <v>11.99716097123871</v>
       </c>
       <c r="AF20" t="n">
         <v>3.119152271531618</v>
       </c>
       <c r="AG20" t="n">
-        <v>6.930017754245922</v>
+        <v>7.179193988801213</v>
       </c>
     </row>
     <row r="21">
@@ -2646,13 +2646,13 @@
         <v>-4.347034464661159</v>
       </c>
       <c r="AE21" t="n">
-        <v>10.4388273621725</v>
+        <v>10.64084482047585</v>
       </c>
       <c r="AF21" t="n">
         <v>3.253217425700312</v>
       </c>
       <c r="AG21" t="n">
-        <v>2.838575471811025</v>
+        <v>3.040592930114375</v>
       </c>
     </row>
     <row r="22">
@@ -2749,13 +2749,13 @@
         <v>-2.496441871422757</v>
       </c>
       <c r="AE22" t="n">
-        <v>12.25934018559241</v>
+        <v>12.4497784749184</v>
       </c>
       <c r="AF22" t="n">
         <v>2.326473128727222</v>
       </c>
       <c r="AG22" t="n">
-        <v>7.436425185442428</v>
+        <v>7.626863474768419</v>
       </c>
     </row>
     <row r="23">
@@ -2852,13 +2852,13 @@
         <v>-2.241233552365195</v>
       </c>
       <c r="AE23" t="n">
-        <v>12.95521555342142</v>
+        <v>13.03096986013981</v>
       </c>
       <c r="AF23" t="n">
         <v>2.496649824908592</v>
       </c>
       <c r="AG23" t="n">
-        <v>8.217332176147634</v>
+        <v>8.293086482866025</v>
       </c>
     </row>
     <row r="24">
@@ -2955,13 +2955,13 @@
         <v>-3.333678464299149</v>
       </c>
       <c r="AE24" t="n">
-        <v>13.16772149329283</v>
+        <v>13.35229821660199</v>
       </c>
       <c r="AF24" t="n">
         <v>2.367888785783177</v>
       </c>
       <c r="AG24" t="n">
-        <v>7.466154243210508</v>
+        <v>7.650730966519666</v>
       </c>
     </row>
     <row r="25">
@@ -3058,13 +3058,13 @@
         <v>-1.71937003243905</v>
       </c>
       <c r="AE25" t="n">
-        <v>13.92973582471227</v>
+        <v>14.09205416163184</v>
       </c>
       <c r="AF25" t="n">
         <v>2.756894535999121</v>
       </c>
       <c r="AG25" t="n">
-        <v>9.453471256274101</v>
+        <v>9.615789593193673</v>
       </c>
     </row>
     <row r="26">
@@ -3161,13 +3161,13 @@
         <v>-1.192840131257181</v>
       </c>
       <c r="AE26" t="n">
-        <v>13.0209263040827</v>
+        <v>13.1559824118403</v>
       </c>
       <c r="AF26" t="n">
         <v>2.468263610591526</v>
       </c>
       <c r="AG26" t="n">
-        <v>9.359822562233992</v>
+        <v>9.494878669991595</v>
       </c>
     </row>
     <row r="27">
@@ -3264,13 +3264,13 @@
         <v>-1.552836601735071</v>
       </c>
       <c r="AE27" t="n">
-        <v>11.29752950381966</v>
+        <v>11.40694298563118</v>
       </c>
       <c r="AF27" t="n">
         <v>2.176770978233852</v>
       </c>
       <c r="AG27" t="n">
-        <v>7.56792192385074</v>
+        <v>7.677335405662255</v>
       </c>
     </row>
     <row r="28">
@@ -3367,13 +3367,13 @@
         <v>-2.660812271222367</v>
       </c>
       <c r="AE28" t="n">
-        <v>14.73131341729743</v>
+        <v>14.90906696606726</v>
       </c>
       <c r="AF28" t="n">
         <v>2.79206825249104</v>
       </c>
       <c r="AG28" t="n">
-        <v>9.278432893584023</v>
+        <v>9.456186442353856</v>
       </c>
     </row>
     <row r="29">
@@ -3470,13 +3470,13 @@
         <v>-0.445375982062657</v>
       </c>
       <c r="AE29" t="n">
-        <v>10.48715867512957</v>
+        <v>10.6625181294375</v>
       </c>
       <c r="AF29" t="n">
         <v>2.96434199520753</v>
       </c>
       <c r="AG29" t="n">
-        <v>7.077440697859382</v>
+        <v>7.252800152167314</v>
       </c>
     </row>
     <row r="30">
@@ -3573,13 +3573,13 @@
         <v>-3.020347065099521</v>
       </c>
       <c r="AE30" t="n">
-        <v>12.22955459708531</v>
+        <v>12.26650352013645</v>
       </c>
       <c r="AF30" t="n">
         <v>3.157693416302038</v>
       </c>
       <c r="AG30" t="n">
-        <v>6.051514115683755</v>
+        <v>6.088463038734886</v>
       </c>
     </row>
     <row r="31">
@@ -3676,13 +3676,13 @@
         <v>-4.018983435710643</v>
       </c>
       <c r="AE31" t="n">
-        <v>12.39481825753288</v>
+        <v>12.54315067882748</v>
       </c>
       <c r="AF31" t="n">
         <v>2.816984400016397</v>
       </c>
       <c r="AG31" t="n">
-        <v>5.558850421805841</v>
+        <v>5.707182843100437</v>
       </c>
     </row>
     <row r="32">
@@ -3779,13 +3779,13 @@
         <v>-1.554972880726069</v>
       </c>
       <c r="AE32" t="n">
-        <v>14.0058736937249</v>
+        <v>14.04173456276912</v>
       </c>
       <c r="AF32" t="n">
         <v>1.700090545577031</v>
       </c>
       <c r="AG32" t="n">
-        <v>10.75081026742179</v>
+        <v>10.78667113646602</v>
       </c>
     </row>
     <row r="33">
@@ -3882,13 +3882,13 @@
         <v>-2.938616151824918</v>
       </c>
       <c r="AE33" t="n">
-        <v>10.29313570729648</v>
+        <v>10.61390266985545</v>
       </c>
       <c r="AF33" t="n">
         <v>3.031725283185861</v>
       </c>
       <c r="AG33" t="n">
-        <v>4.322794272285702</v>
+        <v>4.643561234844674</v>
       </c>
     </row>
     <row r="34">
@@ -3985,13 +3985,13 @@
         <v>-1.425207382882489</v>
       </c>
       <c r="AE34" t="n">
-        <v>13.29343870241226</v>
+        <v>13.34067530921292</v>
       </c>
       <c r="AF34" t="n">
         <v>2.57710761741724</v>
       </c>
       <c r="AG34" t="n">
-        <v>9.291123702112536</v>
+        <v>9.338360308913188</v>
       </c>
     </row>
     <row r="35">
@@ -4088,13 +4088,13 @@
         <v>-3.126821346811668</v>
       </c>
       <c r="AE35" t="n">
-        <v>9.40623219898362</v>
+        <v>10.68295423017317</v>
       </c>
       <c r="AF35" t="n">
         <v>2.725849737383146</v>
       </c>
       <c r="AG35" t="n">
-        <v>3.553561114788806</v>
+        <v>4.83028314597836</v>
       </c>
     </row>
     <row r="36">
@@ -4191,13 +4191,13 @@
         <v>-2.66692559497466</v>
       </c>
       <c r="AE36" t="n">
-        <v>10.83359646338153</v>
+        <v>11.11820274898126</v>
       </c>
       <c r="AF36" t="n">
         <v>2.584924633664547</v>
       </c>
       <c r="AG36" t="n">
-        <v>5.581746234742317</v>
+        <v>5.866352520342057</v>
       </c>
     </row>
     <row r="37">
@@ -4294,13 +4294,13 @@
         <v>-2.210547051267355</v>
       </c>
       <c r="AE37" t="n">
-        <v>12.07124095739535</v>
+        <v>12.19860116682559</v>
       </c>
       <c r="AF37" t="n">
         <v>2.105639746971739</v>
       </c>
       <c r="AG37" t="n">
-        <v>7.755054159156256</v>
+        <v>7.882414368586492</v>
       </c>
     </row>
     <row r="38">
@@ -4397,13 +4397,13 @@
         <v>-1.173515200567452</v>
       </c>
       <c r="AE38" t="n">
-        <v>13.05735859131712</v>
+        <v>13.2024270099755</v>
       </c>
       <c r="AF38" t="n">
         <v>2.375564778330544</v>
       </c>
       <c r="AG38" t="n">
-        <v>9.508278612419128</v>
+        <v>9.653347031077505</v>
       </c>
     </row>
     <row r="39">
@@ -4500,13 +4500,13 @@
         <v>0.09253389402968186</v>
       </c>
       <c r="AE39" t="n">
-        <v>12.84525758701781</v>
+        <v>12.9997840726113</v>
       </c>
       <c r="AF39" t="n">
         <v>3.432658560789324</v>
       </c>
       <c r="AG39" t="n">
-        <v>9.505132920258164</v>
+        <v>9.659659405851659</v>
       </c>
     </row>
     <row r="40">
@@ -4603,13 +4603,13 @@
         <v>-1.355875285012855</v>
       </c>
       <c r="AE40" t="n">
-        <v>14.94512352444527</v>
+        <v>15.06446348441912</v>
       </c>
       <c r="AF40" t="n">
         <v>2.909579690590713</v>
       </c>
       <c r="AG40" t="n">
-        <v>10.67966854884171</v>
+        <v>10.79900850881555</v>
       </c>
     </row>
     <row r="41">
@@ -4706,13 +4706,13 @@
         <v>-2.345699161821965</v>
       </c>
       <c r="AE41" t="n">
-        <v>13.31491556058478</v>
+        <v>13.48522943201806</v>
       </c>
       <c r="AF41" t="n">
         <v>2.407429868159737</v>
       </c>
       <c r="AG41" t="n">
-        <v>8.561786530603078</v>
+        <v>8.732100402036355</v>
       </c>
     </row>
     <row r="42">
@@ -4809,13 +4809,13 @@
         <v>-1.019839633062165</v>
       </c>
       <c r="AE42" t="n">
-        <v>12.4203429810224</v>
+        <v>12.67359967908071</v>
       </c>
       <c r="AF42" t="n">
         <v>3.343456731499479</v>
       </c>
       <c r="AG42" t="n">
-        <v>8.057046616460754</v>
+        <v>8.310303314519064</v>
       </c>
     </row>
     <row r="43">
@@ -4912,13 +4912,13 @@
         <v>-2.720293408378807</v>
       </c>
       <c r="AE43" t="n">
-        <v>11.76360190243341</v>
+        <v>11.90477475879558</v>
       </c>
       <c r="AF43" t="n">
         <v>3.293796111048356</v>
       </c>
       <c r="AG43" t="n">
-        <v>5.749512383006244</v>
+        <v>5.890685239368419</v>
       </c>
     </row>
     <row r="44">
@@ -5015,13 +5015,13 @@
         <v>-3.019131006775191</v>
       </c>
       <c r="AE44" t="n">
-        <v>13.73447771869042</v>
+        <v>13.79892655811657</v>
       </c>
       <c r="AF44" t="n">
         <v>2.395329167291155</v>
       </c>
       <c r="AG44" t="n">
-        <v>8.320017544624079</v>
+        <v>8.384466384050224</v>
       </c>
     </row>
     <row r="45">
@@ -5118,13 +5118,13 @@
         <v>-2.906713763785051</v>
       </c>
       <c r="AE45" t="n">
-        <v>12.75645778198074</v>
+        <v>12.93795781574384</v>
       </c>
       <c r="AF45" t="n">
         <v>2.633644577255411</v>
       </c>
       <c r="AG45" t="n">
-        <v>7.216099440940282</v>
+        <v>7.397599474703376</v>
       </c>
     </row>
     <row r="46">
@@ -5221,13 +5221,13 @@
         <v>-2.385548344717861</v>
       </c>
       <c r="AE46" t="n">
-        <v>14.17710116969799</v>
+        <v>14.14625678105321</v>
       </c>
       <c r="AF46" t="n">
         <v>1.76104150121723</v>
       </c>
       <c r="AG46" t="n">
-        <v>10.03051132376289</v>
+        <v>9.999666935118119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the data - phenotype_microbiome file
</commit_message>
<xml_diff>
--- a/input/comp_mrs_cat.xlsx
+++ b/input/comp_mrs_cat.xlsx
@@ -531,47 +531,47 @@
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Cutaneous T‐cell Lymphoma</t>
+          <t>Osteoarthritis</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Osteoarthritis</t>
+          <t>Atopic Dermatitis</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Atopic Dermatitis</t>
+          <t>Food Allergy</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Food Allergy</t>
+          <t>Glaucoma</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Glaucoma</t>
+          <t>Diarrhea</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>Diarrhea</t>
+          <t>Acute Diarrhea</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>Acute Diarrhea</t>
+          <t>Chronic Enteropathy</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>Chronic Enteropathy</t>
+          <t>Obesity</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>Obesity</t>
+          <t>Constipation</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
@@ -647,46 +647,46 @@
         <v>-0.01617794500210694</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.1944100133419557</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
         <v>-0.01132796641150682</v>
       </c>
       <c r="S2" t="n">
-        <v>-0.05543519192027378</v>
+        <v>-0.05848688641437708</v>
       </c>
       <c r="T2" t="n">
         <v>-0.3672207100426312</v>
       </c>
       <c r="U2" t="n">
-        <v>-0.03464701462091963</v>
+        <v>0.00178183310199658</v>
       </c>
       <c r="V2" t="n">
-        <v>0.00178183310199658</v>
+        <v>-0.09380089734981277</v>
       </c>
       <c r="W2" t="n">
-        <v>-0.09380089734981277</v>
+        <v>-0.0002532522288930111</v>
       </c>
       <c r="X2" t="n">
-        <v>-0.0002532522288930111</v>
+        <v>-0.09697608190740231</v>
       </c>
       <c r="Y2" t="n">
-        <v>-0.09697608190740231</v>
+        <v>-0.06464400721828273</v>
       </c>
       <c r="Z2" t="n">
-        <v>-0.06464400721828273</v>
+        <v>1.89121022699381</v>
       </c>
       <c r="AA2" t="n">
-        <v>1.89121022699381</v>
+        <v>-0.02746085482650446</v>
       </c>
       <c r="AB2" t="n">
-        <v>-0.02746085482650446</v>
+        <v>0.05422453157262382</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.05422453157262382</v>
+        <v>-0.005123542545699736</v>
       </c>
       <c r="AD2" t="n">
-        <v>-1.16216567582168</v>
+        <v>-1.066398706047424</v>
       </c>
       <c r="AE2" t="n">
         <v>11.77990626116324</v>
@@ -695,7 +695,7 @@
         <v>1.21525785660293</v>
       </c>
       <c r="AG2" t="n">
-        <v>9.402482728738628</v>
+        <v>9.498249698512884</v>
       </c>
     </row>
     <row r="3">
@@ -750,46 +750,46 @@
         <v>-0.05429379170355585</v>
       </c>
       <c r="Q3" t="n">
-        <v>-0.2063472174771852</v>
+        <v>-0.1082004288786222</v>
       </c>
       <c r="R3" t="n">
         <v>-0.005648889304671684</v>
       </c>
       <c r="S3" t="n">
-        <v>-0.1049062631792872</v>
+        <v>-0.08805076812481212</v>
       </c>
       <c r="T3" t="n">
         <v>-0.300119973230965</v>
       </c>
       <c r="U3" t="n">
-        <v>-0.00396421248671902</v>
+        <v>0.001197096824273261</v>
       </c>
       <c r="V3" t="n">
-        <v>0.001197096824273261</v>
+        <v>-0.09848168655829577</v>
       </c>
       <c r="W3" t="n">
-        <v>-0.09848168655829577</v>
+        <v>0.001090659531956615</v>
       </c>
       <c r="X3" t="n">
-        <v>0.001090659531956615</v>
+        <v>-0.2190722673694516</v>
       </c>
       <c r="Y3" t="n">
-        <v>-0.2190722673694516</v>
+        <v>-0.108034256276491</v>
       </c>
       <c r="Z3" t="n">
-        <v>-0.108034256276491</v>
+        <v>1.808537904884726</v>
       </c>
       <c r="AA3" t="n">
-        <v>1.808537904884726</v>
+        <v>-0.1428386930053857</v>
       </c>
       <c r="AB3" t="n">
-        <v>-0.1428386930053857</v>
+        <v>0.1004406976427049</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.1004406976427049</v>
+        <v>0.007416023467377744</v>
       </c>
       <c r="AD3" t="n">
-        <v>-2.479977037671318</v>
+        <v>-2.430105050124304</v>
       </c>
       <c r="AE3" t="n">
         <v>14.09549045834902</v>
@@ -798,7 +798,7 @@
         <v>1.907476798064713</v>
       </c>
       <c r="AG3" t="n">
-        <v>9.708036622612987</v>
+        <v>9.757908610160005</v>
       </c>
     </row>
     <row r="4">
@@ -811,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.07669944457269055</v>
+        <v>0.07638797993178624</v>
       </c>
       <c r="D4" t="n">
         <v>-0.01170403240353044</v>
@@ -832,7 +832,7 @@
         <v>0.0002770022172285946</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.102660741290673</v>
+        <v>-0.1029332728514643</v>
       </c>
       <c r="K4" t="n">
         <v>-0.1983235493385482</v>
@@ -853,46 +853,46 @@
         <v>0.0772117530087509</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.1627783421399945</v>
+        <v>-0.05319557614683399</v>
       </c>
       <c r="R4" t="n">
         <v>-0.00330360449192901</v>
       </c>
       <c r="S4" t="n">
-        <v>-0.07215359292822139</v>
+        <v>-0.07600926257200749</v>
       </c>
       <c r="T4" t="n">
         <v>-0.362563598888024</v>
       </c>
       <c r="U4" t="n">
-        <v>-0.005142669546960935</v>
+        <v>0.004415955908644617</v>
       </c>
       <c r="V4" t="n">
-        <v>0.004415955908644617</v>
+        <v>-0.1723359622863692</v>
       </c>
       <c r="W4" t="n">
-        <v>-0.1721377575148846</v>
+        <v>0.00139791135651783</v>
       </c>
       <c r="X4" t="n">
-        <v>0.00139791135651783</v>
+        <v>-0.1983201587105889</v>
       </c>
       <c r="Y4" t="n">
-        <v>-0.1983201587105889</v>
+        <v>-0.01785303827539394</v>
       </c>
       <c r="Z4" t="n">
-        <v>-0.01785303827539394</v>
+        <v>1.779849160605177</v>
       </c>
       <c r="AA4" t="n">
-        <v>1.779849160605177</v>
+        <v>-0.1063990140144021</v>
       </c>
       <c r="AB4" t="n">
-        <v>-0.1063990140144021</v>
+        <v>0.138315192858073</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.138315192858073</v>
+        <v>0.03437362076989906</v>
       </c>
       <c r="AD4" t="n">
-        <v>-1.234927003671412</v>
+        <v>-0.7162638989153116</v>
       </c>
       <c r="AE4" t="n">
         <v>12.05507120829597</v>
@@ -901,7 +901,7 @@
         <v>3.004803121989122</v>
       </c>
       <c r="AG4" t="n">
-        <v>7.81534108263544</v>
+        <v>8.334004187391541</v>
       </c>
     </row>
     <row r="5">
@@ -914,7 +914,7 @@
         <v>-0.0002086536761009553</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02503754184678446</v>
+        <v>0.02473301039138521</v>
       </c>
       <c r="D5" t="n">
         <v>-0.01395092525180149</v>
@@ -935,7 +935,7 @@
         <v>-0.0272316492603727</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.07196616619731964</v>
+        <v>-0.07223263122079399</v>
       </c>
       <c r="K5" t="n">
         <v>-0.2019067391014378</v>
@@ -956,55 +956,55 @@
         <v>0.1523808318742656</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.1237478820109895</v>
+        <v>-0.005813059825648474</v>
       </c>
       <c r="R5" t="n">
         <v>-0.003278049398107327</v>
       </c>
       <c r="S5" t="n">
-        <v>-0.08402214405291504</v>
+        <v>-0.08828525028758026</v>
       </c>
       <c r="T5" t="n">
         <v>-0.3749471067347218</v>
       </c>
       <c r="U5" t="n">
-        <v>-0.04169485254456643</v>
+        <v>0.02487681866274705</v>
       </c>
       <c r="V5" t="n">
-        <v>0.02487681866274705</v>
+        <v>-0.1630451139817905</v>
       </c>
       <c r="W5" t="n">
-        <v>-0.1628513212374456</v>
+        <v>0.004642844498893362</v>
       </c>
       <c r="X5" t="n">
-        <v>0.004642844498893362</v>
+        <v>-0.2587036733432321</v>
       </c>
       <c r="Y5" t="n">
-        <v>-0.2587036733432321</v>
+        <v>-0.01896172557542928</v>
       </c>
       <c r="Z5" t="n">
-        <v>-0.01896172557542928</v>
+        <v>1.706039903079128</v>
       </c>
       <c r="AA5" t="n">
-        <v>1.706039903079128</v>
+        <v>-0.1028599066275024</v>
       </c>
       <c r="AB5" t="n">
-        <v>-0.1028599066275024</v>
+        <v>0.05404592228070815</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.05404592228070815</v>
+        <v>-0.01519820461218374</v>
       </c>
       <c r="AD5" t="n">
-        <v>-1.468658039209249</v>
+        <v>-0.9574454854465974</v>
       </c>
       <c r="AE5" t="n">
-        <v>15.14395095318842</v>
+        <v>15.14418650838776</v>
       </c>
       <c r="AF5" t="n">
         <v>2.79833508502352</v>
       </c>
       <c r="AG5" t="n">
-        <v>10.87695782895565</v>
+        <v>11.38840593791764</v>
       </c>
     </row>
     <row r="6">
@@ -1059,46 +1059,46 @@
         <v>0.04364258649251861</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.1941143736607782</v>
+        <v>-0.001052835623266473</v>
       </c>
       <c r="R6" t="n">
         <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.03353282679389131</v>
+        <v>-0.03538163277660466</v>
       </c>
       <c r="T6" t="n">
         <v>-0.4130252976466455</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.00312829326751056</v>
+        <v>0.00315088067895816</v>
       </c>
       <c r="V6" t="n">
-        <v>0.00315088067895816</v>
+        <v>-0.002673305334841715</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.002673305334841715</v>
+        <v>0</v>
       </c>
       <c r="X6" t="n">
-        <v>0</v>
+        <v>-0.1148422719248623</v>
       </c>
       <c r="Y6" t="n">
-        <v>-0.1148422719248623</v>
+        <v>-0.07183145793693584</v>
       </c>
       <c r="Z6" t="n">
-        <v>-0.07183145793693584</v>
+        <v>1.908498032422194</v>
       </c>
       <c r="AA6" t="n">
-        <v>1.908498032422194</v>
+        <v>-0.01875854222731535</v>
       </c>
       <c r="AB6" t="n">
-        <v>-0.01875854222731535</v>
+        <v>0.06051661563918916</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.06051661563918916</v>
+        <v>-0.1147592896947943</v>
       </c>
       <c r="AD6" t="n">
-        <v>-0.9005002960522448</v>
+        <v>-0.9096866557961611</v>
       </c>
       <c r="AE6" t="n">
         <v>11.41663563776412</v>
@@ -1107,7 +1107,7 @@
         <v>1.398649254021426</v>
       </c>
       <c r="AG6" t="n">
-        <v>9.117486087690445</v>
+        <v>9.10829972794653</v>
       </c>
     </row>
     <row r="7">
@@ -1120,7 +1120,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.05111316883441714</v>
+        <v>0.05065161285327728</v>
       </c>
       <c r="D7" t="n">
         <v>-0.04231232821757515</v>
@@ -1141,7 +1141,7 @@
         <v>-0.08367968631077287</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.1162985390859103</v>
+        <v>-0.1167024005694077</v>
       </c>
       <c r="K7" t="n">
         <v>-0.2431717279214084</v>
@@ -1162,55 +1162,55 @@
         <v>0.09124046027285174</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.16767641714478</v>
+        <v>0</v>
       </c>
       <c r="R7" t="n">
         <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>-0.05556733474085974</v>
+        <v>-0.0585482451900935</v>
       </c>
       <c r="T7" t="n">
         <v>-0.3405054600143866</v>
       </c>
       <c r="U7" t="n">
-        <v>-0.008002747972187916</v>
+        <v>0.007317276576014255</v>
       </c>
       <c r="V7" t="n">
-        <v>0.007317276576014255</v>
+        <v>-0.2710742405624526</v>
       </c>
       <c r="W7" t="n">
-        <v>-0.270780523119909</v>
+        <v>0</v>
       </c>
       <c r="X7" t="n">
-        <v>0</v>
+        <v>-0.2012413867633076</v>
       </c>
       <c r="Y7" t="n">
-        <v>-0.2012413867633076</v>
+        <v>-0.003648950867323071</v>
       </c>
       <c r="Z7" t="n">
-        <v>-0.003648950867323071</v>
+        <v>1.723139493075088</v>
       </c>
       <c r="AA7" t="n">
-        <v>1.723139493075088</v>
+        <v>-0.2522495684019206</v>
       </c>
       <c r="AB7" t="n">
-        <v>-0.2522495684019206</v>
+        <v>0.1080074877997258</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.1080074877997258</v>
+        <v>0.1173506255765141</v>
       </c>
       <c r="AD7" t="n">
-        <v>-2.116910323168911</v>
+        <v>-1.325279253088115</v>
       </c>
       <c r="AE7" t="n">
-        <v>11.5961704773125</v>
+        <v>11.59625371340653</v>
       </c>
       <c r="AF7" t="n">
         <v>2.713662913782229</v>
       </c>
       <c r="AG7" t="n">
-        <v>6.765597240361365</v>
+        <v>7.557311546536181</v>
       </c>
     </row>
     <row r="8">
@@ -1223,7 +1223,7 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.03296239770773735</v>
+        <v>-0.03306993230237358</v>
       </c>
       <c r="D8" t="n">
         <v>-0.01031326905790914</v>
@@ -1244,7 +1244,7 @@
         <v>0.004053915783882515</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.03919575741960697</v>
+        <v>-0.03928985018991367</v>
       </c>
       <c r="K8" t="n">
         <v>-0.2029671771144906</v>
@@ -1265,55 +1265,55 @@
         <v>-0.1015816935502055</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.1417678591587906</v>
+        <v>-0.003024083813591936</v>
       </c>
       <c r="R8" t="n">
         <v>-0.002264132851548667</v>
       </c>
       <c r="S8" t="n">
-        <v>-0.07837845689444789</v>
+        <v>-0.0828110670756747</v>
       </c>
       <c r="T8" t="n">
         <v>-0.449461213218675</v>
       </c>
       <c r="U8" t="n">
-        <v>-0.009383695971463806</v>
+        <v>0.004528265703097334</v>
       </c>
       <c r="V8" t="n">
-        <v>0.004528265703097334</v>
+        <v>-0.0570252734281524</v>
       </c>
       <c r="W8" t="n">
-        <v>-0.0569568423224748</v>
+        <v>-0.0002697732840032522</v>
       </c>
       <c r="X8" t="n">
-        <v>-0.0002697732840032522</v>
+        <v>-0.2009072169070735</v>
       </c>
       <c r="Y8" t="n">
-        <v>-0.2009072169070735</v>
+        <v>-0.1179805042303452</v>
       </c>
       <c r="Z8" t="n">
-        <v>-0.1179805042303452</v>
+        <v>1.680273660067903</v>
       </c>
       <c r="AA8" t="n">
-        <v>1.680273660067903</v>
+        <v>-0.07278670528648094</v>
       </c>
       <c r="AB8" t="n">
-        <v>-0.07278670528648094</v>
+        <v>0.1773995312111843</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.1773995312111843</v>
+        <v>0.02297643311931965</v>
       </c>
       <c r="AD8" t="n">
-        <v>-2.960680884375331</v>
+        <v>-1.885550327985199</v>
       </c>
       <c r="AE8" t="n">
-        <v>11.52701059773078</v>
+        <v>11.52707889346317</v>
       </c>
       <c r="AF8" t="n">
         <v>3.149142237757889</v>
       </c>
       <c r="AG8" t="n">
-        <v>5.417187475597562</v>
+        <v>6.492386327720084</v>
       </c>
     </row>
     <row r="9">
@@ -1326,7 +1326,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.07997246681846366</v>
+        <v>-0.08903099733509404</v>
       </c>
       <c r="D9" t="n">
         <v>-0.04881534472571435</v>
@@ -1347,7 +1347,7 @@
         <v>-0.06298381549329174</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.05872860048399509</v>
+        <v>-0.06665481468604668</v>
       </c>
       <c r="K9" t="n">
         <v>-0.2042396510648194</v>
@@ -1368,46 +1368,46 @@
         <v>-0.04068911600148702</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.007997745948629958</v>
+        <v>0</v>
       </c>
       <c r="R9" t="n">
         <v>-0.0004700667296227052</v>
       </c>
       <c r="S9" t="n">
-        <v>-0.1346105990529776</v>
+        <v>-0.1413390511005015</v>
       </c>
       <c r="T9" t="n">
         <v>-0.3539921674347238</v>
       </c>
       <c r="U9" t="n">
-        <v>-0.006142180239621491</v>
+        <v>0.004680447088870762</v>
       </c>
       <c r="V9" t="n">
-        <v>0.004680447088870762</v>
+        <v>-0.01122864015349732</v>
       </c>
       <c r="W9" t="n">
-        <v>-0.005464120733823438</v>
+        <v>6.715238994610074e-05</v>
       </c>
       <c r="X9" t="n">
-        <v>6.715238994610074e-05</v>
+        <v>-0.3614220732463613</v>
       </c>
       <c r="Y9" t="n">
-        <v>-0.3614220732463613</v>
+        <v>-0.0245160724833677</v>
       </c>
       <c r="Z9" t="n">
-        <v>-0.0245160724833677</v>
+        <v>1.412204431314538</v>
       </c>
       <c r="AA9" t="n">
-        <v>1.412204431314538</v>
+        <v>-0.001560149029623587</v>
       </c>
       <c r="AB9" t="n">
-        <v>-0.001560149029623587</v>
+        <v>0.2002605397648755</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.2002605397648755</v>
+        <v>0.02388775041531606</v>
       </c>
       <c r="AD9" t="n">
-        <v>-3.614753164174113</v>
+        <v>-3.182515033969153</v>
       </c>
       <c r="AE9" t="n">
         <v>11.96681525992708</v>
@@ -1416,7 +1416,7 @@
         <v>3.276139743624471</v>
       </c>
       <c r="AG9" t="n">
-        <v>5.075922352128496</v>
+        <v>5.508160482333455</v>
       </c>
     </row>
     <row r="10">
@@ -1429,7 +1429,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.09388023770082492</v>
+        <v>0.09311136547414241</v>
       </c>
       <c r="D10" t="n">
         <v>-0.07004488916426878</v>
@@ -1450,7 +1450,7 @@
         <v>0.01998096443830198</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.1113947925747019</v>
+        <v>-0.1120675557730491</v>
       </c>
       <c r="K10" t="n">
         <v>-0.1553495541835453</v>
@@ -1471,55 +1471,55 @@
         <v>-0.0273341985998691</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.02719744978214569</v>
+        <v>-0.4841886663797277</v>
       </c>
       <c r="R10" t="n">
         <v>-0.03741253581668721</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.1469531828872614</v>
+        <v>-0.1521342635392507</v>
       </c>
       <c r="T10" t="n">
         <v>-0.04399658812410889</v>
       </c>
       <c r="U10" t="n">
-        <v>-0.03167364675653141</v>
+        <v>0.005137693971413827</v>
       </c>
       <c r="V10" t="n">
-        <v>0.005137693971413827</v>
+        <v>-0.02919656940027784</v>
       </c>
       <c r="W10" t="n">
-        <v>-0.02870728707420715</v>
+        <v>0.03574151486956014</v>
       </c>
       <c r="X10" t="n">
-        <v>0.03574151486956014</v>
+        <v>-0.3747007667098363</v>
       </c>
       <c r="Y10" t="n">
-        <v>-0.3747007667098363</v>
+        <v>0.01756870559646433</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.01756870559646433</v>
+        <v>1.232598430047946</v>
       </c>
       <c r="AA10" t="n">
-        <v>1.232598430047946</v>
+        <v>-0.223989214557176</v>
       </c>
       <c r="AB10" t="n">
-        <v>-0.223989214557176</v>
+        <v>0.1733208992790237</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.1733208992790237</v>
+        <v>0.1670352651202235</v>
       </c>
       <c r="AD10" t="n">
-        <v>-0.6538190124457182</v>
+        <v>0.3724108735347949</v>
       </c>
       <c r="AE10" t="n">
-        <v>9.860478640744111</v>
+        <v>9.860527833189106</v>
       </c>
       <c r="AF10" t="n">
         <v>3.828349514488567</v>
       </c>
       <c r="AG10" t="n">
-        <v>5.378310113809826</v>
+        <v>6.404589192235335</v>
       </c>
     </row>
     <row r="11">
@@ -1532,7 +1532,7 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0.06360007781336491</v>
+        <v>0.06217642933002947</v>
       </c>
       <c r="D11" t="n">
         <v>-0.01278288753772612</v>
@@ -1553,7 +1553,7 @@
         <v>-0.04310648961960067</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.1021931998128335</v>
+        <v>-0.103438892235752</v>
       </c>
       <c r="K11" t="n">
         <v>-0.2830156461365023</v>
@@ -1574,55 +1574,55 @@
         <v>-0.06679420680688045</v>
       </c>
       <c r="Q11" t="n">
-        <v>-0.0939803841873408</v>
+        <v>0</v>
       </c>
       <c r="R11" t="n">
         <v>-0.002907875989194988</v>
       </c>
       <c r="S11" t="n">
-        <v>-0.1772516224792788</v>
+        <v>-0.1818066595385164</v>
       </c>
       <c r="T11" t="n">
         <v>-0.2186435295673452</v>
       </c>
       <c r="U11" t="n">
-        <v>-0.007096688698567215</v>
+        <v>0.04886310065124592</v>
       </c>
       <c r="V11" t="n">
-        <v>0.04886310065124592</v>
+        <v>-0.2062633219408698</v>
       </c>
       <c r="W11" t="n">
-        <v>-0.2053573638151109</v>
+        <v>-0.002924541423441811</v>
       </c>
       <c r="X11" t="n">
-        <v>-0.002924541423441811</v>
+        <v>-0.4172677145939124</v>
       </c>
       <c r="Y11" t="n">
-        <v>-0.4172677145939124</v>
+        <v>-0.02438047727485258</v>
       </c>
       <c r="Z11" t="n">
-        <v>-0.02438047727485258</v>
+        <v>1.464087906257625</v>
       </c>
       <c r="AA11" t="n">
-        <v>1.464087906257625</v>
+        <v>-0.1581203146599285</v>
       </c>
       <c r="AB11" t="n">
-        <v>-0.1581203146599285</v>
+        <v>0.1612421228519281</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.1612421228519281</v>
+        <v>0.03082091273051432</v>
       </c>
       <c r="AD11" t="n">
-        <v>-2.101063399074429</v>
+        <v>-1.719531955728035</v>
       </c>
       <c r="AE11" t="n">
-        <v>10.60976684966777</v>
+        <v>10.60978211399623</v>
       </c>
       <c r="AF11" t="n">
         <v>3.84770481406579</v>
       </c>
       <c r="AG11" t="n">
-        <v>4.660998636527554</v>
+        <v>5.042545344202404</v>
       </c>
     </row>
     <row r="12">
@@ -1635,7 +1635,7 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0.02046576150193214</v>
+        <v>0.02027375494607455</v>
       </c>
       <c r="D12" t="n">
         <v>-0.001865240657484578</v>
@@ -1656,7 +1656,7 @@
         <v>0.02229708415869791</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.01724642410109753</v>
+        <v>-0.01741442983747292</v>
       </c>
       <c r="K12" t="n">
         <v>-0.1713317179851058</v>
@@ -1677,55 +1677,55 @@
         <v>0.07182812444673717</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.1853789304575047</v>
+        <v>-0.006720358187707631</v>
       </c>
       <c r="R12" t="n">
         <v>-0.001014575790511269</v>
       </c>
       <c r="S12" t="n">
-        <v>-0.04944789763113653</v>
+        <v>-0.05219773660378963</v>
       </c>
       <c r="T12" t="n">
         <v>-0.4374428520269442</v>
       </c>
       <c r="U12" t="n">
-        <v>-0.002468817461685432</v>
+        <v>0.004715147321515603</v>
       </c>
       <c r="V12" t="n">
-        <v>0.004715147321515603</v>
+        <v>-0.1745376227030314</v>
       </c>
       <c r="W12" t="n">
-        <v>-0.1744154367129402</v>
+        <v>9.660119732224762e-05</v>
       </c>
       <c r="X12" t="n">
-        <v>9.660119732224762e-05</v>
+        <v>-0.1525601048949838</v>
       </c>
       <c r="Y12" t="n">
-        <v>-0.1525601048949838</v>
+        <v>-0.0279917735258155</v>
       </c>
       <c r="Z12" t="n">
-        <v>-0.0279917735258155</v>
+        <v>1.816792840889407</v>
       </c>
       <c r="AA12" t="n">
-        <v>1.816792840889407</v>
+        <v>-0.004657715238659752</v>
       </c>
       <c r="AB12" t="n">
-        <v>-0.004657715238659752</v>
+        <v>0.1321892540934846</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.1321892540934846</v>
+        <v>0.1397611512177132</v>
       </c>
       <c r="AD12" t="n">
-        <v>-1.51729773178816</v>
+        <v>-0.587582500574083</v>
       </c>
       <c r="AE12" t="n">
-        <v>13.2386734764729</v>
+        <v>13.23877518635641</v>
       </c>
       <c r="AF12" t="n">
         <v>2.289331898834243</v>
       </c>
       <c r="AG12" t="n">
-        <v>9.432043845850497</v>
+        <v>10.36186078694808</v>
       </c>
     </row>
     <row r="13">
@@ -1738,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.003191395267973607</v>
+        <v>-0.003309371798086172</v>
       </c>
       <c r="D13" t="n">
         <v>-0.01424409562357496</v>
@@ -1759,7 +1759,7 @@
         <v>-0.09421870624869831</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.03232940302289108</v>
+        <v>-0.03243263248673957</v>
       </c>
       <c r="K13" t="n">
         <v>-0.08506592374183965</v>
@@ -1780,46 +1780,46 @@
         <v>0.08921884575933638</v>
       </c>
       <c r="Q13" t="n">
-        <v>-0.2076426279374849</v>
+        <v>0</v>
       </c>
       <c r="R13" t="n">
         <v>-0.000206950791872157</v>
       </c>
       <c r="S13" t="n">
-        <v>-0.02529995560244494</v>
+        <v>-0.02673951716277804</v>
       </c>
       <c r="T13" t="n">
         <v>-0.324628415325401</v>
       </c>
       <c r="U13" t="n">
-        <v>-0.000275934389162876</v>
+        <v>0.003300219966570374</v>
       </c>
       <c r="V13" t="n">
-        <v>0.003300219966570374</v>
+        <v>-0.08740891399853484</v>
       </c>
       <c r="W13" t="n">
-        <v>-0.08733383802482685</v>
+        <v>-2.956439883887957e-05</v>
       </c>
       <c r="X13" t="n">
-        <v>-2.956439883887957e-05</v>
+        <v>-0.07187468220206643</v>
       </c>
       <c r="Y13" t="n">
-        <v>-0.07187468220206643</v>
+        <v>-0.02037043499578953</v>
       </c>
       <c r="Z13" t="n">
-        <v>-0.02037043499578953</v>
+        <v>1.916189070380353</v>
       </c>
       <c r="AA13" t="n">
-        <v>1.916189070380353</v>
+        <v>-0.07890103011922783</v>
       </c>
       <c r="AB13" t="n">
-        <v>-0.07890103011922783</v>
+        <v>0.03446330418885177</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.03446330418885177</v>
+        <v>-0.01959671602417035</v>
       </c>
       <c r="AD13" t="n">
-        <v>-0.8013112033540528</v>
+        <v>-0.7032524999018033</v>
       </c>
       <c r="AE13" t="n">
         <v>11.88895917226999</v>
@@ -1828,7 +1828,7 @@
         <v>1.034388269386078</v>
       </c>
       <c r="AG13" t="n">
-        <v>10.05325969952986</v>
+        <v>10.15131840298211</v>
       </c>
     </row>
     <row r="14">
@@ -1841,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.05462553669484729</v>
+        <v>-0.0575689117662238</v>
       </c>
       <c r="D14" t="n">
         <v>-0.09627607272011163</v>
@@ -1862,7 +1862,7 @@
         <v>-0.05344209554187902</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.1761058730386431</v>
+        <v>-0.1786813262260975</v>
       </c>
       <c r="K14" t="n">
         <v>-0.2555009038446274</v>
@@ -1883,55 +1883,55 @@
         <v>0.05811198836759764</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.03428808157900386</v>
+        <v>-0.01672537527065896</v>
       </c>
       <c r="R14" t="n">
         <v>-0.002493221577150223</v>
       </c>
       <c r="S14" t="n">
-        <v>-0.1372720893490379</v>
+        <v>-0.1419797693286048</v>
       </c>
       <c r="T14" t="n">
         <v>-0.2848874509950664</v>
       </c>
       <c r="U14" t="n">
-        <v>-0.01688187502377081</v>
+        <v>0.01284754708782828</v>
       </c>
       <c r="V14" t="n">
-        <v>0.01284754708782828</v>
+        <v>-0.1572107570601716</v>
       </c>
       <c r="W14" t="n">
-        <v>-0.1553377001965684</v>
+        <v>0</v>
       </c>
       <c r="X14" t="n">
-        <v>0</v>
+        <v>-0.3982292566945077</v>
       </c>
       <c r="Y14" t="n">
-        <v>-0.3982292566945077</v>
+        <v>0.02536771841533217</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.02536771841533217</v>
+        <v>1.515483340451495</v>
       </c>
       <c r="AA14" t="n">
-        <v>1.515483340451495</v>
+        <v>-0.2289954687923547</v>
       </c>
       <c r="AB14" t="n">
-        <v>-0.2289954687923547</v>
+        <v>0.2013273141344778</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.2013273141344778</v>
+        <v>0.04521343668164262</v>
       </c>
       <c r="AD14" t="n">
-        <v>-2.089801509041681</v>
+        <v>-1.695149335452476</v>
       </c>
       <c r="AE14" t="n">
-        <v>10.16256479919443</v>
+        <v>10.16261714606267</v>
       </c>
       <c r="AF14" t="n">
         <v>3.641193771392695</v>
       </c>
       <c r="AG14" t="n">
-        <v>4.431569518760055</v>
+        <v>4.826274039217498</v>
       </c>
     </row>
     <row r="15">
@@ -1986,55 +1986,55 @@
         <v>0.0001999662825159529</v>
       </c>
       <c r="Q15" t="n">
-        <v>-0.1864103696918848</v>
+        <v>-0.01002250653838596</v>
       </c>
       <c r="R15" t="n">
         <v>-0.02362463272120596</v>
       </c>
       <c r="S15" t="n">
-        <v>-0.01816579581611789</v>
+        <v>-0.01923437204059541</v>
       </c>
       <c r="T15" t="n">
         <v>-0.4758033213668364</v>
       </c>
       <c r="U15" t="n">
-        <v>-0.002580815891667767</v>
+        <v>0.005425457597809015</v>
       </c>
       <c r="V15" t="n">
-        <v>0.005425457597809015</v>
+        <v>-0.05977596208405951</v>
       </c>
       <c r="W15" t="n">
-        <v>-0.05977596208405951</v>
+        <v>0.0001113181998198481</v>
       </c>
       <c r="X15" t="n">
-        <v>0.0001113181998198481</v>
+        <v>-0.05462414305886012</v>
       </c>
       <c r="Y15" t="n">
-        <v>-0.05462414305886012</v>
+        <v>-0.05542093062651843</v>
       </c>
       <c r="Z15" t="n">
-        <v>-0.05542093062651843</v>
+        <v>1.844496411284426</v>
       </c>
       <c r="AA15" t="n">
-        <v>1.844496411284426</v>
+        <v>-0.002572109935550683</v>
       </c>
       <c r="AB15" t="n">
-        <v>-0.002572109935550683</v>
+        <v>0.09606169688343277</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.09606169688343277</v>
+        <v>-0.04877761063397409</v>
       </c>
       <c r="AD15" t="n">
-        <v>-0.3942163585171082</v>
+        <v>-0.0378648007857209</v>
       </c>
       <c r="AE15" t="n">
-        <v>14.79637055232094</v>
+        <v>14.79667321669343</v>
       </c>
       <c r="AF15" t="n">
         <v>1.785537558360071</v>
       </c>
       <c r="AG15" t="n">
-        <v>12.61661663544376</v>
+        <v>12.97327085754764</v>
       </c>
     </row>
     <row r="16">
@@ -2047,7 +2047,7 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.0007067912335571228</v>
+        <v>-0.0008322885129182032</v>
       </c>
       <c r="D16" t="n">
         <v>-0.03872366813426362</v>
@@ -2068,7 +2068,7 @@
         <v>-0.06995739410365349</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.1021781967553508</v>
+        <v>-0.1022880068747918</v>
       </c>
       <c r="K16" t="n">
         <v>-0.1733360122764915</v>
@@ -2089,46 +2089,46 @@
         <v>-0.01726285904678449</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.1940412182960933</v>
+        <v>-0.002805710914145983</v>
       </c>
       <c r="R16" t="n">
         <v>-0.03045530098480336</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.03639042721287476</v>
+        <v>-0.03687494574885909</v>
       </c>
       <c r="T16" t="n">
         <v>-0.3300637531225312</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.00280103316489918</v>
+        <v>0.01020018127604768</v>
       </c>
       <c r="V16" t="n">
-        <v>0.01020018127604768</v>
+        <v>-0.1856673246321635</v>
       </c>
       <c r="W16" t="n">
-        <v>-0.1855874627271155</v>
+        <v>0.0001334613215337476</v>
       </c>
       <c r="X16" t="n">
-        <v>0.0001334613215337476</v>
+        <v>-0.1452417757505976</v>
       </c>
       <c r="Y16" t="n">
-        <v>-0.1452417757505976</v>
+        <v>-0.02593918737751226</v>
       </c>
       <c r="Z16" t="n">
-        <v>-0.02593918737751226</v>
+        <v>1.825382175595229</v>
       </c>
       <c r="AA16" t="n">
-        <v>1.825382175595229</v>
+        <v>-0.2133597810137022</v>
       </c>
       <c r="AB16" t="n">
-        <v>-0.2133597810137022</v>
+        <v>0.08901275588646708</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.08901275588646708</v>
+        <v>0.006593193458761211</v>
       </c>
       <c r="AD16" t="n">
-        <v>-1.681326404290318</v>
+        <v>-1.358471064252903</v>
       </c>
       <c r="AE16" t="n">
         <v>11.76908737648015</v>
@@ -2137,7 +2137,7 @@
         <v>2.030937895387919</v>
       </c>
       <c r="AG16" t="n">
-        <v>8.056823076801912</v>
+        <v>8.379678416839326</v>
       </c>
     </row>
     <row r="17">
@@ -2150,7 +2150,7 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>0.04050626109830331</v>
+        <v>0.03987785433991763</v>
       </c>
       <c r="D17" t="n">
         <v>-0.005388613119527071</v>
@@ -2171,7 +2171,7 @@
         <v>-0.06480118373964831</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.07333637265200189</v>
+        <v>-0.07388622856558937</v>
       </c>
       <c r="K17" t="n">
         <v>-0.1311765075480258</v>
@@ -2192,55 +2192,55 @@
         <v>0.06505464253193215</v>
       </c>
       <c r="Q17" t="n">
-        <v>-0.1994903210431524</v>
+        <v>-0.009377515486100056</v>
       </c>
       <c r="R17" t="n">
         <v>-0.001113448529694407</v>
       </c>
       <c r="S17" t="n">
-        <v>-0.05521025114443882</v>
+        <v>-0.05822933162734854</v>
       </c>
       <c r="T17" t="n">
         <v>-0.3470226020070264</v>
       </c>
       <c r="U17" t="n">
-        <v>-0.002032645239559907</v>
+        <v>0.007189188363337521</v>
       </c>
       <c r="V17" t="n">
-        <v>0.007189188363337521</v>
+        <v>-0.1100018830433096</v>
       </c>
       <c r="W17" t="n">
-        <v>-0.1096019878334278</v>
+        <v>7.960848584148697e-05</v>
       </c>
       <c r="X17" t="n">
-        <v>7.960848584148697e-05</v>
+        <v>-0.1365876979522292</v>
       </c>
       <c r="Y17" t="n">
-        <v>-0.1365876979522292</v>
+        <v>-0.08101329952176532</v>
       </c>
       <c r="Z17" t="n">
-        <v>-0.08101329952176532</v>
+        <v>1.842108826591581</v>
       </c>
       <c r="AA17" t="n">
-        <v>1.842108826591581</v>
+        <v>-0.05218090395224684</v>
       </c>
       <c r="AB17" t="n">
-        <v>-0.05218090395224684</v>
+        <v>0.03570594776254914</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.03570594776254914</v>
+        <v>-0.06860644994615983</v>
       </c>
       <c r="AD17" t="n">
-        <v>-1.871859727385615</v>
+        <v>-1.974093539248946</v>
       </c>
       <c r="AE17" t="n">
-        <v>14.3740775733138</v>
+        <v>14.37418480895472</v>
       </c>
       <c r="AF17" t="n">
         <v>1.848962917049874</v>
       </c>
       <c r="AG17" t="n">
-        <v>10.65325492887831</v>
+        <v>10.5511283526559</v>
       </c>
     </row>
     <row r="18">
@@ -2253,7 +2253,7 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.03006374480832288</v>
+        <v>-0.03013988313469768</v>
       </c>
       <c r="D18" t="n">
         <v>-0.05696627717474828</v>
@@ -2274,7 +2274,7 @@
         <v>-0.09015124378579031</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.1660032211069766</v>
+        <v>-0.1660698421425545</v>
       </c>
       <c r="K18" t="n">
         <v>-0.2897705394874062</v>
@@ -2295,46 +2295,46 @@
         <v>0.1605831548301338</v>
       </c>
       <c r="Q18" t="n">
-        <v>-0.1753295510427152</v>
+        <v>-0.001981454673160327</v>
       </c>
       <c r="R18" t="n">
         <v>-0.0009907273365801633</v>
       </c>
       <c r="S18" t="n">
-        <v>-0.1088014597977496</v>
+        <v>-0.09932052373790583</v>
       </c>
       <c r="T18" t="n">
         <v>-0.3241223957680864</v>
       </c>
       <c r="U18" t="n">
-        <v>-0.00360922089980187</v>
+        <v>0.06618577597228457</v>
       </c>
       <c r="V18" t="n">
-        <v>0.06618577597228457</v>
+        <v>-0.2281537224795623</v>
       </c>
       <c r="W18" t="n">
-        <v>-0.2281052708173238</v>
+        <v>0</v>
       </c>
       <c r="X18" t="n">
-        <v>0</v>
+        <v>-0.3092557004259793</v>
       </c>
       <c r="Y18" t="n">
-        <v>-0.3092557004259793</v>
+        <v>-0.01046804714759122</v>
       </c>
       <c r="Z18" t="n">
-        <v>-0.01046804714759122</v>
+        <v>1.668969045666612</v>
       </c>
       <c r="AA18" t="n">
-        <v>1.668969045666612</v>
+        <v>-0.2974052605301021</v>
       </c>
       <c r="AB18" t="n">
-        <v>-0.2974052605301021</v>
+        <v>0.0607841328736138</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.0607841328736138</v>
+        <v>-0.028535357151793</v>
       </c>
       <c r="AD18" t="n">
-        <v>-2.722493136060427</v>
+        <v>-2.689046844765642</v>
       </c>
       <c r="AE18" t="n">
         <v>11.25392851252065</v>
@@ -2343,7 +2343,7 @@
         <v>2.480869506725185</v>
       </c>
       <c r="AG18" t="n">
-        <v>6.050565869735037</v>
+        <v>6.084012161029822</v>
       </c>
     </row>
     <row r="19">
@@ -2398,46 +2398,46 @@
         <v>0.08123286623569242</v>
       </c>
       <c r="Q19" t="n">
-        <v>-0.04654843767110486</v>
+        <v>-0.1067066786298899</v>
       </c>
       <c r="R19" t="n">
         <v>-0.002636530300403404</v>
       </c>
       <c r="S19" t="n">
-        <v>-0.1101502935196483</v>
+        <v>-0.1156501202619924</v>
       </c>
       <c r="T19" t="n">
         <v>-0.04881952625554501</v>
       </c>
       <c r="U19" t="n">
-        <v>-0.0527629560332246</v>
+        <v>1.379630375866064</v>
       </c>
       <c r="V19" t="n">
-        <v>1.379630375866064</v>
+        <v>-0.09696392745091896</v>
       </c>
       <c r="W19" t="n">
-        <v>-0.09696392745091896</v>
+        <v>0.04184722587175884</v>
       </c>
       <c r="X19" t="n">
-        <v>0.04184722587175884</v>
+        <v>-0.2688910904384814</v>
       </c>
       <c r="Y19" t="n">
-        <v>-0.2688910904384814</v>
+        <v>0.1392097960852559</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.1392097960852559</v>
+        <v>1.445245088490034</v>
       </c>
       <c r="AA19" t="n">
-        <v>1.445245088490034</v>
+        <v>-0.08365519128142866</v>
       </c>
       <c r="AB19" t="n">
-        <v>-0.08365519128142866</v>
+        <v>0.1150521858683806</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.1150521858683806</v>
+        <v>-0.02600328465663477</v>
       </c>
       <c r="AD19" t="n">
-        <v>-1.496541490112216</v>
+        <v>-1.194454737114753</v>
       </c>
       <c r="AE19" t="n">
         <v>9.881465367855055</v>
@@ -2446,7 +2446,7 @@
         <v>3.297158965890005</v>
       </c>
       <c r="AG19" t="n">
-        <v>5.087764911852834</v>
+        <v>5.389851664850298</v>
       </c>
     </row>
     <row r="20">
@@ -2459,7 +2459,7 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1345088762483289</v>
+        <v>0.1337038556268655</v>
       </c>
       <c r="D20" t="n">
         <v>-0.05502040578418128</v>
@@ -2480,7 +2480,7 @@
         <v>-0.06887900254868359</v>
       </c>
       <c r="J20" t="n">
-        <v>-0.1871313200407501</v>
+        <v>-0.1878357130845307</v>
       </c>
       <c r="K20" t="n">
         <v>-0.2746237006893114</v>
@@ -2501,55 +2501,55 @@
         <v>0.02641493699033463</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.003190170991470745</v>
+        <v>-0.008790415387021418</v>
       </c>
       <c r="R20" t="n">
         <v>-0.001894564069414078</v>
       </c>
       <c r="S20" t="n">
-        <v>-0.09399030221285845</v>
+        <v>-0.09666277180028435</v>
       </c>
       <c r="T20" t="n">
         <v>-0.1626835813422368</v>
       </c>
       <c r="U20" t="n">
-        <v>-0.004200443444321521</v>
+        <v>0.01434886773793887</v>
       </c>
       <c r="V20" t="n">
-        <v>0.01434886773793887</v>
+        <v>-0.1447169776733954</v>
       </c>
       <c r="W20" t="n">
-        <v>-0.1442046918233732</v>
+        <v>0.0008931388307105969</v>
       </c>
       <c r="X20" t="n">
-        <v>0.0008931388307105969</v>
+        <v>-0.2987487398567908</v>
       </c>
       <c r="Y20" t="n">
-        <v>-0.2987487398567908</v>
+        <v>-0.05405667217505929</v>
       </c>
       <c r="Z20" t="n">
-        <v>-0.05405667217505929</v>
+        <v>1.636607851810394</v>
       </c>
       <c r="AA20" t="n">
-        <v>1.636607851810394</v>
+        <v>-0.2617361715261289</v>
       </c>
       <c r="AB20" t="n">
-        <v>-0.2617361715261289</v>
+        <v>0.233175306703107</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.233175306703107</v>
+        <v>-0.02208543395444281</v>
       </c>
       <c r="AD20" t="n">
-        <v>-1.698814710905883</v>
+        <v>-1.367929584807132</v>
       </c>
       <c r="AE20" t="n">
-        <v>11.99716097123871</v>
+        <v>11.99734307940836</v>
       </c>
       <c r="AF20" t="n">
         <v>3.119152271531618</v>
       </c>
       <c r="AG20" t="n">
-        <v>7.179193988801213</v>
+        <v>7.510261223069611</v>
       </c>
     </row>
     <row r="21">
@@ -2562,7 +2562,7 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>0.02501270293021713</v>
+        <v>0.0238155727225505</v>
       </c>
       <c r="D21" t="n">
         <v>-0.04786427216330914</v>
@@ -2583,7 +2583,7 @@
         <v>-0.08333748761261342</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.1625423393945749</v>
+        <v>-0.1635898283262831</v>
       </c>
       <c r="K21" t="n">
         <v>-0.2900655210408875</v>
@@ -2604,55 +2604,55 @@
         <v>-0.002294791107121729</v>
       </c>
       <c r="Q21" t="n">
-        <v>-0.04259841074205894</v>
+        <v>-0.001803551104885701</v>
       </c>
       <c r="R21" t="n">
         <v>-0.004028821334809671</v>
       </c>
       <c r="S21" t="n">
-        <v>-0.1404427939278815</v>
+        <v>-0.1445890107858145</v>
       </c>
       <c r="T21" t="n">
         <v>-0.2266619783028998</v>
       </c>
       <c r="U21" t="n">
-        <v>-0.01149933844841817</v>
+        <v>0.01071064103520192</v>
       </c>
       <c r="V21" t="n">
-        <v>0.01071064103520192</v>
+        <v>-0.3503391781017794</v>
       </c>
       <c r="W21" t="n">
-        <v>-0.3495773679696279</v>
+        <v>-0.000385942459892275</v>
       </c>
       <c r="X21" t="n">
-        <v>-0.000385942459892275</v>
+        <v>-0.3567659378057634</v>
       </c>
       <c r="Y21" t="n">
-        <v>-0.3567659378057634</v>
+        <v>-0.01283280162287454</v>
       </c>
       <c r="Z21" t="n">
-        <v>-0.01283280162287454</v>
+        <v>1.014625049018254</v>
       </c>
       <c r="AA21" t="n">
-        <v>1.014625049018254</v>
+        <v>-0.3217817741888539</v>
       </c>
       <c r="AB21" t="n">
-        <v>-0.3217817741888539</v>
+        <v>0.07017307020429679</v>
       </c>
       <c r="AC21" t="n">
-        <v>0.07017307020429679</v>
+        <v>0.03004761477359561</v>
       </c>
       <c r="AD21" t="n">
-        <v>-4.347034464661159</v>
+        <v>-3.768416833890145</v>
       </c>
       <c r="AE21" t="n">
-        <v>10.64084482047585</v>
+        <v>10.64092224178287</v>
       </c>
       <c r="AF21" t="n">
         <v>3.253217425700312</v>
       </c>
       <c r="AG21" t="n">
-        <v>3.040592930114375</v>
+        <v>3.619287982192414</v>
       </c>
     </row>
     <row r="22">
@@ -2665,7 +2665,7 @@
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>0.02484063791088694</v>
+        <v>0.001845563709471286</v>
       </c>
       <c r="D22" t="n">
         <v>-0.03603499490108308</v>
@@ -2686,7 +2686,7 @@
         <v>-0.09201523028278108</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.09648359713238065</v>
+        <v>-0.1166042870586193</v>
       </c>
       <c r="K22" t="n">
         <v>-0.1708002711117627</v>
@@ -2707,46 +2707,46 @@
         <v>0.05791102782839777</v>
       </c>
       <c r="Q22" t="n">
-        <v>-0.1858965438979213</v>
+        <v>-0.003296806539425765</v>
       </c>
       <c r="R22" t="n">
         <v>-0.002474948182575837</v>
       </c>
       <c r="S22" t="n">
-        <v>-0.0714532807204591</v>
+        <v>-0.07517432305036229</v>
       </c>
       <c r="T22" t="n">
         <v>-0.3199442673283664</v>
       </c>
       <c r="U22" t="n">
-        <v>-0.008385304961407075</v>
+        <v>0.004117112549703064</v>
       </c>
       <c r="V22" t="n">
-        <v>0.004117112549703064</v>
+        <v>-0.1788664200692573</v>
       </c>
       <c r="W22" t="n">
-        <v>-0.1642331910319928</v>
+        <v>0</v>
       </c>
       <c r="X22" t="n">
-        <v>0</v>
+        <v>-0.2028241843715536</v>
       </c>
       <c r="Y22" t="n">
-        <v>-0.2028241843715536</v>
+        <v>-0.02789959171187314</v>
       </c>
       <c r="Z22" t="n">
-        <v>-0.02789959171187314</v>
+        <v>1.816039344702478</v>
       </c>
       <c r="AA22" t="n">
-        <v>1.816039344702478</v>
+        <v>-0.1522226675145052</v>
       </c>
       <c r="AB22" t="n">
-        <v>-0.1522226675145052</v>
+        <v>0.06138591613981749</v>
       </c>
       <c r="AC22" t="n">
-        <v>0.06138591613981749</v>
+        <v>0.01901326383802912</v>
       </c>
       <c r="AD22" t="n">
-        <v>-2.496441871422757</v>
+        <v>-2.21342717305775</v>
       </c>
       <c r="AE22" t="n">
         <v>12.4497784749184</v>
@@ -2755,7 +2755,7 @@
         <v>2.326473128727222</v>
       </c>
       <c r="AG22" t="n">
-        <v>7.626863474768419</v>
+        <v>7.909878173133426</v>
       </c>
     </row>
     <row r="23">
@@ -2768,7 +2768,7 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.05701769216294623</v>
+        <v>-0.05743922104860822</v>
       </c>
       <c r="D23" t="n">
         <v>-0.02452193920656116</v>
@@ -2789,7 +2789,7 @@
         <v>-0.01678464188764933</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.02438364329584911</v>
+        <v>-0.02475248107080335</v>
       </c>
       <c r="K23" t="n">
         <v>-0.2001415927053884</v>
@@ -2810,46 +2810,46 @@
         <v>-0.06249185790008094</v>
       </c>
       <c r="Q23" t="n">
-        <v>-0.1719031840306497</v>
+        <v>-0.008781274214656853</v>
       </c>
       <c r="R23" t="n">
         <v>-0.007843410102985032</v>
       </c>
       <c r="S23" t="n">
-        <v>-0.05782445563925576</v>
+        <v>-0.05949671913911104</v>
       </c>
       <c r="T23" t="n">
         <v>-0.4639626956433284</v>
       </c>
       <c r="U23" t="n">
-        <v>-0.01098127106140163</v>
+        <v>0.00940176592196341</v>
       </c>
       <c r="V23" t="n">
-        <v>0.00940176592196341</v>
+        <v>-0.05144093279698524</v>
       </c>
       <c r="W23" t="n">
-        <v>-0.05117268714247308</v>
+        <v>0</v>
       </c>
       <c r="X23" t="n">
-        <v>0</v>
+        <v>-0.191754109025529</v>
       </c>
       <c r="Y23" t="n">
-        <v>-0.191754109025529</v>
+        <v>-0.09730982413183514</v>
       </c>
       <c r="Z23" t="n">
-        <v>-0.09730982413183514</v>
+        <v>1.772541662036867</v>
       </c>
       <c r="AA23" t="n">
-        <v>1.772541662036867</v>
+        <v>-0.02905311724059727</v>
       </c>
       <c r="AB23" t="n">
-        <v>-0.02905311724059727</v>
+        <v>0.146702538617229</v>
       </c>
       <c r="AC23" t="n">
-        <v>0.146702538617229</v>
+        <v>-0.08869975580567298</v>
       </c>
       <c r="AD23" t="n">
-        <v>-2.241233552365195</v>
+        <v>-1.874884514531069</v>
       </c>
       <c r="AE23" t="n">
         <v>13.03096986013981</v>
@@ -2858,7 +2858,7 @@
         <v>2.496649824908592</v>
       </c>
       <c r="AG23" t="n">
-        <v>8.293086482866025</v>
+        <v>8.659435520700152</v>
       </c>
     </row>
     <row r="24">
@@ -2871,7 +2871,7 @@
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.1162814136581847</v>
+        <v>-0.1164048952466801</v>
       </c>
       <c r="D24" t="n">
         <v>-0.05127256239563234</v>
@@ -2892,7 +2892,7 @@
         <v>-0.0117941213804539</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.04809350791883561</v>
+        <v>-0.04820155430876911</v>
       </c>
       <c r="K24" t="n">
         <v>-0.3225255487472818</v>
@@ -2913,55 +2913,55 @@
         <v>0.131340568950823</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.004159369000284864</v>
+        <v>-0.001733920464697615</v>
       </c>
       <c r="R24" t="n">
         <v>-0.00216610602443161</v>
       </c>
       <c r="S24" t="n">
-        <v>-0.07860728792527731</v>
+        <v>-0.08312925071707611</v>
       </c>
       <c r="T24" t="n">
         <v>-0.4298507273623662</v>
       </c>
       <c r="U24" t="n">
-        <v>-0.002590865029641853</v>
+        <v>0.005181130545938043</v>
       </c>
       <c r="V24" t="n">
-        <v>0.005181130545938043</v>
+        <v>-0.09896199447332185</v>
       </c>
       <c r="W24" t="n">
-        <v>-0.09888341528064294</v>
+        <v>6.198754045207722e-05</v>
       </c>
       <c r="X24" t="n">
-        <v>6.198754045207722e-05</v>
+        <v>-0.2426018787760083</v>
       </c>
       <c r="Y24" t="n">
-        <v>-0.2426018787760083</v>
+        <v>-0.06394209112704055</v>
       </c>
       <c r="Z24" t="n">
-        <v>-0.06394209112704055</v>
+        <v>1.68462712842111</v>
       </c>
       <c r="AA24" t="n">
-        <v>1.68462712842111</v>
+        <v>-0.05617141471529325</v>
       </c>
       <c r="AB24" t="n">
-        <v>-0.05617141471529325</v>
+        <v>0.1596803015630923</v>
       </c>
       <c r="AC24" t="n">
-        <v>0.1596803015630923</v>
+        <v>-0.1006975673872896</v>
       </c>
       <c r="AD24" t="n">
-        <v>-3.333678464299149</v>
+        <v>-3.237691964380909</v>
       </c>
       <c r="AE24" t="n">
-        <v>13.35229821660199</v>
+        <v>13.35240945679437</v>
       </c>
       <c r="AF24" t="n">
         <v>2.367888785783177</v>
       </c>
       <c r="AG24" t="n">
-        <v>7.650730966519666</v>
+        <v>7.746828706630286</v>
       </c>
     </row>
     <row r="25">
@@ -2974,7 +2974,7 @@
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>0.1211192177434643</v>
+        <v>0.1209007902933625</v>
       </c>
       <c r="D25" t="n">
         <v>-0.003173382710143619</v>
@@ -2995,7 +2995,7 @@
         <v>-0.00702293514870447</v>
       </c>
       <c r="J25" t="n">
-        <v>-0.00795965837237558</v>
+        <v>-0.008150782391214636</v>
       </c>
       <c r="K25" t="n">
         <v>-0.1816188649563365</v>
@@ -3016,46 +3016,46 @@
         <v>0.08643642666148214</v>
       </c>
       <c r="Q25" t="n">
-        <v>-0.1674084413891998</v>
+        <v>-0.002307709290667974</v>
       </c>
       <c r="R25" t="n">
         <v>-0.0007699172756930551</v>
       </c>
       <c r="S25" t="n">
-        <v>-0.05760845097504293</v>
+        <v>-0.06081634640011031</v>
       </c>
       <c r="T25" t="n">
         <v>-0.410285392767733</v>
       </c>
       <c r="U25" t="n">
-        <v>-0.003565998893051836</v>
+        <v>0.003074228748897981</v>
       </c>
       <c r="V25" t="n">
-        <v>0.003074228748897981</v>
+        <v>-0.2236513122829654</v>
       </c>
       <c r="W25" t="n">
-        <v>-0.2235123129965371</v>
+        <v>5.504283785891914e-05</v>
       </c>
       <c r="X25" t="n">
-        <v>5.504283785891914e-05</v>
+        <v>-0.1705853632174941</v>
       </c>
       <c r="Y25" t="n">
-        <v>-0.1705853632174941</v>
+        <v>-0.009476471008226621</v>
       </c>
       <c r="Z25" t="n">
-        <v>-0.009476471008226621</v>
+        <v>1.780641514020425</v>
       </c>
       <c r="AA25" t="n">
-        <v>1.780641514020425</v>
+        <v>-0.000256866576674956</v>
       </c>
       <c r="AB25" t="n">
-        <v>-0.000256866576674956</v>
+        <v>0.1617026503197399</v>
       </c>
       <c r="AC25" t="n">
-        <v>0.1617026503197399</v>
+        <v>0.1542270512310876</v>
       </c>
       <c r="AD25" t="n">
-        <v>-1.71937003243905</v>
+        <v>-0.7063086714815477</v>
       </c>
       <c r="AE25" t="n">
         <v>14.09205416163184</v>
@@ -3064,7 +3064,7 @@
         <v>2.756894535999121</v>
       </c>
       <c r="AG25" t="n">
-        <v>9.615789593193673</v>
+        <v>10.62885095415118</v>
       </c>
     </row>
     <row r="26">
@@ -3077,7 +3077,7 @@
         <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>0.03590587337207014</v>
+        <v>0.03579790461913165</v>
       </c>
       <c r="D26" t="n">
         <v>-0.01838012962347627</v>
@@ -3098,7 +3098,7 @@
         <v>-0.02838748525245819</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.1026662843470553</v>
+        <v>-0.1027607570058765</v>
       </c>
       <c r="K26" t="n">
         <v>-0.1808997576825299</v>
@@ -3119,46 +3119,46 @@
         <v>0.1267855588748059</v>
       </c>
       <c r="Q26" t="n">
-        <v>-0.1844908186597403</v>
+        <v>-0.02271317914201341</v>
       </c>
       <c r="R26" t="n">
         <v>-0.001202746133544725</v>
       </c>
       <c r="S26" t="n">
-        <v>-0.04945648988865176</v>
+        <v>-0.05080616923365613</v>
       </c>
       <c r="T26" t="n">
         <v>-0.3573182365968586</v>
       </c>
       <c r="U26" t="n">
-        <v>-0.003198025684521008</v>
+        <v>0.002405492267089451</v>
       </c>
       <c r="V26" t="n">
-        <v>0.002405492267089451</v>
+        <v>-0.1548602754122925</v>
       </c>
       <c r="W26" t="n">
-        <v>-0.1547915680240589</v>
+        <v>-5.737943374617431e-05</v>
       </c>
       <c r="X26" t="n">
-        <v>-5.737943374617431e-05</v>
+        <v>-0.1628119305180291</v>
       </c>
       <c r="Y26" t="n">
-        <v>-0.1628119305180291</v>
+        <v>-0.01306767702413507</v>
       </c>
       <c r="Z26" t="n">
-        <v>-0.01306767702413507</v>
+        <v>1.858801542215638</v>
       </c>
       <c r="AA26" t="n">
-        <v>1.858801542215638</v>
+        <v>-0.1178200963918431</v>
       </c>
       <c r="AB26" t="n">
-        <v>-0.1178200963918431</v>
+        <v>0.1151802791739185</v>
       </c>
       <c r="AC26" t="n">
-        <v>0.1151802791739185</v>
+        <v>0.0398554604477041</v>
       </c>
       <c r="AD26" t="n">
-        <v>-1.192840131257181</v>
+        <v>-0.7559436167032322</v>
       </c>
       <c r="AE26" t="n">
         <v>13.1559824118403</v>
@@ -3167,7 +3167,7 @@
         <v>2.468263610591526</v>
       </c>
       <c r="AG26" t="n">
-        <v>9.494878669991595</v>
+        <v>9.931775184545543</v>
       </c>
     </row>
     <row r="27">
@@ -3222,46 +3222,46 @@
         <v>0.1242214105494453</v>
       </c>
       <c r="Q27" t="n">
-        <v>-0.1578216555471988</v>
+        <v>0</v>
       </c>
       <c r="R27" t="n">
         <v>-0.0006313709008554685</v>
       </c>
       <c r="S27" t="n">
-        <v>-0.07770728601712898</v>
+        <v>-0.0820561108438248</v>
       </c>
       <c r="T27" t="n">
         <v>-0.3162482246900605</v>
       </c>
       <c r="U27" t="n">
-        <v>-0.006592031008040469</v>
+        <v>0</v>
       </c>
       <c r="V27" t="n">
-        <v>0</v>
+        <v>-0.1499130289642441</v>
       </c>
       <c r="W27" t="n">
-        <v>-0.1499130289642441</v>
+        <v>-0.0001801301953098411</v>
       </c>
       <c r="X27" t="n">
-        <v>-0.0001801301953098411</v>
+        <v>-0.2165434458863551</v>
       </c>
       <c r="Y27" t="n">
-        <v>-0.2165434458863551</v>
+        <v>-0.004819062807422731</v>
       </c>
       <c r="Z27" t="n">
-        <v>-0.004819062807422731</v>
+        <v>1.732304996017548</v>
       </c>
       <c r="AA27" t="n">
-        <v>1.732304996017548</v>
+        <v>-0.03031446488649711</v>
       </c>
       <c r="AB27" t="n">
-        <v>-0.03031446488649711</v>
+        <v>0.04219664885616636</v>
       </c>
       <c r="AC27" t="n">
-        <v>0.04219664885616636</v>
+        <v>-0.03124082328856044</v>
       </c>
       <c r="AD27" t="n">
-        <v>-1.552836601735071</v>
+        <v>-1.414715203818849</v>
       </c>
       <c r="AE27" t="n">
         <v>11.40694298563118</v>
@@ -3270,7 +3270,7 @@
         <v>2.176770978233852</v>
       </c>
       <c r="AG27" t="n">
-        <v>7.677335405662255</v>
+        <v>7.815456803578478</v>
       </c>
     </row>
     <row r="28">
@@ -3283,7 +3283,7 @@
         <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>0.01066982647728075</v>
+        <v>0.0097001115323988</v>
       </c>
       <c r="D28" t="n">
         <v>-0.05165670186935776</v>
@@ -3304,7 +3304,7 @@
         <v>-0.08549684360882658</v>
       </c>
       <c r="J28" t="n">
-        <v>-0.1333905005757458</v>
+        <v>-0.1342390011525176</v>
       </c>
       <c r="K28" t="n">
         <v>-0.230630033806269</v>
@@ -3325,46 +3325,46 @@
         <v>0.09741693424620586</v>
       </c>
       <c r="Q28" t="n">
-        <v>-0.1650141077394742</v>
+        <v>-0.008463160235523267</v>
       </c>
       <c r="R28" t="n">
         <v>-0.006316843570779088</v>
       </c>
       <c r="S28" t="n">
-        <v>-0.06368272349473429</v>
+        <v>-0.06640234148976595</v>
       </c>
       <c r="T28" t="n">
         <v>-0.3384584338635786</v>
       </c>
       <c r="U28" t="n">
-        <v>-0.01004483602926698</v>
+        <v>0.002131301729975717</v>
       </c>
       <c r="V28" t="n">
-        <v>0.002131301729975717</v>
+        <v>-0.244566810508596</v>
       </c>
       <c r="W28" t="n">
-        <v>-0.2439497191800347</v>
+        <v>0</v>
       </c>
       <c r="X28" t="n">
-        <v>0</v>
+        <v>-0.1743988414938286</v>
       </c>
       <c r="Y28" t="n">
-        <v>-0.1743988414938286</v>
+        <v>-0.0187677418749836</v>
       </c>
       <c r="Z28" t="n">
-        <v>-0.0187677418749836</v>
+        <v>1.644457790449553</v>
       </c>
       <c r="AA28" t="n">
-        <v>1.644457790449553</v>
+        <v>-0.2933569295274565</v>
       </c>
       <c r="AB28" t="n">
-        <v>-0.2933569295274565</v>
+        <v>0.04566274694072794</v>
       </c>
       <c r="AC28" t="n">
-        <v>0.04566274694072794</v>
+        <v>0.07546828095951706</v>
       </c>
       <c r="AD28" t="n">
-        <v>-2.660812271222367</v>
+        <v>-1.916602226486096</v>
       </c>
       <c r="AE28" t="n">
         <v>14.90906696606726</v>
@@ -3373,7 +3373,7 @@
         <v>2.79206825249104</v>
       </c>
       <c r="AG28" t="n">
-        <v>9.456186442353856</v>
+        <v>10.20039648709013</v>
       </c>
     </row>
     <row r="29">
@@ -3386,7 +3386,7 @@
         <v>0.0004404538507627297</v>
       </c>
       <c r="C29" t="n">
-        <v>0.135474195652802</v>
+        <v>0.1342485123916262</v>
       </c>
       <c r="D29" t="n">
         <v>-0.01445895034125077</v>
@@ -3407,7 +3407,7 @@
         <v>0.0043158007088385</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.09659787728033171</v>
+        <v>-0.09767035013386045</v>
       </c>
       <c r="K29" t="n">
         <v>-0.1738941422812645</v>
@@ -3428,46 +3428,46 @@
         <v>-0.03906564621522744</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.03087050022430499</v>
+        <v>-0.006144619788438694</v>
       </c>
       <c r="R29" t="n">
         <v>-0.002313750734141482</v>
       </c>
       <c r="S29" t="n">
-        <v>-0.100812219159674</v>
+        <v>-0.1049841757279839</v>
       </c>
       <c r="T29" t="n">
         <v>0.002904742451408175</v>
       </c>
       <c r="U29" t="n">
-        <v>-0.01455627695838061</v>
+        <v>0</v>
       </c>
       <c r="V29" t="n">
-        <v>0</v>
+        <v>-0.09012750124281915</v>
       </c>
       <c r="W29" t="n">
-        <v>-0.08934752098570733</v>
+        <v>-0.0003305358191630689</v>
       </c>
       <c r="X29" t="n">
-        <v>-0.0003305358191630689</v>
+        <v>-0.307442215238001</v>
       </c>
       <c r="Y29" t="n">
-        <v>-0.307442215238001</v>
+        <v>0.009216639380475268</v>
       </c>
       <c r="Z29" t="n">
-        <v>0.009216639380475268</v>
+        <v>1.738618593728726</v>
       </c>
       <c r="AA29" t="n">
-        <v>1.738618593728726</v>
+        <v>-0.1339330134230141</v>
       </c>
       <c r="AB29" t="n">
-        <v>-0.1339330134230141</v>
+        <v>0.248052521384538</v>
       </c>
       <c r="AC29" t="n">
-        <v>0.248052521384538</v>
+        <v>0.1380915755905483</v>
       </c>
       <c r="AD29" t="n">
-        <v>-0.445375982062657</v>
+        <v>0.421323962360644</v>
       </c>
       <c r="AE29" t="n">
         <v>10.6625181294375</v>
@@ -3476,7 +3476,7 @@
         <v>2.96434199520753</v>
       </c>
       <c r="AG29" t="n">
-        <v>7.252800152167314</v>
+        <v>8.119500096590615</v>
       </c>
     </row>
     <row r="30">
@@ -3489,7 +3489,7 @@
         <v>0.002922553218555146</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.03352717131379954</v>
+        <v>-0.035338369499292</v>
       </c>
       <c r="D30" t="n">
         <v>-0.01175661892491891</v>
@@ -3510,7 +3510,7 @@
         <v>-0.1136983221457946</v>
       </c>
       <c r="J30" t="n">
-        <v>-0.0739471738270235</v>
+        <v>-0.07553197223932939</v>
       </c>
       <c r="K30" t="n">
         <v>-0.1673732560508098</v>
@@ -3531,55 +3531,55 @@
         <v>-0.01805355592308459</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.01378823483758099</v>
+        <v>-0.03268278159033097</v>
       </c>
       <c r="R30" t="n">
         <v>-0.002818483321196309</v>
       </c>
       <c r="S30" t="n">
-        <v>-0.0135651553520089</v>
+        <v>-0.01370605956870724</v>
       </c>
       <c r="T30" t="n">
         <v>-0.3841205598028452</v>
       </c>
       <c r="U30" t="n">
-        <v>-0.1042399239935072</v>
+        <v>0.04134125182631532</v>
       </c>
       <c r="V30" t="n">
-        <v>0.04134125182631532</v>
+        <v>-0.0568571146392447</v>
       </c>
       <c r="W30" t="n">
-        <v>-0.05570453397574949</v>
+        <v>0.03007911475986191</v>
       </c>
       <c r="X30" t="n">
-        <v>0.03007911475986191</v>
+        <v>-0.09052390515242217</v>
       </c>
       <c r="Y30" t="n">
-        <v>-0.09052390515242217</v>
+        <v>0.00189893265201366</v>
       </c>
       <c r="Z30" t="n">
-        <v>0.00189893265201366</v>
+        <v>1.501284664139907</v>
       </c>
       <c r="AA30" t="n">
-        <v>1.501284664139907</v>
+        <v>-0.08465109450326329</v>
       </c>
       <c r="AB30" t="n">
-        <v>-0.08465109450326329</v>
+        <v>0.09950743356071774</v>
       </c>
       <c r="AC30" t="n">
-        <v>0.09950743356071774</v>
+        <v>-0.09675979702385633</v>
       </c>
       <c r="AD30" t="n">
-        <v>-3.020347065099521</v>
+        <v>-2.315639296001383</v>
       </c>
       <c r="AE30" t="n">
-        <v>12.26650352013645</v>
+        <v>12.26781624115958</v>
       </c>
       <c r="AF30" t="n">
         <v>3.157693416302038</v>
       </c>
       <c r="AG30" t="n">
-        <v>6.088463038734886</v>
+        <v>6.794483528856158</v>
       </c>
     </row>
     <row r="31">
@@ -3592,7 +3592,7 @@
         <v>0.0002978358599740457</v>
       </c>
       <c r="C31" t="n">
-        <v>0.03213098024695798</v>
+        <v>0.03142292375291122</v>
       </c>
       <c r="D31" t="n">
         <v>-0.05108461766930342</v>
@@ -3613,7 +3613,7 @@
         <v>-0.1562311835472462</v>
       </c>
       <c r="J31" t="n">
-        <v>-0.1521493314381205</v>
+        <v>-0.1527688808704114</v>
       </c>
       <c r="K31" t="n">
         <v>-0.2808136140543632</v>
@@ -3634,55 +3634,55 @@
         <v>-0.04117989301347329</v>
       </c>
       <c r="Q31" t="n">
-        <v>-0.1377137400637965</v>
+        <v>-0.00208485101981832</v>
       </c>
       <c r="R31" t="n">
         <v>-0.009814798665344692</v>
       </c>
       <c r="S31" t="n">
-        <v>-0.06970237693629165</v>
+        <v>-0.07260184777581674</v>
       </c>
       <c r="T31" t="n">
         <v>-0.3619090372874325</v>
       </c>
       <c r="U31" t="n">
-        <v>-0.02248610617888018</v>
+        <v>0.004159741412002104</v>
       </c>
       <c r="V31" t="n">
-        <v>0.004159741412002104</v>
+        <v>-0.2669900492769576</v>
       </c>
       <c r="W31" t="n">
-        <v>-0.2665394678716551</v>
+        <v>-0.0002978358599740457</v>
       </c>
       <c r="X31" t="n">
-        <v>-0.0002978358599740457</v>
+        <v>-0.2320076514361891</v>
       </c>
       <c r="Y31" t="n">
-        <v>-0.2320076514361891</v>
+        <v>0.01222321468117648</v>
       </c>
       <c r="Z31" t="n">
-        <v>0.01222321468117648</v>
+        <v>1.64452809842187</v>
       </c>
       <c r="AA31" t="n">
-        <v>1.64452809842187</v>
+        <v>-0.3031319054320287</v>
       </c>
       <c r="AB31" t="n">
-        <v>-0.3031319054320287</v>
+        <v>0.1730939102254399</v>
       </c>
       <c r="AC31" t="n">
-        <v>0.1730939102254399</v>
+        <v>0.0509059380855933</v>
       </c>
       <c r="AD31" t="n">
-        <v>-4.018983435710643</v>
+        <v>-3.655156411060432</v>
       </c>
       <c r="AE31" t="n">
-        <v>12.54315067882748</v>
+        <v>12.54327878527785</v>
       </c>
       <c r="AF31" t="n">
         <v>2.816984400016397</v>
       </c>
       <c r="AG31" t="n">
-        <v>5.707182843100437</v>
+        <v>6.071137974201017</v>
       </c>
     </row>
     <row r="32">
@@ -3737,46 +3737,46 @@
         <v>-0.01667087183367884</v>
       </c>
       <c r="Q32" t="n">
-        <v>-0.1839130426870931</v>
+        <v>0</v>
       </c>
       <c r="R32" t="n">
         <v>-0.01708729536216787</v>
       </c>
       <c r="S32" t="n">
-        <v>-0.04525153822716313</v>
+        <v>-0.04791339341699625</v>
       </c>
       <c r="T32" t="n">
         <v>-0.5254254339507041</v>
       </c>
       <c r="U32" t="n">
-        <v>-0.009354979288477179</v>
+        <v>0</v>
       </c>
       <c r="V32" t="n">
-        <v>0</v>
+        <v>0.03584489644882279</v>
       </c>
       <c r="W32" t="n">
-        <v>0.03584489644882279</v>
+        <v>-0.002872310819178508</v>
       </c>
       <c r="X32" t="n">
-        <v>-0.002872310819178508</v>
+        <v>-0.1309683213402924</v>
       </c>
       <c r="Y32" t="n">
-        <v>-0.1309683213402924</v>
+        <v>-0.1210654711899132</v>
       </c>
       <c r="Z32" t="n">
-        <v>-0.1210654711899132</v>
+        <v>1.782585460461879</v>
       </c>
       <c r="AA32" t="n">
-        <v>1.782585460461879</v>
+        <v>0.004854780936305264</v>
       </c>
       <c r="AB32" t="n">
-        <v>0.004854780936305264</v>
+        <v>0.07321779553341845</v>
       </c>
       <c r="AC32" t="n">
-        <v>0.07321779553341845</v>
+        <v>-0.1954034322000275</v>
       </c>
       <c r="AD32" t="n">
-        <v>-1.554972880726069</v>
+        <v>-1.525559421423126</v>
       </c>
       <c r="AE32" t="n">
         <v>14.04173456276912</v>
@@ -3785,7 +3785,7 @@
         <v>1.700090545577031</v>
       </c>
       <c r="AG32" t="n">
-        <v>10.78667113646602</v>
+        <v>10.81608459576896</v>
       </c>
     </row>
     <row r="33">
@@ -3798,7 +3798,7 @@
         <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>0.01182014788017184</v>
+        <v>0.009733000167742577</v>
       </c>
       <c r="D33" t="n">
         <v>-0.08867205360729043</v>
@@ -3819,7 +3819,7 @@
         <v>-0.1292114234709451</v>
       </c>
       <c r="J33" t="n">
-        <v>-0.3085623073558492</v>
+        <v>-0.3103885616042248</v>
       </c>
       <c r="K33" t="n">
         <v>-0.2537062429655836</v>
@@ -3840,46 +3840,46 @@
         <v>-0.1022884803966865</v>
       </c>
       <c r="Q33" t="n">
-        <v>-0.01239826057006225</v>
+        <v>0</v>
       </c>
       <c r="R33" t="n">
         <v>-0.005766225762193705</v>
       </c>
       <c r="S33" t="n">
-        <v>-0.1393014003664866</v>
+        <v>-0.1451430127430058</v>
       </c>
       <c r="T33" t="n">
         <v>-0.07010990066164101</v>
       </c>
       <c r="U33" t="n">
-        <v>-0.01592090899091532</v>
+        <v>0.004630048990826603</v>
       </c>
       <c r="V33" t="n">
-        <v>0.004630048990826603</v>
+        <v>-0.1061699681320083</v>
       </c>
       <c r="W33" t="n">
-        <v>-0.1048417832240988</v>
+        <v>-0.007525936724989973</v>
       </c>
       <c r="X33" t="n">
-        <v>-0.007525936724989973</v>
+        <v>-0.3398367667531608</v>
       </c>
       <c r="Y33" t="n">
-        <v>-0.3398367667531608</v>
+        <v>-0.04777631202061359</v>
       </c>
       <c r="Z33" t="n">
-        <v>-0.04777631202061359</v>
+        <v>1.692101319966596</v>
       </c>
       <c r="AA33" t="n">
-        <v>1.692101319966596</v>
+        <v>-0.3749577094189353</v>
       </c>
       <c r="AB33" t="n">
-        <v>-0.3749577094189353</v>
+        <v>0.2403033457363206</v>
       </c>
       <c r="AC33" t="n">
-        <v>0.2403033457363206</v>
+        <v>-0.06963157584844971</v>
       </c>
       <c r="AD33" t="n">
-        <v>-2.938616151824918</v>
+        <v>-2.906495438549417</v>
       </c>
       <c r="AE33" t="n">
         <v>10.61390266985545</v>
@@ -3888,7 +3888,7 @@
         <v>3.031725283185861</v>
       </c>
       <c r="AG33" t="n">
-        <v>4.643561234844674</v>
+        <v>4.675681948120174</v>
       </c>
     </row>
     <row r="34">
@@ -3901,7 +3901,7 @@
         <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>0.03675776513350145</v>
+        <v>0.03650585821857492</v>
       </c>
       <c r="D34" t="n">
         <v>-0.01751750232085277</v>
@@ -3922,7 +3922,7 @@
         <v>-0.008045334845812872</v>
       </c>
       <c r="J34" t="n">
-        <v>-0.04490310374765161</v>
+        <v>-0.04512352229821234</v>
       </c>
       <c r="K34" t="n">
         <v>-0.1795350075130328</v>
@@ -3943,46 +3943,46 @@
         <v>-0.0004674062084320889</v>
       </c>
       <c r="Q34" t="n">
-        <v>-0.1469580624626828</v>
+        <v>-0.007593086145383525</v>
       </c>
       <c r="R34" t="n">
         <v>-0.01480344705009463</v>
       </c>
       <c r="S34" t="n">
-        <v>-0.02714217480068188</v>
+        <v>-0.02668346104972013</v>
       </c>
       <c r="T34" t="n">
         <v>-0.3496628497965747</v>
       </c>
       <c r="U34" t="n">
-        <v>-0.00630308469110714</v>
+        <v>0.001910753585553961</v>
       </c>
       <c r="V34" t="n">
-        <v>0.001910753585553961</v>
+        <v>-0.2299790593165399</v>
       </c>
       <c r="W34" t="n">
-        <v>-0.229818754916132</v>
+        <v>0.004785998754033904</v>
       </c>
       <c r="X34" t="n">
-        <v>0.004785998754033904</v>
+        <v>-0.08469376012095642</v>
       </c>
       <c r="Y34" t="n">
-        <v>-0.08469376012095642</v>
+        <v>0.002173200999044765</v>
       </c>
       <c r="Z34" t="n">
-        <v>0.002173200999044765</v>
+        <v>1.736070836475786</v>
       </c>
       <c r="AA34" t="n">
-        <v>1.736070836475786</v>
+        <v>-0.1076512542135793</v>
       </c>
       <c r="AB34" t="n">
-        <v>-0.1076512542135793</v>
+        <v>0.1536516028968188</v>
       </c>
       <c r="AC34" t="n">
-        <v>0.1536516028968188</v>
+        <v>0.1169510938134758</v>
       </c>
       <c r="AD34" t="n">
-        <v>-1.425207382882489</v>
+        <v>-0.704444160747245</v>
       </c>
       <c r="AE34" t="n">
         <v>13.34067530921292</v>
@@ -3991,7 +3991,7 @@
         <v>2.57710761741724</v>
       </c>
       <c r="AG34" t="n">
-        <v>9.338360308913188</v>
+        <v>10.05912353104843</v>
       </c>
     </row>
     <row r="35">
@@ -4004,7 +4004,7 @@
         <v>0.0002525940662116038</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.07108529390909497</v>
+        <v>-0.07194533081424266</v>
       </c>
       <c r="D35" t="n">
         <v>-0.1029340095784494</v>
@@ -4025,7 +4025,7 @@
         <v>-0.1474328271605639</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.2458797488745472</v>
+        <v>-0.2466322811665514</v>
       </c>
       <c r="K35" t="n">
         <v>-0.2142025198016358</v>
@@ -4046,46 +4046,46 @@
         <v>0.05456201811287884</v>
       </c>
       <c r="Q35" t="n">
-        <v>0.01685774967892124</v>
+        <v>-0.003529147340884357</v>
       </c>
       <c r="R35" t="n">
         <v>0</v>
       </c>
       <c r="S35" t="n">
-        <v>-0.1527950099504439</v>
+        <v>-0.1400849036995038</v>
       </c>
       <c r="T35" t="n">
         <v>-0.1477218821926766</v>
       </c>
       <c r="U35" t="n">
-        <v>-0.007549594274268416</v>
+        <v>0</v>
       </c>
       <c r="V35" t="n">
-        <v>0</v>
+        <v>-0.1509971292006992</v>
       </c>
       <c r="W35" t="n">
-        <v>-0.1504498329883325</v>
+        <v>0.001361767514258528</v>
       </c>
       <c r="X35" t="n">
-        <v>0.001361767514258528</v>
+        <v>-0.3233523778989975</v>
       </c>
       <c r="Y35" t="n">
-        <v>-0.3233523778989975</v>
+        <v>0.01311903207520703</v>
       </c>
       <c r="Z35" t="n">
-        <v>0.01311903207520703</v>
+        <v>0.9230355856435032</v>
       </c>
       <c r="AA35" t="n">
-        <v>0.9230355856435032</v>
+        <v>-0.4727449176712932</v>
       </c>
       <c r="AB35" t="n">
-        <v>-0.4727449176712932</v>
+        <v>0.05476731098093935</v>
       </c>
       <c r="AC35" t="n">
-        <v>0.05476731098093935</v>
+        <v>0.01467944913957132</v>
       </c>
       <c r="AD35" t="n">
-        <v>-3.126821346811668</v>
+        <v>-3.011613572747994</v>
       </c>
       <c r="AE35" t="n">
         <v>10.68295423017317</v>
@@ -4094,7 +4094,7 @@
         <v>2.725849737383146</v>
       </c>
       <c r="AG35" t="n">
-        <v>4.83028314597836</v>
+        <v>4.945490920042034</v>
       </c>
     </row>
     <row r="36">
@@ -4149,55 +4149,55 @@
         <v>0.007079504077700256</v>
       </c>
       <c r="Q36" t="n">
-        <v>0.06762611201565284</v>
+        <v>0</v>
       </c>
       <c r="R36" t="n">
         <v>0</v>
       </c>
       <c r="S36" t="n">
-        <v>-0.1643831051465275</v>
+        <v>-0.1723740521734858</v>
       </c>
       <c r="T36" t="n">
         <v>-0.2180518585177918</v>
       </c>
       <c r="U36" t="n">
-        <v>-0.005158287683866762</v>
+        <v>0</v>
       </c>
       <c r="V36" t="n">
-        <v>0</v>
+        <v>0.04367777777976124</v>
       </c>
       <c r="W36" t="n">
-        <v>0.04367777777976124</v>
+        <v>-0.09129006175040112</v>
       </c>
       <c r="X36" t="n">
-        <v>-0.09129006175040112</v>
+        <v>-0.4451325544503666</v>
       </c>
       <c r="Y36" t="n">
-        <v>-0.4451325544503666</v>
+        <v>0.0664908501598282</v>
       </c>
       <c r="Z36" t="n">
-        <v>0.0664908501598282</v>
+        <v>0.8590347833095633</v>
       </c>
       <c r="AA36" t="n">
-        <v>0.8590347833095633</v>
+        <v>0.001138496900938303</v>
       </c>
       <c r="AB36" t="n">
-        <v>0.001138496900938303</v>
+        <v>0.1223463028689423</v>
       </c>
       <c r="AC36" t="n">
-        <v>0.1223463028689423</v>
+        <v>0.01563405171280815</v>
       </c>
       <c r="AD36" t="n">
-        <v>-2.66692559497466</v>
+        <v>-2.55764642164621</v>
       </c>
       <c r="AE36" t="n">
-        <v>11.11820274898126</v>
+        <v>11.11824299134706</v>
       </c>
       <c r="AF36" t="n">
         <v>2.584924633664547</v>
       </c>
       <c r="AG36" t="n">
-        <v>5.866352520342057</v>
+        <v>5.975671936036302</v>
       </c>
     </row>
     <row r="37">
@@ -4252,46 +4252,46 @@
         <v>-0.01551710665825198</v>
       </c>
       <c r="Q37" t="n">
-        <v>-0.1677001992745181</v>
+        <v>-0.03978757412620653</v>
       </c>
       <c r="R37" t="n">
         <v>0</v>
       </c>
       <c r="S37" t="n">
-        <v>-0.05385511498868789</v>
+        <v>-0.05693244587111397</v>
       </c>
       <c r="T37" t="n">
         <v>-0.4464945808505398</v>
       </c>
       <c r="U37" t="n">
-        <v>-0.006558414680702424</v>
+        <v>0.1050372767942514</v>
       </c>
       <c r="V37" t="n">
-        <v>0.1050372767942514</v>
+        <v>-0.122914323842251</v>
       </c>
       <c r="W37" t="n">
-        <v>-0.122914323842251</v>
+        <v>0.001571458097759289</v>
       </c>
       <c r="X37" t="n">
-        <v>0.001571458097759289</v>
+        <v>-0.1350348341675899</v>
       </c>
       <c r="Y37" t="n">
-        <v>-0.1350348341675899</v>
+        <v>-0.02954313188640124</v>
       </c>
       <c r="Z37" t="n">
-        <v>-0.02954313188640124</v>
+        <v>1.695854504028458</v>
       </c>
       <c r="AA37" t="n">
-        <v>1.695854504028458</v>
+        <v>-0.04428380612626755</v>
       </c>
       <c r="AB37" t="n">
-        <v>-0.04428380612626755</v>
+        <v>0.09511147720648441</v>
       </c>
       <c r="AC37" t="n">
-        <v>0.09511147720648441</v>
+        <v>-0.05319080767964831</v>
       </c>
       <c r="AD37" t="n">
-        <v>-2.210547051267355</v>
+        <v>-2.049591005763167</v>
       </c>
       <c r="AE37" t="n">
         <v>12.19860116682559</v>
@@ -4300,7 +4300,7 @@
         <v>2.105639746971739</v>
       </c>
       <c r="AG37" t="n">
-        <v>7.882414368586492</v>
+        <v>8.043370414090679</v>
       </c>
     </row>
     <row r="38">
@@ -4355,55 +4355,55 @@
         <v>0.1237817696790089</v>
       </c>
       <c r="Q38" t="n">
-        <v>-0.1246414413689071</v>
+        <v>-0.03254240240211884</v>
       </c>
       <c r="R38" t="n">
         <v>-0.002197681198280891</v>
       </c>
       <c r="S38" t="n">
-        <v>-0.04833045366231216</v>
+        <v>-0.04630897283395414</v>
       </c>
       <c r="T38" t="n">
         <v>-0.2563542449745604</v>
       </c>
       <c r="U38" t="n">
-        <v>-0.01655909644496618</v>
+        <v>0.01302590339440693</v>
       </c>
       <c r="V38" t="n">
-        <v>0.01302590339440693</v>
+        <v>-0.1774607754703996</v>
       </c>
       <c r="W38" t="n">
-        <v>-0.1774607754703996</v>
+        <v>0.03533990633352037</v>
       </c>
       <c r="X38" t="n">
-        <v>0.03533990633352037</v>
+        <v>-0.1855298497960725</v>
       </c>
       <c r="Y38" t="n">
-        <v>-0.1855298497960725</v>
+        <v>-0.01159992651582026</v>
       </c>
       <c r="Z38" t="n">
-        <v>-0.01159992651582026</v>
+        <v>1.768574445934317</v>
       </c>
       <c r="AA38" t="n">
-        <v>1.768574445934317</v>
+        <v>-0.1015559042416925</v>
       </c>
       <c r="AB38" t="n">
-        <v>-0.1015559042416925</v>
+        <v>0.0225485170932838</v>
       </c>
       <c r="AC38" t="n">
-        <v>0.0225485170932838</v>
+        <v>-0.01562435112510588</v>
       </c>
       <c r="AD38" t="n">
-        <v>-1.173515200567452</v>
+        <v>-1.040805086227627</v>
       </c>
       <c r="AE38" t="n">
-        <v>13.2024270099755</v>
+        <v>13.20265445483215</v>
       </c>
       <c r="AF38" t="n">
         <v>2.375564778330544</v>
       </c>
       <c r="AG38" t="n">
-        <v>9.653347031077505</v>
+        <v>9.786284590273983</v>
       </c>
     </row>
     <row r="39">
@@ -4416,7 +4416,7 @@
         <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.08639390862986066</v>
+        <v>-0.08833354794504777</v>
       </c>
       <c r="D39" t="n">
         <v>-0.03525322122783131</v>
@@ -4437,7 +4437,7 @@
         <v>0.08048112718027316</v>
       </c>
       <c r="J39" t="n">
-        <v>-0.1294233976562274</v>
+        <v>-0.1311205820570161</v>
       </c>
       <c r="K39" t="n">
         <v>-0.223025762262975</v>
@@ -4458,46 +4458,46 @@
         <v>-0.02863358399989044</v>
       </c>
       <c r="Q39" t="n">
-        <v>0.02597713450189413</v>
+        <v>-0.05517505542881185</v>
       </c>
       <c r="R39" t="n">
         <v>-0.01174491471623067</v>
       </c>
       <c r="S39" t="n">
-        <v>-0.1584630056595312</v>
+        <v>-0.1654942242745552</v>
       </c>
       <c r="T39" t="n">
         <v>-0.1651963534015348</v>
       </c>
       <c r="U39" t="n">
-        <v>-0.06399687408783243</v>
+        <v>0.001505929182904178</v>
       </c>
       <c r="V39" t="n">
-        <v>0.001505929182904178</v>
+        <v>-0.01817526218317339</v>
       </c>
       <c r="W39" t="n">
-        <v>-0.01694094625532705</v>
+        <v>-0.0009574595358463767</v>
       </c>
       <c r="X39" t="n">
-        <v>-0.0009574595358463767</v>
+        <v>-0.4229578482985926</v>
       </c>
       <c r="Y39" t="n">
-        <v>-0.4229578482985926</v>
+        <v>0.01390609064560883</v>
       </c>
       <c r="Z39" t="n">
-        <v>0.01390609064560883</v>
+        <v>1.589133251762917</v>
       </c>
       <c r="AA39" t="n">
-        <v>1.589133251762917</v>
+        <v>0.01868504957018772</v>
       </c>
       <c r="AB39" t="n">
-        <v>0.01868504957018772</v>
+        <v>0.2476512555869857</v>
       </c>
       <c r="AC39" t="n">
-        <v>0.2476512555869857</v>
+        <v>0.2449634840304473</v>
       </c>
       <c r="AD39" t="n">
-        <v>0.09253389402968186</v>
+        <v>1.734973520336572</v>
       </c>
       <c r="AE39" t="n">
         <v>12.9997840726113</v>
@@ -4506,7 +4506,7 @@
         <v>3.432658560789324</v>
       </c>
       <c r="AG39" t="n">
-        <v>9.659659405851659</v>
+        <v>11.30209903215855</v>
       </c>
     </row>
     <row r="40">
@@ -4561,46 +4561,46 @@
         <v>0.1518222965741862</v>
       </c>
       <c r="Q40" t="n">
-        <v>-0.1729055548172881</v>
+        <v>-0.0227166849472894</v>
       </c>
       <c r="R40" t="n">
         <v>-0.003861999231760256</v>
       </c>
       <c r="S40" t="n">
-        <v>-0.04178531566138307</v>
+        <v>-0.04341838990139772</v>
       </c>
       <c r="T40" t="n">
         <v>-0.3786634273008698</v>
       </c>
       <c r="U40" t="n">
-        <v>-0.009378768394276508</v>
+        <v>0.002583555994465855</v>
       </c>
       <c r="V40" t="n">
-        <v>0.002583555994465855</v>
+        <v>-0.09914676776338119</v>
       </c>
       <c r="W40" t="n">
-        <v>-0.09914676776338119</v>
+        <v>-0.001986724299950002</v>
       </c>
       <c r="X40" t="n">
-        <v>-0.001986724299950002</v>
+        <v>-0.1407111529934249</v>
       </c>
       <c r="Y40" t="n">
-        <v>-0.1407111529934249</v>
+        <v>-0.06477437685621433</v>
       </c>
       <c r="Z40" t="n">
-        <v>-0.06477437685621433</v>
+        <v>1.803609467804682</v>
       </c>
       <c r="AA40" t="n">
-        <v>1.803609467804682</v>
+        <v>-0.1872980485485691</v>
       </c>
       <c r="AB40" t="n">
-        <v>-0.1872980485485691</v>
+        <v>0.1127755515204362</v>
       </c>
       <c r="AC40" t="n">
-        <v>0.1127755515204362</v>
+        <v>0.05746772304475978</v>
       </c>
       <c r="AD40" t="n">
-        <v>-1.355875285012855</v>
+        <v>-0.5229094113036656</v>
       </c>
       <c r="AE40" t="n">
         <v>15.06446348441912</v>
@@ -4609,7 +4609,7 @@
         <v>2.909579690590713</v>
       </c>
       <c r="AG40" t="n">
-        <v>10.79900850881555</v>
+        <v>11.63197438252474</v>
       </c>
     </row>
     <row r="41">
@@ -4622,7 +4622,7 @@
         <v>0.0003404891175879805</v>
       </c>
       <c r="C41" t="n">
-        <v>0.0409834725813167</v>
+        <v>0.04082949521381195</v>
       </c>
       <c r="D41" t="n">
         <v>-0.03099449195681327</v>
@@ -4643,7 +4643,7 @@
         <v>-0.08318916618122033</v>
       </c>
       <c r="J41" t="n">
-        <v>-0.119774448242739</v>
+        <v>-0.1199091784393057</v>
       </c>
       <c r="K41" t="n">
         <v>-0.2265886259334638</v>
@@ -4664,46 +4664,46 @@
         <v>-0.00704502515805786</v>
       </c>
       <c r="Q41" t="n">
-        <v>-0.166154789400565</v>
+        <v>-0.001193346949023353</v>
       </c>
       <c r="R41" t="n">
         <v>-0.005324775587301118</v>
       </c>
       <c r="S41" t="n">
-        <v>-0.04595220659664839</v>
+        <v>-0.0460511849512119</v>
       </c>
       <c r="T41" t="n">
         <v>-0.3425631229056075</v>
       </c>
       <c r="U41" t="n">
-        <v>-0.007468689347896563</v>
+        <v>0</v>
       </c>
       <c r="V41" t="n">
-        <v>0</v>
+        <v>-0.2649236252672512</v>
       </c>
       <c r="W41" t="n">
-        <v>-0.2648256396697481</v>
+        <v>8.523906778738233e-05</v>
       </c>
       <c r="X41" t="n">
-        <v>8.523906778738233e-05</v>
+        <v>-0.1371363814257089</v>
       </c>
       <c r="Y41" t="n">
-        <v>-0.1371363814257089</v>
+        <v>-0.007189637850541959</v>
       </c>
       <c r="Z41" t="n">
-        <v>-0.007189637850541959</v>
+        <v>1.735221743630062</v>
       </c>
       <c r="AA41" t="n">
-        <v>1.735221743630062</v>
+        <v>-0.2253924869779931</v>
       </c>
       <c r="AB41" t="n">
-        <v>-0.2253924869779931</v>
+        <v>0.1247325745368508</v>
       </c>
       <c r="AC41" t="n">
-        <v>0.1247325745368508</v>
+        <v>0.1653755235501174</v>
       </c>
       <c r="AD41" t="n">
-        <v>-2.345699161821965</v>
+        <v>-1.335639786281787</v>
       </c>
       <c r="AE41" t="n">
         <v>13.48522943201806</v>
@@ -4712,7 +4712,7 @@
         <v>2.407429868159737</v>
       </c>
       <c r="AG41" t="n">
-        <v>8.732100402036355</v>
+        <v>9.742159777576534</v>
       </c>
     </row>
     <row r="42">
@@ -4725,7 +4725,7 @@
         <v>0.0004529464822739851</v>
       </c>
       <c r="C42" t="n">
-        <v>0.07871535044107678</v>
+        <v>0.07676588435464038</v>
       </c>
       <c r="D42" t="n">
         <v>-0.003618863707738315</v>
@@ -4746,7 +4746,7 @@
         <v>0.00326871083033616</v>
       </c>
       <c r="J42" t="n">
-        <v>-0.1560229276275519</v>
+        <v>-0.1577287104531838</v>
       </c>
       <c r="K42" t="n">
         <v>-0.1691041968059824</v>
@@ -4767,46 +4767,46 @@
         <v>-0.04429596207223301</v>
       </c>
       <c r="Q42" t="n">
-        <v>0.03165361200564941</v>
+        <v>-0.003170625375917896</v>
       </c>
       <c r="R42" t="n">
         <v>-0.007044500141194452</v>
       </c>
       <c r="S42" t="n">
-        <v>-0.1448350483450927</v>
+        <v>-0.1525259923487809</v>
       </c>
       <c r="T42" t="n">
         <v>-0.01614247716834035</v>
       </c>
       <c r="U42" t="n">
-        <v>-0.0221827884838854</v>
+        <v>0.0156265996293639</v>
       </c>
       <c r="V42" t="n">
-        <v>0.0156265996293639</v>
+        <v>-0.006381908893782792</v>
       </c>
       <c r="W42" t="n">
-        <v>-0.005141339566050552</v>
+        <v>0</v>
       </c>
       <c r="X42" t="n">
-        <v>0</v>
+        <v>-0.343538908190531</v>
       </c>
       <c r="Y42" t="n">
-        <v>-0.343538908190531</v>
+        <v>-0.02659658190229063</v>
       </c>
       <c r="Z42" t="n">
-        <v>-0.02659658190229063</v>
+        <v>1.710105423841004</v>
       </c>
       <c r="AA42" t="n">
-        <v>1.710105423841004</v>
+        <v>-0.05497114366317671</v>
       </c>
       <c r="AB42" t="n">
-        <v>-0.05497114366317671</v>
+        <v>0.2441498820600434</v>
       </c>
       <c r="AC42" t="n">
-        <v>0.2441498820600434</v>
+        <v>-0.01944818619511846</v>
       </c>
       <c r="AD42" t="n">
-        <v>-1.019839633062165</v>
+        <v>-0.5873710461598136</v>
       </c>
       <c r="AE42" t="n">
         <v>12.67359967908071</v>
@@ -4815,7 +4815,7 @@
         <v>3.343456731499479</v>
       </c>
       <c r="AG42" t="n">
-        <v>8.310303314519064</v>
+        <v>8.742771901421417</v>
       </c>
     </row>
     <row r="43">
@@ -4828,7 +4828,7 @@
         <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>0.03298017749682267</v>
+        <v>0.03266250107903376</v>
       </c>
       <c r="D43" t="n">
         <v>-0.02281315505587091</v>
@@ -4849,7 +4849,7 @@
         <v>-0.1155369449270417</v>
       </c>
       <c r="J43" t="n">
-        <v>-0.07697537391731146</v>
+        <v>-0.07725334078287674</v>
       </c>
       <c r="K43" t="n">
         <v>-0.2192966397290622</v>
@@ -4870,46 +4870,46 @@
         <v>0.07764357313268104</v>
       </c>
       <c r="Q43" t="n">
-        <v>-0.1420571457400098</v>
+        <v>0</v>
       </c>
       <c r="R43" t="n">
         <v>-0.004725915385836726</v>
       </c>
       <c r="S43" t="n">
-        <v>-0.08122484245834408</v>
+        <v>-0.08423835827020872</v>
       </c>
       <c r="T43" t="n">
         <v>-0.2485239142528386</v>
       </c>
       <c r="U43" t="n">
-        <v>-0.01861833850147294</v>
+        <v>0</v>
       </c>
       <c r="V43" t="n">
-        <v>0</v>
+        <v>-0.1471602859451619</v>
       </c>
       <c r="W43" t="n">
-        <v>-0.1469581282247508</v>
+        <v>-0.0001683185595709296</v>
       </c>
       <c r="X43" t="n">
-        <v>-0.0001683185595709296</v>
+        <v>-0.220909447590796</v>
       </c>
       <c r="Y43" t="n">
-        <v>-0.220909447590796</v>
+        <v>-0.0706857199386793</v>
       </c>
       <c r="Z43" t="n">
-        <v>-0.0706857199386793</v>
+        <v>1.679915389836719</v>
       </c>
       <c r="AA43" t="n">
-        <v>1.679915389836719</v>
+        <v>-0.1678167311473384</v>
       </c>
       <c r="AB43" t="n">
-        <v>-0.1678167311473384</v>
+        <v>0.1348847002901711</v>
       </c>
       <c r="AC43" t="n">
-        <v>0.1348847002901711</v>
+        <v>-0.005291032417084248</v>
       </c>
       <c r="AD43" t="n">
-        <v>-2.720293408378807</v>
+        <v>-2.255815493726691</v>
       </c>
       <c r="AE43" t="n">
         <v>11.90477475879558</v>
@@ -4918,7 +4918,7 @@
         <v>3.293796111048356</v>
       </c>
       <c r="AG43" t="n">
-        <v>5.890685239368419</v>
+        <v>6.355163154020537</v>
       </c>
     </row>
     <row r="44">
@@ -4931,7 +4931,7 @@
         <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>0.05769158632751586</v>
+        <v>0.05722861821514813</v>
       </c>
       <c r="D44" t="n">
         <v>-0.02613216374762322</v>
@@ -4952,7 +4952,7 @@
         <v>-0.1153193347707847</v>
       </c>
       <c r="J44" t="n">
-        <v>-0.1004560430750489</v>
+        <v>-0.1008611401733707</v>
       </c>
       <c r="K44" t="n">
         <v>-0.2053853469602089</v>
@@ -4973,55 +4973,55 @@
         <v>0.01351954842329187</v>
       </c>
       <c r="Q44" t="n">
-        <v>-0.1654081018438112</v>
+        <v>-0.001673454913916418</v>
       </c>
       <c r="R44" t="n">
         <v>-0.01776460357140172</v>
       </c>
       <c r="S44" t="n">
-        <v>-0.05369299381350064</v>
+        <v>-0.05607431741851939</v>
       </c>
       <c r="T44" t="n">
         <v>-0.3333728162785933</v>
       </c>
       <c r="U44" t="n">
-        <v>-0.008797187731230959</v>
+        <v>0</v>
       </c>
       <c r="V44" t="n">
-        <v>0</v>
+        <v>-0.1683644664513856</v>
       </c>
       <c r="W44" t="n">
-        <v>-0.1680698503798789</v>
+        <v>0.0001195324938511727</v>
       </c>
       <c r="X44" t="n">
-        <v>0.0001195324938511727</v>
+        <v>-0.1742537139585623</v>
       </c>
       <c r="Y44" t="n">
-        <v>-0.1742537139585623</v>
+        <v>-0.05903284929897933</v>
       </c>
       <c r="Z44" t="n">
-        <v>-0.05903284929897933</v>
+        <v>1.7530678016603</v>
       </c>
       <c r="AA44" t="n">
-        <v>1.7530678016603</v>
+        <v>-0.1499860621409728</v>
       </c>
       <c r="AB44" t="n">
-        <v>-0.1499860621409728</v>
+        <v>0.1421947695082295</v>
       </c>
       <c r="AC44" t="n">
-        <v>0.1421947695082295</v>
+        <v>-0.06007901647844682</v>
       </c>
       <c r="AD44" t="n">
-        <v>-3.019131006775191</v>
+        <v>-3.022482729343171</v>
       </c>
       <c r="AE44" t="n">
-        <v>13.79892655811657</v>
+        <v>13.79915854929949</v>
       </c>
       <c r="AF44" t="n">
         <v>2.395329167291155</v>
       </c>
       <c r="AG44" t="n">
-        <v>8.384466384050224</v>
+        <v>8.381346652665162</v>
       </c>
     </row>
     <row r="45">
@@ -5034,7 +5034,7 @@
         <v>0.0001340407314868982</v>
       </c>
       <c r="C45" t="n">
-        <v>0.04731095135059623</v>
+        <v>0.04684912050851105</v>
       </c>
       <c r="D45" t="n">
         <v>-0.03748313569811572</v>
@@ -5055,7 +5055,7 @@
         <v>-0.1048047465614692</v>
       </c>
       <c r="J45" t="n">
-        <v>-0.07886122713872284</v>
+        <v>-0.07926532912554737</v>
       </c>
       <c r="K45" t="n">
         <v>-0.2610971772858854</v>
@@ -5076,46 +5076,46 @@
         <v>-0.001110487327418489</v>
       </c>
       <c r="Q45" t="n">
-        <v>-0.1382094180026973</v>
+        <v>0</v>
       </c>
       <c r="R45" t="n">
         <v>-0.0004691425602041436</v>
       </c>
       <c r="S45" t="n">
-        <v>-0.05420034408899056</v>
+        <v>-0.05364356055177398</v>
       </c>
       <c r="T45" t="n">
         <v>-0.3611973922183474</v>
       </c>
       <c r="U45" t="n">
-        <v>-0.01232436060873714</v>
+        <v>0.0009382851204082873</v>
       </c>
       <c r="V45" t="n">
-        <v>0.0009382851204082873</v>
+        <v>-0.2346359650331817</v>
       </c>
       <c r="W45" t="n">
-        <v>-0.2343420726791275</v>
+        <v>-6.70203657434491e-05</v>
       </c>
       <c r="X45" t="n">
-        <v>-6.70203657434491e-05</v>
+        <v>-0.1735409595785531</v>
       </c>
       <c r="Y45" t="n">
-        <v>-0.1735409595785531</v>
+        <v>-0.0182552859367114</v>
       </c>
       <c r="Z45" t="n">
-        <v>-0.0182552859367114</v>
+        <v>1.574528436022056</v>
       </c>
       <c r="AA45" t="n">
-        <v>1.574528436022056</v>
+        <v>-0.1620143090696582</v>
       </c>
       <c r="AB45" t="n">
-        <v>-0.1620143090696582</v>
+        <v>0.1662318820686763</v>
       </c>
       <c r="AC45" t="n">
-        <v>0.1662318820686763</v>
+        <v>0.01613656651047477</v>
       </c>
       <c r="AD45" t="n">
-        <v>-2.906713763785051</v>
+        <v>-2.675942816488306</v>
       </c>
       <c r="AE45" t="n">
         <v>12.93795781574384</v>
@@ -5124,7 +5124,7 @@
         <v>2.633644577255411</v>
       </c>
       <c r="AG45" t="n">
-        <v>7.397599474703376</v>
+        <v>7.628370422000121</v>
       </c>
     </row>
     <row r="46">
@@ -5179,46 +5179,46 @@
         <v>-0.006164483362739988</v>
       </c>
       <c r="Q46" t="n">
-        <v>-0.1726861726566842</v>
+        <v>-0.002194408599350581</v>
       </c>
       <c r="R46" t="n">
         <v>0</v>
       </c>
       <c r="S46" t="n">
-        <v>-0.03059286216984158</v>
+        <v>-0.03239244229747932</v>
       </c>
       <c r="T46" t="n">
         <v>-0.4617362691711948</v>
       </c>
       <c r="U46" t="n">
-        <v>-0.005804351963598534</v>
+        <v>0.004377784983794698</v>
       </c>
       <c r="V46" t="n">
-        <v>0.004377784983794698</v>
+        <v>-0.05605935243969639</v>
       </c>
       <c r="W46" t="n">
-        <v>-0.05605935243969639</v>
+        <v>-0.0006191719832570797</v>
       </c>
       <c r="X46" t="n">
-        <v>-0.0006191719832570797</v>
+        <v>-0.01706777608156256</v>
       </c>
       <c r="Y46" t="n">
-        <v>-0.01706777608156256</v>
+        <v>-0.09918342189266417</v>
       </c>
       <c r="Z46" t="n">
-        <v>-0.09918342189266417</v>
+        <v>1.72388883596655</v>
       </c>
       <c r="AA46" t="n">
-        <v>1.72388883596655</v>
+        <v>-0.01364078174187934</v>
       </c>
       <c r="AB46" t="n">
-        <v>-0.01364078174187934</v>
+        <v>0.0478015526197952</v>
       </c>
       <c r="AC46" t="n">
-        <v>0.0478015526197952</v>
+        <v>-0.1658286969761122</v>
       </c>
       <c r="AD46" t="n">
-        <v>-2.385548344717861</v>
+        <v>-2.316763206859496</v>
       </c>
       <c r="AE46" t="n">
         <v>14.14625678105321</v>
@@ -5227,7 +5227,7 @@
         <v>1.76104150121723</v>
       </c>
       <c r="AG46" t="n">
-        <v>9.999666935118119</v>
+        <v>10.06845207297649</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the code - HealthyDistance
</commit_message>
<xml_diff>
--- a/input/comp_mrs_cat.xlsx
+++ b/input/comp_mrs_cat.xlsx
@@ -689,13 +689,13 @@
         <v>-1.162357477637666</v>
       </c>
       <c r="AE2" t="n">
-        <v>11.77990626116324</v>
+        <v>11.93731123504216</v>
       </c>
       <c r="AF2" t="n">
         <v>1.21525785660293</v>
       </c>
       <c r="AG2" t="n">
-        <v>9.402290926922644</v>
+        <v>9.559695900801563</v>
       </c>
     </row>
     <row r="3">
@@ -792,13 +792,13 @@
         <v>-2.564258810921626</v>
       </c>
       <c r="AE3" t="n">
-        <v>14.09549045834902</v>
+        <v>14.51851968851755</v>
       </c>
       <c r="AF3" t="n">
         <v>1.907476798064713</v>
       </c>
       <c r="AG3" t="n">
-        <v>9.623754849362683</v>
+        <v>10.04678407953121</v>
       </c>
     </row>
     <row r="4">
@@ -895,13 +895,13 @@
         <v>-0.4619109132700263</v>
       </c>
       <c r="AE4" t="n">
-        <v>12.05507120829597</v>
+        <v>12.25232032141117</v>
       </c>
       <c r="AF4" t="n">
         <v>3.004803121989122</v>
       </c>
       <c r="AG4" t="n">
-        <v>8.588357173036826</v>
+        <v>8.785606286152021</v>
       </c>
     </row>
     <row r="5">
@@ -998,13 +998,13 @@
         <v>-1.19013821421626</v>
       </c>
       <c r="AE5" t="n">
-        <v>15.14418650838776</v>
+        <v>15.37709491931022</v>
       </c>
       <c r="AF5" t="n">
         <v>2.79833508502352</v>
       </c>
       <c r="AG5" t="n">
-        <v>11.15571320914798</v>
+        <v>11.38862162007044</v>
       </c>
     </row>
     <row r="6">
@@ -1101,13 +1101,13 @@
         <v>-1.050455219130762</v>
       </c>
       <c r="AE6" t="n">
-        <v>11.41663563776412</v>
+        <v>11.69034257985</v>
       </c>
       <c r="AF6" t="n">
         <v>1.398649254021426</v>
       </c>
       <c r="AG6" t="n">
-        <v>8.96753116461193</v>
+        <v>9.241238106697811</v>
       </c>
     </row>
     <row r="7">
@@ -1204,13 +1204,13 @@
         <v>-1.489922128018698</v>
       </c>
       <c r="AE7" t="n">
-        <v>11.59625371340653</v>
+        <v>11.80088658660416</v>
       </c>
       <c r="AF7" t="n">
         <v>2.713662913782229</v>
       </c>
       <c r="AG7" t="n">
-        <v>7.392668671605599</v>
+        <v>7.597301544803238</v>
       </c>
     </row>
     <row r="8">
@@ -1307,13 +1307,13 @@
         <v>-2.140233106274022</v>
       </c>
       <c r="AE8" t="n">
-        <v>11.52707889346317</v>
+        <v>11.59930400537542</v>
       </c>
       <c r="AF8" t="n">
         <v>3.149142237757889</v>
       </c>
       <c r="AG8" t="n">
-        <v>6.237703549431259</v>
+        <v>6.309928661343509</v>
       </c>
     </row>
     <row r="9">
@@ -1410,13 +1410,13 @@
         <v>-3.355275426373559</v>
       </c>
       <c r="AE9" t="n">
-        <v>11.96681525992708</v>
+        <v>12.23381602137246</v>
       </c>
       <c r="AF9" t="n">
         <v>3.276139743624471</v>
       </c>
       <c r="AG9" t="n">
-        <v>5.335400089929049</v>
+        <v>5.602400851374426</v>
       </c>
     </row>
     <row r="10">
@@ -1513,13 +1513,13 @@
         <v>0.3161112590376853</v>
       </c>
       <c r="AE10" t="n">
-        <v>9.860527833189106</v>
+        <v>9.980634714575309</v>
       </c>
       <c r="AF10" t="n">
         <v>3.828349514488567</v>
       </c>
       <c r="AG10" t="n">
-        <v>6.348289577738225</v>
+        <v>6.468396459124428</v>
       </c>
     </row>
     <row r="11">
@@ -1616,13 +1616,13 @@
         <v>-2.567119051838167</v>
       </c>
       <c r="AE11" t="n">
-        <v>10.60978211399623</v>
+        <v>10.5941472827577</v>
       </c>
       <c r="AF11" t="n">
         <v>3.84770481406579</v>
       </c>
       <c r="AG11" t="n">
-        <v>4.194958248092273</v>
+        <v>4.17932341685374</v>
       </c>
     </row>
     <row r="12">
@@ -1719,13 +1719,13 @@
         <v>-0.6566552737072212</v>
       </c>
       <c r="AE12" t="n">
-        <v>13.23877518635641</v>
+        <v>13.42280115001057</v>
       </c>
       <c r="AF12" t="n">
         <v>2.289331898834243</v>
       </c>
       <c r="AG12" t="n">
-        <v>10.29278801381494</v>
+        <v>10.4768139774691</v>
       </c>
     </row>
     <row r="13">
@@ -1822,13 +1822,13 @@
         <v>-0.8763367219235041</v>
       </c>
       <c r="AE13" t="n">
-        <v>11.88895917226999</v>
+        <v>12.11516833859528</v>
       </c>
       <c r="AF13" t="n">
         <v>1.034388269386078</v>
       </c>
       <c r="AG13" t="n">
-        <v>9.978234180960408</v>
+        <v>10.2044433472857</v>
       </c>
     </row>
     <row r="14">
@@ -1925,13 +1925,13 @@
         <v>-2.131726055724423</v>
       </c>
       <c r="AE14" t="n">
-        <v>10.16261714606267</v>
+        <v>10.19883691937124</v>
       </c>
       <c r="AF14" t="n">
         <v>3.641193771392695</v>
       </c>
       <c r="AG14" t="n">
-        <v>4.389697318945551</v>
+        <v>4.425917092254123</v>
       </c>
     </row>
     <row r="15">
@@ -2028,13 +2028,13 @@
         <v>-0.1161005024478145</v>
       </c>
       <c r="AE15" t="n">
-        <v>14.79667321669343</v>
+        <v>15.0921182512653</v>
       </c>
       <c r="AF15" t="n">
         <v>1.785537558360071</v>
       </c>
       <c r="AG15" t="n">
-        <v>12.89503515588554</v>
+        <v>13.19048019045741</v>
       </c>
     </row>
     <row r="16">
@@ -2131,13 +2131,13 @@
         <v>-1.600987236505321</v>
       </c>
       <c r="AE16" t="n">
-        <v>11.76908737648015</v>
+        <v>12.01886751273979</v>
       </c>
       <c r="AF16" t="n">
         <v>2.030937895387919</v>
       </c>
       <c r="AG16" t="n">
-        <v>8.137162244586911</v>
+        <v>8.386942380846545</v>
       </c>
     </row>
     <row r="17">
@@ -2234,13 +2234,13 @@
         <v>-2.258120318159745</v>
       </c>
       <c r="AE17" t="n">
-        <v>14.37418480895472</v>
+        <v>14.58010571514267</v>
       </c>
       <c r="AF17" t="n">
         <v>1.848962917049874</v>
       </c>
       <c r="AG17" t="n">
-        <v>10.2671015737451</v>
+        <v>10.47302247993305</v>
       </c>
     </row>
     <row r="18">
@@ -2337,13 +2337,13 @@
         <v>-2.915336689430267</v>
       </c>
       <c r="AE18" t="n">
-        <v>11.25392851252065</v>
+        <v>11.46661957331528</v>
       </c>
       <c r="AF18" t="n">
         <v>2.480869506725185</v>
       </c>
       <c r="AG18" t="n">
-        <v>5.857722316365196</v>
+        <v>6.070413377159827</v>
       </c>
     </row>
     <row r="19">
@@ -2440,13 +2440,13 @@
         <v>-1.41859203731189</v>
       </c>
       <c r="AE19" t="n">
-        <v>9.881465367855055</v>
+        <v>9.882164425305898</v>
       </c>
       <c r="AF19" t="n">
         <v>3.297158965890005</v>
       </c>
       <c r="AG19" t="n">
-        <v>5.16571436465316</v>
+        <v>5.166413422104005</v>
       </c>
     </row>
     <row r="20">
@@ -2543,13 +2543,13 @@
         <v>-0.9469282098765193</v>
       </c>
       <c r="AE20" t="n">
-        <v>11.99734307940836</v>
+        <v>12.52280151862626</v>
       </c>
       <c r="AF20" t="n">
         <v>3.119152271531618</v>
       </c>
       <c r="AG20" t="n">
-        <v>7.931262598000222</v>
+        <v>8.456721037218118</v>
       </c>
     </row>
     <row r="21">
@@ -2646,13 +2646,13 @@
         <v>-3.925782267886767</v>
       </c>
       <c r="AE21" t="n">
-        <v>10.64092224178287</v>
+        <v>10.71328130126241</v>
       </c>
       <c r="AF21" t="n">
         <v>3.253217425700312</v>
       </c>
       <c r="AG21" t="n">
-        <v>3.461922548195792</v>
+        <v>3.534281607675332</v>
       </c>
     </row>
     <row r="22">
@@ -2749,13 +2749,13 @@
         <v>-2.476094526427489</v>
       </c>
       <c r="AE22" t="n">
-        <v>12.4497784749184</v>
+        <v>12.74396681066839</v>
       </c>
       <c r="AF22" t="n">
         <v>2.326473128727222</v>
       </c>
       <c r="AG22" t="n">
-        <v>7.647210819763687</v>
+        <v>7.941399155513683</v>
       </c>
     </row>
     <row r="23">
@@ -2852,13 +2852,13 @@
         <v>-2.034038055125093</v>
       </c>
       <c r="AE23" t="n">
-        <v>13.03096986013981</v>
+        <v>13.21500831137032</v>
       </c>
       <c r="AF23" t="n">
         <v>2.496649824908592</v>
       </c>
       <c r="AG23" t="n">
-        <v>8.500281980106127</v>
+        <v>8.684320431336637</v>
       </c>
     </row>
     <row r="24">
@@ -2955,13 +2955,13 @@
         <v>-3.557335164022657</v>
       </c>
       <c r="AE24" t="n">
-        <v>13.35240945679437</v>
+        <v>13.73356444982923</v>
       </c>
       <c r="AF24" t="n">
         <v>2.367888785783177</v>
       </c>
       <c r="AG24" t="n">
-        <v>7.427185506988537</v>
+        <v>7.808340500023394</v>
       </c>
     </row>
     <row r="25">
@@ -3058,13 +3058,13 @@
         <v>-0.3024935433907597</v>
       </c>
       <c r="AE25" t="n">
-        <v>14.09205416163184</v>
+        <v>14.38470400851906</v>
       </c>
       <c r="AF25" t="n">
         <v>2.756894535999121</v>
       </c>
       <c r="AG25" t="n">
-        <v>11.03266608224196</v>
+        <v>11.32531592912918</v>
       </c>
     </row>
     <row r="26">
@@ -3161,13 +3161,13 @@
         <v>-0.8365829261980727</v>
       </c>
       <c r="AE26" t="n">
-        <v>13.1559824118403</v>
+        <v>13.43459926052832</v>
       </c>
       <c r="AF26" t="n">
         <v>2.468263610591526</v>
       </c>
       <c r="AG26" t="n">
-        <v>9.851135875050703</v>
+        <v>10.12975272373872</v>
       </c>
     </row>
     <row r="27">
@@ -3264,13 +3264,13 @@
         <v>-1.685725131043076</v>
       </c>
       <c r="AE27" t="n">
-        <v>11.40694298563118</v>
+        <v>11.54009724639915</v>
       </c>
       <c r="AF27" t="n">
         <v>2.176770978233852</v>
       </c>
       <c r="AG27" t="n">
-        <v>7.544446876354252</v>
+        <v>7.677601137122219</v>
       </c>
     </row>
     <row r="28">
@@ -3367,13 +3367,13 @@
         <v>-2.260025396428075</v>
       </c>
       <c r="AE28" t="n">
-        <v>14.90906696606726</v>
+        <v>15.37184469244659</v>
       </c>
       <c r="AF28" t="n">
         <v>2.79206825249104</v>
       </c>
       <c r="AG28" t="n">
-        <v>9.856973317148148</v>
+        <v>10.31975104352748</v>
       </c>
     </row>
     <row r="29">
@@ -3470,13 +3470,13 @@
         <v>0.9489823367935053</v>
       </c>
       <c r="AE29" t="n">
-        <v>10.6625181294375</v>
+        <v>11.06433018238832</v>
       </c>
       <c r="AF29" t="n">
         <v>2.96434199520753</v>
       </c>
       <c r="AG29" t="n">
-        <v>8.647158471023477</v>
+        <v>9.048970523974299</v>
       </c>
     </row>
     <row r="30">
@@ -3573,13 +3573,13 @@
         <v>-2.480804844348842</v>
       </c>
       <c r="AE30" t="n">
-        <v>12.26781624115958</v>
+        <v>12.66605846681442</v>
       </c>
       <c r="AF30" t="n">
         <v>3.157693416302038</v>
       </c>
       <c r="AG30" t="n">
-        <v>6.629317980508702</v>
+        <v>7.027560206163539</v>
       </c>
     </row>
     <row r="31">
@@ -3676,13 +3676,13 @@
         <v>-3.929252485985064</v>
       </c>
       <c r="AE31" t="n">
-        <v>12.54327878527785</v>
+        <v>12.91365853710254</v>
       </c>
       <c r="AF31" t="n">
         <v>2.816984400016397</v>
       </c>
       <c r="AG31" t="n">
-        <v>5.797041899276385</v>
+        <v>6.167421651101076</v>
       </c>
     </row>
     <row r="32">
@@ -3779,13 +3779,13 @@
         <v>-1.661383318422347</v>
       </c>
       <c r="AE32" t="n">
-        <v>14.04173456276912</v>
+        <v>14.47207605144228</v>
       </c>
       <c r="AF32" t="n">
         <v>1.700090545577031</v>
       </c>
       <c r="AG32" t="n">
-        <v>10.68026069876974</v>
+        <v>11.1106021874429</v>
       </c>
     </row>
     <row r="33">
@@ -3882,13 +3882,13 @@
         <v>-3.561139889682237</v>
       </c>
       <c r="AE33" t="n">
-        <v>10.61390266985545</v>
+        <v>10.88123827321872</v>
       </c>
       <c r="AF33" t="n">
         <v>3.031725283185861</v>
       </c>
       <c r="AG33" t="n">
-        <v>4.021037496987354</v>
+        <v>4.288373100350624</v>
       </c>
     </row>
     <row r="34">
@@ -3985,13 +3985,13 @@
         <v>-0.7128195526356281</v>
       </c>
       <c r="AE34" t="n">
-        <v>13.34067530921292</v>
+        <v>13.76433087242771</v>
       </c>
       <c r="AF34" t="n">
         <v>2.57710761741724</v>
       </c>
       <c r="AG34" t="n">
-        <v>10.05074813916005</v>
+        <v>10.47440370237484</v>
       </c>
     </row>
     <row r="35">
@@ -4088,13 +4088,13 @@
         <v>-4.517807365965699</v>
       </c>
       <c r="AE35" t="n">
-        <v>10.68295423017317</v>
+        <v>11.44494132331521</v>
       </c>
       <c r="AF35" t="n">
         <v>2.725849737383146</v>
       </c>
       <c r="AG35" t="n">
-        <v>3.439297126824329</v>
+        <v>4.201284219966366</v>
       </c>
     </row>
     <row r="36">
@@ -4191,13 +4191,13 @@
         <v>-2.998958752638037</v>
       </c>
       <c r="AE36" t="n">
-        <v>11.11824299134706</v>
+        <v>11.43590039691728</v>
       </c>
       <c r="AF36" t="n">
         <v>2.584924633664547</v>
       </c>
       <c r="AG36" t="n">
-        <v>5.534359605044475</v>
+        <v>5.852017010614691</v>
       </c>
     </row>
     <row r="37">
@@ -4294,13 +4294,13 @@
         <v>-2.265199734619479</v>
       </c>
       <c r="AE37" t="n">
-        <v>12.19860116682559</v>
+        <v>12.58340269662471</v>
       </c>
       <c r="AF37" t="n">
         <v>2.105639746971739</v>
       </c>
       <c r="AG37" t="n">
-        <v>7.827761685234368</v>
+        <v>8.212563215033487</v>
       </c>
     </row>
     <row r="38">
@@ -4397,13 +4397,13 @@
         <v>-1.316366547806062</v>
       </c>
       <c r="AE38" t="n">
-        <v>13.20265445483215</v>
+        <v>13.58696023262923</v>
       </c>
       <c r="AF38" t="n">
         <v>2.375564778330544</v>
       </c>
       <c r="AG38" t="n">
-        <v>9.510723128695547</v>
+        <v>9.89502890649262</v>
       </c>
     </row>
     <row r="39">
@@ -4500,13 +4500,13 @@
         <v>1.890858344191473</v>
       </c>
       <c r="AE39" t="n">
-        <v>12.9997840726113</v>
+        <v>13.61467158714544</v>
       </c>
       <c r="AF39" t="n">
         <v>3.432658560789324</v>
       </c>
       <c r="AG39" t="n">
-        <v>11.45798385601345</v>
+        <v>12.07287137054759</v>
       </c>
     </row>
     <row r="40">
@@ -4603,13 +4603,13 @@
         <v>-0.8022396189408132</v>
       </c>
       <c r="AE40" t="n">
-        <v>15.06446348441912</v>
+        <v>15.49813795156405</v>
       </c>
       <c r="AF40" t="n">
         <v>2.909579690590713</v>
       </c>
       <c r="AG40" t="n">
-        <v>11.35264417488759</v>
+        <v>11.78631864203252</v>
       </c>
     </row>
     <row r="41">
@@ -4706,13 +4706,13 @@
         <v>-1.592518608634948</v>
       </c>
       <c r="AE41" t="n">
-        <v>13.48522943201806</v>
+        <v>13.7896516881348</v>
       </c>
       <c r="AF41" t="n">
         <v>2.407429868159737</v>
       </c>
       <c r="AG41" t="n">
-        <v>9.485280955223372</v>
+        <v>9.789703211340111</v>
       </c>
     </row>
     <row r="42">
@@ -4809,13 +4809,13 @@
         <v>-0.7241190181262075</v>
       </c>
       <c r="AE42" t="n">
-        <v>12.67359967908071</v>
+        <v>12.95483354674426</v>
       </c>
       <c r="AF42" t="n">
         <v>3.343456731499479</v>
       </c>
       <c r="AG42" t="n">
-        <v>8.606023929455022</v>
+        <v>8.88725779711857</v>
       </c>
     </row>
     <row r="43">
@@ -4912,13 +4912,13 @@
         <v>-2.724743836260621</v>
       </c>
       <c r="AE43" t="n">
-        <v>11.90477475879558</v>
+        <v>12.0595945518373</v>
       </c>
       <c r="AF43" t="n">
         <v>3.293796111048356</v>
       </c>
       <c r="AG43" t="n">
-        <v>5.886234811486605</v>
+        <v>6.041054604528326</v>
       </c>
     </row>
     <row r="44">
@@ -5015,13 +5015,13 @@
         <v>-3.304339929430232</v>
       </c>
       <c r="AE44" t="n">
-        <v>13.79915854929949</v>
+        <v>14.02098915234082</v>
       </c>
       <c r="AF44" t="n">
         <v>2.395329167291155</v>
       </c>
       <c r="AG44" t="n">
-        <v>8.0994894525781</v>
+        <v>8.321320055619427</v>
       </c>
     </row>
     <row r="45">
@@ -5118,13 +5118,13 @@
         <v>-2.811052041239895</v>
       </c>
       <c r="AE45" t="n">
-        <v>12.93795781574384</v>
+        <v>13.36936733974361</v>
       </c>
       <c r="AF45" t="n">
         <v>2.633644577255411</v>
       </c>
       <c r="AG45" t="n">
-        <v>7.493261197248532</v>
+        <v>7.924670721248304</v>
       </c>
     </row>
     <row r="46">
@@ -5221,13 +5221,13 @@
         <v>-2.358294644854253</v>
       </c>
       <c r="AE46" t="n">
-        <v>14.14625678105321</v>
+        <v>14.66525189983984</v>
       </c>
       <c r="AF46" t="n">
         <v>1.76104150121723</v>
       </c>
       <c r="AG46" t="n">
-        <v>10.02692063498173</v>
+        <v>10.54591575376836</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the code - Subtract Abundance
</commit_message>
<xml_diff>
--- a/input/comp_mrs_cat.xlsx
+++ b/input/comp_mrs_cat.xlsx
@@ -611,13 +611,13 @@
         <v>0.04786427216330914</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.0691357704801407</v>
+        <v>-0.06915146600327188</v>
       </c>
       <c r="F2" t="n">
         <v>-0.0177070788043226</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2451957425560409</v>
+        <v>0.2452361024726639</v>
       </c>
       <c r="H2" t="n">
         <v>-0.06478319286059628</v>
@@ -635,7 +635,7 @@
         <v>0.08668433451400606</v>
       </c>
       <c r="M2" t="n">
-        <v>0.2498520949191223</v>
+        <v>0.2498738271819193</v>
       </c>
       <c r="N2" t="n">
         <v>0.1546109508261594</v>
@@ -662,13 +662,13 @@
         <v>-0.01071064103520192</v>
       </c>
       <c r="V2" t="n">
-        <v>-0.03412040778646576</v>
+        <v>-0.03412896898090094</v>
       </c>
       <c r="W2" t="n">
-        <v>-0.0153790390743014</v>
+        <v>-0.01536020444654401</v>
       </c>
       <c r="X2" t="n">
-        <v>0.3567659378057634</v>
+        <v>0.3568365676598537</v>
       </c>
       <c r="Y2" t="n">
         <v>0.01283280162287454</v>
@@ -714,13 +714,13 @@
         <v>0.005388613119527071</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.01759838729598341</v>
+        <v>-0.01761141973292286</v>
       </c>
       <c r="F3" t="n">
         <v>-0.01748691686885945</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0831701089862841</v>
+        <v>0.08320362096698553</v>
       </c>
       <c r="H3" t="n">
         <v>-0.09290174365479457</v>
@@ -738,7 +738,7 @@
         <v>0.07436087431959684</v>
       </c>
       <c r="M3" t="n">
-        <v>0.1960082981281036</v>
+        <v>0.1960263430407889</v>
       </c>
       <c r="N3" t="n">
         <v>0.08901284744670426</v>
@@ -765,13 +765,13 @@
         <v>-0.007189188363337521</v>
       </c>
       <c r="V3" t="n">
-        <v>-0.008809211343072528</v>
+        <v>-0.008816319945039496</v>
       </c>
       <c r="W3" t="n">
-        <v>-0.03048919950032463</v>
+        <v>-0.0304735605759973</v>
       </c>
       <c r="X3" t="n">
-        <v>0.1365876979522292</v>
+        <v>0.1366463439184566</v>
       </c>
       <c r="Y3" t="n">
         <v>0.08101329952176532</v>
@@ -817,13 +817,13 @@
         <v>0.01278288753772612</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.1203196332280734</v>
+        <v>-0.1203243515595868</v>
       </c>
       <c r="F4" t="n">
         <v>-0.5441656144978185</v>
       </c>
       <c r="G4" t="n">
-        <v>0.262702541130244</v>
+        <v>0.2627146739827071</v>
       </c>
       <c r="H4" t="n">
         <v>-0.08545836189003257</v>
@@ -841,7 +841,7 @@
         <v>0.04220881389032572</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2508465965677043</v>
+        <v>0.2508531296421075</v>
       </c>
       <c r="N4" t="n">
         <v>0.1746579379889124</v>
@@ -868,13 +868,13 @@
         <v>-0.04886310065124592</v>
       </c>
       <c r="V4" t="n">
-        <v>-0.02378884303223451</v>
+        <v>-0.02379141666760547</v>
       </c>
       <c r="W4" t="n">
-        <v>0.06030260476986081</v>
+        <v>0.06030826676767691</v>
       </c>
       <c r="X4" t="n">
-        <v>0.4172677145939124</v>
+        <v>0.4172889470857228</v>
       </c>
       <c r="Y4" t="n">
         <v>0.02438047727485258</v>
@@ -901,7 +901,7 @@
         <v>3.84770481406579</v>
       </c>
       <c r="AG4" t="n">
-        <v>-5.482663297224214</v>
+        <v>-5.482663297224213</v>
       </c>
     </row>
     <row r="5">
@@ -920,13 +920,13 @@
         <v>0.09627607272011163</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.1136057552035623</v>
+        <v>-0.1136161662394637</v>
       </c>
       <c r="F5" t="n">
         <v>-0.04835957912187718</v>
       </c>
       <c r="G5" t="n">
-        <v>0.274922222121789</v>
+        <v>0.2749489933569641</v>
       </c>
       <c r="H5" t="n">
         <v>-0.06392586158854568</v>
@@ -944,7 +944,7 @@
         <v>0.05247600693637849</v>
       </c>
       <c r="M5" t="n">
-        <v>0.2774728835522772</v>
+        <v>0.2774872988327561</v>
       </c>
       <c r="N5" t="n">
         <v>0.3126220818369637</v>
@@ -971,13 +971,13 @@
         <v>-0.01284754708782828</v>
       </c>
       <c r="V5" t="n">
-        <v>-0.03382579625329873</v>
+        <v>-0.03383147500015405</v>
       </c>
       <c r="W5" t="n">
-        <v>-0.01925289416733546</v>
+        <v>-0.01924040092425374</v>
       </c>
       <c r="X5" t="n">
-        <v>0.3982292566945077</v>
+        <v>0.3982761063560641</v>
       </c>
       <c r="Y5" t="n">
         <v>-0.02536771841533217</v>
@@ -1126,13 +1126,13 @@
         <v>0.05502040578418128</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.1160955295776552</v>
+        <v>-0.1161099478111528</v>
       </c>
       <c r="F7" t="n">
         <v>-0.03179034198756253</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1781347331156849</v>
+        <v>0.1781718085732502</v>
       </c>
       <c r="H7" t="n">
         <v>-0.05288777946452097</v>
@@ -1150,7 +1150,7 @@
         <v>0.1362988697307019</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1536782271330579</v>
+        <v>0.1536981908409776</v>
       </c>
       <c r="N7" t="n">
         <v>0.2335370949992155</v>
@@ -1177,13 +1177,13 @@
         <v>-0.01434886773793887</v>
       </c>
       <c r="V7" t="n">
-        <v>-0.0279616767764074</v>
+        <v>-0.02796954126740608</v>
       </c>
       <c r="W7" t="n">
-        <v>0.02888061686909736</v>
+        <v>0.02889791874929446</v>
       </c>
       <c r="X7" t="n">
-        <v>0.2987487398567908</v>
+        <v>0.2988136219075299</v>
       </c>
       <c r="Y7" t="n">
         <v>0.05405667217505929</v>
@@ -1229,13 +1229,13 @@
         <v>0.02724208106097042</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.04145058064219156</v>
+        <v>-0.04147808135323742</v>
       </c>
       <c r="F8" t="n">
         <v>-0.0007792273987389368</v>
       </c>
       <c r="G8" t="n">
-        <v>0.05090524860827616</v>
+        <v>0.05097596472239408</v>
       </c>
       <c r="H8" t="n">
         <v>-0.1101812279159363</v>
@@ -1253,7 +1253,7 @@
         <v>0.1124401353019988</v>
       </c>
       <c r="M8" t="n">
-        <v>0.206647594603232</v>
+        <v>0.2066856725108339</v>
       </c>
       <c r="N8" t="n">
         <v>0.1895889336310535</v>
@@ -1280,13 +1280,13 @@
         <v>-0.005425457597809015</v>
       </c>
       <c r="V8" t="n">
-        <v>-0.01603157013714994</v>
+        <v>-0.01604657052499314</v>
       </c>
       <c r="W8" t="n">
-        <v>-0.04331939236360915</v>
+        <v>-0.04328639151035411</v>
       </c>
       <c r="X8" t="n">
-        <v>0.05462414305886012</v>
+        <v>0.05474789625856648</v>
       </c>
       <c r="Y8" t="n">
         <v>0.05542093062651843</v>
@@ -1931,7 +1931,7 @@
         <v>3.297158965890005</v>
       </c>
       <c r="AG14" t="n">
-        <v>-6.051455152389472</v>
+        <v>-6.051455152389473</v>
       </c>
     </row>
     <row r="15">
@@ -1950,13 +1950,13 @@
         <v>0.04231232821757515</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.01009197909567424</v>
+        <v>-0.01010005610189488</v>
       </c>
       <c r="F15" t="n">
         <v>-0.00408036450651417</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1272813294972666</v>
+        <v>0.127302098941834</v>
       </c>
       <c r="H15" t="n">
         <v>-0.1121020264815606</v>
@@ -1974,7 +1974,7 @@
         <v>0.07263336467053373</v>
       </c>
       <c r="M15" t="n">
-        <v>0.2432089240902902</v>
+        <v>0.243220107637365</v>
       </c>
       <c r="N15" t="n">
         <v>0.1618000115602442</v>
@@ -2001,13 +2001,13 @@
         <v>-0.007317276576014255</v>
       </c>
       <c r="V15" t="n">
-        <v>-0.02048666093650901</v>
+        <v>-0.02049106657626572</v>
       </c>
       <c r="W15" t="n">
-        <v>-0.06061376330111708</v>
+        <v>-0.06060407089365231</v>
       </c>
       <c r="X15" t="n">
-        <v>0.2012413867633076</v>
+        <v>0.2012777332913005</v>
       </c>
       <c r="Y15" t="n">
         <v>0.003648950867323071</v>
@@ -2150,19 +2150,19 @@
         <v>0.0002086536761009553</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.02473301039138521</v>
+        <v>-0.02047805632364246</v>
       </c>
       <c r="D17" t="n">
-        <v>0.01395092525180149</v>
+        <v>0.01551853990833829</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.0542876860074101</v>
+        <v>-0.05596632225691329</v>
       </c>
       <c r="F17" t="n">
         <v>-0.006534251777863015</v>
       </c>
       <c r="G17" t="n">
-        <v>0.1915782009591904</v>
+        <v>0.1916397401044558</v>
       </c>
       <c r="H17" t="n">
         <v>-0.09882329251645561</v>
@@ -2174,16 +2174,16 @@
         <v>0.07223263122079399</v>
       </c>
       <c r="K17" t="n">
-        <v>0.2019067391014378</v>
+        <v>0.2043887956409544</v>
       </c>
       <c r="L17" t="n">
         <v>0.09574051498808948</v>
       </c>
       <c r="M17" t="n">
-        <v>0.2376897132601159</v>
+        <v>0.2400139788363511</v>
       </c>
       <c r="N17" t="n">
-        <v>0.1673171054099228</v>
+        <v>0.1715720594776655</v>
       </c>
       <c r="O17" t="n">
         <v>0.01078814364947524</v>
@@ -2201,19 +2201,19 @@
         <v>0.08828525028758026</v>
       </c>
       <c r="T17" t="n">
-        <v>0.3749471067347218</v>
+        <v>0.379911219813755</v>
       </c>
       <c r="U17" t="n">
         <v>-0.02487681866274705</v>
       </c>
       <c r="V17" t="n">
-        <v>-0.0252736666046096</v>
+        <v>-0.02528672036269618</v>
       </c>
       <c r="W17" t="n">
-        <v>-0.01039091056203051</v>
+        <v>-0.01036219229424002</v>
       </c>
       <c r="X17" t="n">
-        <v>0.2587036733432321</v>
+        <v>0.2588113668474464</v>
       </c>
       <c r="Y17" t="n">
         <v>0.01896172557542928</v>
@@ -2259,13 +2259,13 @@
         <v>0.001865240657484578</v>
       </c>
       <c r="E18" t="n">
-        <v>0.01295899666119223</v>
+        <v>0.01294894250073136</v>
       </c>
       <c r="F18" t="n">
         <v>-0.001352416762511467</v>
       </c>
       <c r="G18" t="n">
-        <v>0.09120397822031737</v>
+        <v>0.09122983177578818</v>
       </c>
       <c r="H18" t="n">
         <v>-0.1153939857112073</v>
@@ -2283,7 +2283,7 @@
         <v>0.1382053456090095</v>
       </c>
       <c r="M18" t="n">
-        <v>0.1794868265958185</v>
+        <v>0.1795007477410721</v>
       </c>
       <c r="N18" t="n">
         <v>0.1739658628388188</v>
@@ -2310,13 +2310,13 @@
         <v>-0.004715147321515603</v>
       </c>
       <c r="V18" t="n">
-        <v>-0.02825130294470561</v>
+        <v>-0.02825678703222972</v>
       </c>
       <c r="W18" t="n">
-        <v>-0.02989444598896712</v>
+        <v>-0.02988238099641407</v>
       </c>
       <c r="X18" t="n">
-        <v>0.1525601048949838</v>
+        <v>0.1526053486170577</v>
       </c>
       <c r="Y18" t="n">
         <v>0.0279917735258155</v>
@@ -2465,13 +2465,13 @@
         <v>0.05127256239563234</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.1181896635926588</v>
+        <v>-0.1182016946041659</v>
       </c>
       <c r="F20" t="n">
         <v>-0</v>
       </c>
       <c r="G20" t="n">
-        <v>0.155950237906072</v>
+        <v>0.1559811747928045</v>
       </c>
       <c r="H20" t="n">
         <v>-0.01159712607057287</v>
@@ -2489,7 +2489,7 @@
         <v>0.3676502037677124</v>
       </c>
       <c r="M20" t="n">
-        <v>0.1626004115277309</v>
+        <v>0.1626170698513561</v>
       </c>
       <c r="N20" t="n">
         <v>0.3652012624826623</v>
@@ -2516,13 +2516,13 @@
         <v>-0.005181130545938043</v>
       </c>
       <c r="V20" t="n">
-        <v>-0.02120503193786133</v>
+        <v>-0.02121159430777428</v>
       </c>
       <c r="W20" t="n">
-        <v>0.003784139616682314</v>
+        <v>0.003798576830490822</v>
       </c>
       <c r="X20" t="n">
-        <v>0.2426018787760083</v>
+        <v>0.2426560183277902</v>
       </c>
       <c r="Y20" t="n">
         <v>0.06394209112704055</v>
@@ -2774,13 +2774,13 @@
         <v>0.01031326905790914</v>
       </c>
       <c r="E23" t="n">
-        <v>-0.06868350017420979</v>
+        <v>-0.06869258106451698</v>
       </c>
       <c r="F23" t="n">
         <v>-0.006774815148715739</v>
       </c>
       <c r="G23" t="n">
-        <v>0.1467153444867631</v>
+        <v>0.146738695347553</v>
       </c>
       <c r="H23" t="n">
         <v>-0.1048226635448603</v>
@@ -2798,7 +2798,7 @@
         <v>0.2362303892503788</v>
       </c>
       <c r="M23" t="n">
-        <v>0.2220361024237795</v>
+        <v>0.2220486759642048</v>
       </c>
       <c r="N23" t="n">
         <v>0.2230709686436158</v>
@@ -2825,13 +2825,13 @@
         <v>-0.004528265703097334</v>
       </c>
       <c r="V23" t="n">
-        <v>-0.02959958902244815</v>
+        <v>-0.02960454223534299</v>
       </c>
       <c r="W23" t="n">
-        <v>0.01386129239362595</v>
+        <v>0.01387218946199456</v>
       </c>
       <c r="X23" t="n">
-        <v>0.2009072169070735</v>
+        <v>0.2009480809134558</v>
       </c>
       <c r="Y23" t="n">
         <v>0.1179805042303452</v>
@@ -2980,13 +2980,13 @@
         <v>0.07004488916426878</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.1112623876538693</v>
+        <v>-0.1112708680732126</v>
       </c>
       <c r="F25" t="n">
         <v>-0.249417259345411</v>
       </c>
       <c r="G25" t="n">
-        <v>0.2690901046517643</v>
+        <v>0.2691119114443614</v>
       </c>
       <c r="H25" t="n">
         <v>-0.0516695160113288</v>
@@ -3004,7 +3004,7 @@
         <v>0.006913960666865749</v>
       </c>
       <c r="M25" t="n">
-        <v>0.1411572903892908</v>
+        <v>0.1411690325083815</v>
       </c>
       <c r="N25" t="n">
         <v>0.1814795857666027</v>
@@ -3031,13 +3031,13 @@
         <v>-0.005137693971413827</v>
       </c>
       <c r="V25" t="n">
-        <v>-0.06885721971749208</v>
+        <v>-0.06886184540077024</v>
       </c>
       <c r="W25" t="n">
-        <v>0.07704941445593662</v>
+        <v>0.07705959095914858</v>
       </c>
       <c r="X25" t="n">
-        <v>0.3747007667098363</v>
+        <v>0.3747389285968811</v>
       </c>
       <c r="Y25" t="n">
         <v>-0.01756870559646433</v>
@@ -3283,13 +3283,13 @@
         <v>-0</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.0097001115323988</v>
+        <v>-0.009142685142860476</v>
       </c>
       <c r="D28" t="n">
-        <v>0.05165670186935776</v>
+        <v>0.05186206948655609</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.01174124281579688</v>
+        <v>-0.01195801974506178</v>
       </c>
       <c r="F28" t="n">
         <v>-0.002131301729975717</v>
@@ -3307,16 +3307,16 @@
         <v>0.1342390011525176</v>
       </c>
       <c r="K28" t="n">
-        <v>0.230630033806269</v>
+        <v>0.2309551992001664</v>
       </c>
       <c r="L28" t="n">
         <v>0.05753034718752632</v>
       </c>
       <c r="M28" t="n">
-        <v>0.2466503761517987</v>
+        <v>0.2469505288230885</v>
       </c>
       <c r="N28" t="n">
-        <v>0.11806426345717</v>
+        <v>0.1186216898467083</v>
       </c>
       <c r="O28" t="n">
         <v>0.03764022814627359</v>
@@ -3334,7 +3334,7 @@
         <v>0.06640234148976595</v>
       </c>
       <c r="T28" t="n">
-        <v>0.3384584338635786</v>
+        <v>0.3391087646513734</v>
       </c>
       <c r="U28" t="n">
         <v>-0.002131301729975717</v>
@@ -3386,19 +3386,19 @@
         <v>0.002253291514122555</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.04285163562572453</v>
+        <v>-0.03928305103429752</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0872251535730359</v>
+        <v>0.08853989526461427</v>
       </c>
       <c r="E29" t="n">
-        <v>-0.0005459094108950786</v>
+        <v>-0.004256320690603644</v>
       </c>
       <c r="F29" t="n">
         <v>-0.1748204269952363</v>
       </c>
       <c r="G29" t="n">
-        <v>0.1027656793382975</v>
+        <v>0.1087381523232639</v>
       </c>
       <c r="H29" t="n">
         <v>-0.1091711013930607</v>
@@ -3410,16 +3410,16 @@
         <v>0.2852344705249856</v>
       </c>
       <c r="K29" t="n">
-        <v>0.1298848495456771</v>
+        <v>0.1319665238906762</v>
       </c>
       <c r="L29" t="n">
         <v>-0.0003329837021480609</v>
       </c>
       <c r="M29" t="n">
-        <v>0.1578809714455749</v>
+        <v>0.1630184639867099</v>
       </c>
       <c r="N29" t="n">
-        <v>0.2295037736829385</v>
+        <v>0.2330723582743655</v>
       </c>
       <c r="O29" t="n">
         <v>0.05386387913357002</v>
@@ -3437,19 +3437,19 @@
         <v>0.08338576834920983</v>
       </c>
       <c r="T29" t="n">
-        <v>0.2128790573889443</v>
+        <v>0.2170424060789425</v>
       </c>
       <c r="U29" t="n">
         <v>-0.08440497192430108</v>
       </c>
       <c r="V29" t="n">
-        <v>-0.0216174322162775</v>
+        <v>-0.02288432042520977</v>
       </c>
       <c r="W29" t="n">
-        <v>-0.03444398641112591</v>
+        <v>-0.03165683235147491</v>
       </c>
       <c r="X29" t="n">
-        <v>0.1798399388420205</v>
+        <v>0.1902917665657118</v>
       </c>
       <c r="Y29" t="n">
         <v>0.007850848349414281</v>
@@ -3489,19 +3489,19 @@
         <v>0.006078481491720643</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.1287088779740412</v>
+        <v>-0.1267181590273987</v>
       </c>
       <c r="D30" t="n">
-        <v>0.074196007674543</v>
+        <v>0.07492943044435864</v>
       </c>
       <c r="E30" t="n">
-        <v>0.06680171364876236</v>
+        <v>0.06461312778889555</v>
       </c>
       <c r="F30" t="n">
         <v>-0.1344754880639383</v>
       </c>
       <c r="G30" t="n">
-        <v>0.06120228598085292</v>
+        <v>0.06483935924529653</v>
       </c>
       <c r="H30" t="n">
         <v>-0.1291198780258286</v>
@@ -3513,16 +3513,16 @@
         <v>0.1576434970302112</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.05496559507026133</v>
+        <v>-0.05380434235138657</v>
       </c>
       <c r="L30" t="n">
         <v>0.01158447056211998</v>
       </c>
       <c r="M30" t="n">
-        <v>0.09231953354477204</v>
+        <v>0.09534988319689527</v>
       </c>
       <c r="N30" t="n">
-        <v>0.1057950946979625</v>
+        <v>0.1077858136446049</v>
       </c>
       <c r="O30" t="n">
         <v>0.04804690822809381</v>
@@ -3540,19 +3540,19 @@
         <v>0.009292517710935141</v>
       </c>
       <c r="T30" t="n">
-        <v>0.3200951234388031</v>
+        <v>0.3224176288765526</v>
       </c>
       <c r="U30" t="n">
         <v>-0.03992512136018329</v>
       </c>
       <c r="V30" t="n">
-        <v>-0.01495141822317106</v>
+        <v>-0.0157229186125985</v>
       </c>
       <c r="W30" t="n">
-        <v>-0.03171310737039766</v>
+        <v>-0.03001580651365731</v>
       </c>
       <c r="X30" t="n">
-        <v>0.1047178458138739</v>
+        <v>0.1110827240266502</v>
       </c>
       <c r="Y30" t="n">
         <v>0.007300185077791756</v>
@@ -3592,19 +3592,19 @@
         <v>0.002380483389314005</v>
       </c>
       <c r="C31" t="n">
-        <v>0.01587759386664762</v>
+        <v>0.02244531534483283</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0701104337776073</v>
+        <v>0.07253012063799132</v>
       </c>
       <c r="E31" t="n">
-        <v>-0.01428012639132874</v>
+        <v>-0.01728244844634158</v>
       </c>
       <c r="F31" t="n">
         <v>-0.1238031692983954</v>
       </c>
       <c r="G31" t="n">
-        <v>0.06099090082750042</v>
+        <v>0.06214343606220535</v>
       </c>
       <c r="H31" t="n">
         <v>-0.1033372125065265</v>
@@ -3616,16 +3616,16 @@
         <v>0.2165667295894009</v>
       </c>
       <c r="K31" t="n">
-        <v>0.1671709553610742</v>
+        <v>0.1710021262233489</v>
       </c>
       <c r="L31" t="n">
         <v>0.1102858053234974</v>
       </c>
       <c r="M31" t="n">
-        <v>0.1860160195493085</v>
+        <v>0.1901730808562494</v>
       </c>
       <c r="N31" t="n">
-        <v>0.1972608355295093</v>
+        <v>0.2038285570076945</v>
       </c>
       <c r="O31" t="n">
         <v>0.04086424986191433</v>
@@ -3643,19 +3643,19 @@
         <v>0.05330310442416811</v>
       </c>
       <c r="T31" t="n">
-        <v>0.4075018347744928</v>
+        <v>0.4151641764990422</v>
       </c>
       <c r="U31" t="n">
         <v>-0.01177660231534626</v>
       </c>
       <c r="V31" t="n">
-        <v>-0.002917044520754873</v>
+        <v>-0.003161521691752886</v>
       </c>
       <c r="W31" t="n">
-        <v>-0.02589723285983568</v>
+        <v>-0.02535938308364006</v>
       </c>
       <c r="X31" t="n">
-        <v>0.1054625095195338</v>
+        <v>0.1074794461802674</v>
       </c>
       <c r="Y31" t="n">
         <v>0.006648163645472684</v>
@@ -3695,19 +3695,19 @@
         <v>0.01086921305210565</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.08978275869871159</v>
+        <v>-0.08389401347717132</v>
       </c>
       <c r="D32" t="n">
-        <v>0.09927176938800328</v>
+        <v>0.1014413071012023</v>
       </c>
       <c r="E32" t="n">
-        <v>0.03552244162243907</v>
+        <v>0.03191352464528123</v>
       </c>
       <c r="F32" t="n">
         <v>-0.2498790370442326</v>
       </c>
       <c r="G32" t="n">
-        <v>0.1031365730995384</v>
+        <v>0.1065279001049754</v>
       </c>
       <c r="H32" t="n">
         <v>-0.1294351458808304</v>
@@ -3719,16 +3719,16 @@
         <v>0.2110718861745414</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.00774581955393893</v>
+        <v>-0.004310718174707104</v>
       </c>
       <c r="L32" t="n">
         <v>0.01162870118029167</v>
       </c>
       <c r="M32" t="n">
-        <v>0.1339762900339816</v>
+        <v>0.1389732520023541</v>
       </c>
       <c r="N32" t="n">
-        <v>0.1383825767283993</v>
+        <v>0.1442713219499396</v>
       </c>
       <c r="O32" t="n">
         <v>0.06124041759588909</v>
@@ -3746,19 +3746,19 @@
         <v>0.04885958681484082</v>
       </c>
       <c r="T32" t="n">
-        <v>0.3321376026552221</v>
+        <v>0.3390078054136858</v>
       </c>
       <c r="U32" t="n">
         <v>-0.02903310428216221</v>
       </c>
       <c r="V32" t="n">
-        <v>-0.02470815619454044</v>
+        <v>-0.02542752858963314</v>
       </c>
       <c r="W32" t="n">
-        <v>-0.03157282464197977</v>
+        <v>-0.02999020537277581</v>
       </c>
       <c r="X32" t="n">
-        <v>0.1780152701176099</v>
+        <v>0.1839500923771247</v>
       </c>
       <c r="Y32" t="n">
         <v>0.01518559832283175</v>
@@ -3798,13 +3798,13 @@
         <v>-0.0004529464822739851</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.07676588435464038</v>
+        <v>-0.07258090347007892</v>
       </c>
       <c r="D33" t="n">
-        <v>0.003618863707738315</v>
+        <v>0.005160698770471492</v>
       </c>
       <c r="E33" t="n">
-        <v>-0.1295107647996273</v>
+        <v>-0.1311382573658456</v>
       </c>
       <c r="F33" t="n">
         <v>-0.060777388752385</v>
@@ -3822,16 +3822,16 @@
         <v>0.1577287104531838</v>
       </c>
       <c r="K33" t="n">
-        <v>0.1691041968059824</v>
+        <v>0.1715454356553099</v>
       </c>
       <c r="L33" t="n">
         <v>0.03036258259274987</v>
       </c>
       <c r="M33" t="n">
-        <v>0.1247962289594196</v>
+        <v>0.1270496802049527</v>
       </c>
       <c r="N33" t="n">
-        <v>0.2404162002655612</v>
+        <v>0.2446011811501226</v>
       </c>
       <c r="O33" t="n">
         <v>0.01936595784708519</v>
@@ -3849,7 +3849,7 @@
         <v>0.1525259923487809</v>
       </c>
       <c r="T33" t="n">
-        <v>0.01614247716834035</v>
+        <v>0.02102495486699539</v>
       </c>
       <c r="U33" t="n">
         <v>-0.0156265996293639</v>
@@ -3901,19 +3901,19 @@
         <v>-0.0002473671346151503</v>
       </c>
       <c r="C34" t="n">
-        <v>0.182070881727525</v>
+        <v>0.1823849989124708</v>
       </c>
       <c r="D34" t="n">
-        <v>0.04832834350666946</v>
+        <v>0.04844407089059686</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.2101914941352176</v>
+        <v>-0.2103239210177529</v>
       </c>
       <c r="F34" t="n">
         <v>-0.04291840263460987</v>
       </c>
       <c r="G34" t="n">
-        <v>0.3439264107040222</v>
+        <v>0.3439528197884528</v>
       </c>
       <c r="H34" t="n">
         <v>-0.006969570718892651</v>
@@ -3925,16 +3925,16 @@
         <v>0.01195400729728161</v>
       </c>
       <c r="K34" t="n">
-        <v>0.2048562018678183</v>
+        <v>0.20503943689237</v>
       </c>
       <c r="L34" t="n">
         <v>0.1924051739171407</v>
       </c>
       <c r="M34" t="n">
-        <v>0.237603182223709</v>
+        <v>0.2377865425226039</v>
       </c>
       <c r="N34" t="n">
-        <v>0.3044171845964673</v>
+        <v>0.3047313017814131</v>
       </c>
       <c r="O34" t="n">
         <v>0.0006628313538093232</v>
@@ -3952,19 +3952,19 @@
         <v>0.1723740521734858</v>
       </c>
       <c r="T34" t="n">
-        <v>0.2180518585177918</v>
+        <v>0.2184183285668952</v>
       </c>
       <c r="U34" t="n">
         <v>-0</v>
       </c>
       <c r="V34" t="n">
-        <v>-0.0439909099032513</v>
+        <v>-0.04399651183025172</v>
       </c>
       <c r="W34" t="n">
-        <v>0.07648857428050793</v>
+        <v>0.07650089851990881</v>
       </c>
       <c r="X34" t="n">
-        <v>0.4451325544503666</v>
+        <v>0.44517877034812</v>
       </c>
       <c r="Y34" t="n">
         <v>-0.0664908501598282</v>
@@ -3991,7 +3991,7 @@
         <v>2.584924633664547</v>
       </c>
       <c r="AG34" t="n">
-        <v>-7.766735742086705</v>
+        <v>-7.766735742086704</v>
       </c>
     </row>
     <row r="35">
@@ -4004,13 +4004,13 @@
         <v>-0.0001340407314868982</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.04684912050851105</v>
+        <v>-0.04098065932523993</v>
       </c>
       <c r="D35" t="n">
-        <v>0.03748313569811572</v>
+        <v>0.03964520034458403</v>
       </c>
       <c r="E35" t="n">
-        <v>-0.05072910562969241</v>
+        <v>-0.05301128497874229</v>
       </c>
       <c r="F35" t="n">
         <v>-0.0009382851204082873</v>
@@ -4028,16 +4028,16 @@
         <v>0.07926532912554737</v>
       </c>
       <c r="K35" t="n">
-        <v>0.2610971772858854</v>
+        <v>0.2645204463094602</v>
       </c>
       <c r="L35" t="n">
         <v>0.126509612967338</v>
       </c>
       <c r="M35" t="n">
-        <v>0.1952269372664152</v>
+        <v>0.1983868779035612</v>
       </c>
       <c r="N35" t="n">
-        <v>0.1637766384004119</v>
+        <v>0.169645099583683</v>
       </c>
       <c r="O35" t="n">
         <v>0.05187353923638021</v>
@@ -4055,7 +4055,7 @@
         <v>0.05364356055177398</v>
       </c>
       <c r="T35" t="n">
-        <v>0.3611973922183474</v>
+        <v>0.3680439302654971</v>
       </c>
       <c r="U35" t="n">
         <v>-0.0009382851204082873</v>
@@ -4107,13 +4107,13 @@
         <v>-0</v>
       </c>
       <c r="C36" t="n">
-        <v>0.008060234978557722</v>
+        <v>0.01140563123140829</v>
       </c>
       <c r="D36" t="n">
-        <v>0.03697082726705431</v>
+        <v>0.03820334167599925</v>
       </c>
       <c r="E36" t="n">
-        <v>-0.02549339408610742</v>
+        <v>-0.02679438151777152</v>
       </c>
       <c r="F36" t="n">
         <v>-0</v>
@@ -4131,16 +4131,16 @@
         <v>0.1099796932107996</v>
       </c>
       <c r="K36" t="n">
-        <v>0.19671380112632</v>
+        <v>0.1986652822738162</v>
       </c>
       <c r="L36" t="n">
         <v>0.1112404031450112</v>
       </c>
       <c r="M36" t="n">
-        <v>0.2136534677181354</v>
+        <v>0.2154548349312088</v>
       </c>
       <c r="N36" t="n">
-        <v>0.2061633193930752</v>
+        <v>0.2095087156459258</v>
       </c>
       <c r="O36" t="n">
         <v>0.02602913443599769</v>
@@ -4158,7 +4158,7 @@
         <v>0.04341838990139772</v>
       </c>
       <c r="T36" t="n">
-        <v>0.3786634273008698</v>
+        <v>0.3825663895958621</v>
       </c>
       <c r="U36" t="n">
         <v>-0.002583555994465855</v>
@@ -4210,19 +4210,19 @@
         <v>-0.002922553218555146</v>
       </c>
       <c r="C37" t="n">
-        <v>0.035338369499292</v>
+        <v>0.03770044838746033</v>
       </c>
       <c r="D37" t="n">
-        <v>0.01175661892491891</v>
+        <v>0.01262685851529671</v>
       </c>
       <c r="E37" t="n">
-        <v>-0.05699782721878225</v>
+        <v>-0.05806758857933206</v>
       </c>
       <c r="F37" t="n">
         <v>-0.0130038002531055</v>
       </c>
       <c r="G37" t="n">
-        <v>0.1939977261606941</v>
+        <v>0.1943864621996538</v>
       </c>
       <c r="H37" t="n">
         <v>-0.1010482927587011</v>
@@ -4234,16 +4234,16 @@
         <v>0.07553197223932939</v>
       </c>
       <c r="K37" t="n">
-        <v>0.1673732560508098</v>
+        <v>0.1687511354022413</v>
       </c>
       <c r="L37" t="n">
         <v>0.1990549055573617</v>
       </c>
       <c r="M37" t="n">
-        <v>0.193799356652173</v>
+        <v>0.1952805646898574</v>
       </c>
       <c r="N37" t="n">
-        <v>0.1900220228555958</v>
+        <v>0.1923841017437641</v>
       </c>
       <c r="O37" t="n">
         <v>0.08664140217252934</v>
@@ -4261,19 +4261,19 @@
         <v>0.01370605956870724</v>
       </c>
       <c r="T37" t="n">
-        <v>0.3841205598028452</v>
+        <v>0.3868763185057082</v>
       </c>
       <c r="U37" t="n">
         <v>-0.04134125182631532</v>
       </c>
       <c r="V37" t="n">
-        <v>-0.01545754967199268</v>
+        <v>-0.01554000883177202</v>
       </c>
       <c r="W37" t="n">
-        <v>-0.03346916878071032</v>
+        <v>-0.03328775862919579</v>
       </c>
       <c r="X37" t="n">
-        <v>0.09052390515242217</v>
+        <v>0.09120419322060166</v>
       </c>
       <c r="Y37" t="n">
         <v>-0.00189893265201366</v>
@@ -4313,13 +4313,13 @@
         <v>-0</v>
       </c>
       <c r="C38" t="n">
-        <v>0.08833354794504777</v>
+        <v>0.08920621027250765</v>
       </c>
       <c r="D38" t="n">
-        <v>0.03525322122783131</v>
+        <v>0.035574728401106</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.1563110937913584</v>
+        <v>-0.1566504624742595</v>
       </c>
       <c r="F38" t="n">
         <v>-0</v>
@@ -4337,16 +4337,16 @@
         <v>0.1311205820570161</v>
       </c>
       <c r="K38" t="n">
-        <v>0.223025762262975</v>
+        <v>0.2235348152873266</v>
       </c>
       <c r="L38" t="n">
         <v>0.03835872345503332</v>
       </c>
       <c r="M38" t="n">
-        <v>0.2058387130667262</v>
+        <v>0.2063086081661277</v>
       </c>
       <c r="N38" t="n">
-        <v>0.3591844567739272</v>
+        <v>0.3600571191013871</v>
       </c>
       <c r="O38" t="n">
         <v>0.01430621900241</v>
@@ -4364,7 +4364,7 @@
         <v>0.1654942242745552</v>
       </c>
       <c r="T38" t="n">
-        <v>0.1651963534015348</v>
+        <v>0.166214459450238</v>
       </c>
       <c r="U38" t="n">
         <v>-0.001505929182904178</v>
@@ -4416,13 +4416,13 @@
         <v>-0.0001944650189244947</v>
       </c>
       <c r="C39" t="n">
-        <v>0.1299975132814174</v>
+        <v>0.1302617529910674</v>
       </c>
       <c r="D39" t="n">
-        <v>0.04915925799983758</v>
+        <v>0.0492566094718139</v>
       </c>
       <c r="E39" t="n">
-        <v>-0.1338206187776782</v>
+        <v>-0.1339233786647644</v>
       </c>
       <c r="F39" t="n">
         <v>-0</v>
@@ -4440,16 +4440,16 @@
         <v>0.002031830377935811</v>
       </c>
       <c r="K39" t="n">
-        <v>0.1634967925648373</v>
+        <v>0.1636509323954665</v>
       </c>
       <c r="L39" t="n">
         <v>0.1881723781555248</v>
       </c>
       <c r="M39" t="n">
-        <v>0.2492220519846535</v>
+        <v>0.2493643349052342</v>
       </c>
       <c r="N39" t="n">
-        <v>0.2081348006439534</v>
+        <v>0.2083990403536034</v>
       </c>
       <c r="O39" t="n">
         <v>0.03141195552189376</v>
@@ -4467,7 +4467,7 @@
         <v>0.04791339341699625</v>
       </c>
       <c r="T39" t="n">
-        <v>0.5254254339507041</v>
+        <v>0.5257337136119624</v>
       </c>
       <c r="U39" t="n">
         <v>-0</v>
@@ -4519,13 +4519,13 @@
         <v>-0</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.009733000167742577</v>
+        <v>-0.00497040178923982</v>
       </c>
       <c r="D40" t="n">
-        <v>0.08867205360729043</v>
+        <v>0.09042669511515988</v>
       </c>
       <c r="E40" t="n">
-        <v>-0.09977444638368366</v>
+        <v>-0.1016265679753236</v>
       </c>
       <c r="F40" t="n">
         <v>-0</v>
@@ -4543,16 +4543,16 @@
         <v>0.3103885616042248</v>
       </c>
       <c r="K40" t="n">
-        <v>0.2537062429655836</v>
+        <v>0.2564844253530434</v>
       </c>
       <c r="L40" t="n">
         <v>0.01203580161086853</v>
       </c>
       <c r="M40" t="n">
-        <v>0.2197658992841344</v>
+        <v>0.2223303753340974</v>
       </c>
       <c r="N40" t="n">
-        <v>0.2524067886651168</v>
+        <v>0.2571693870436195</v>
       </c>
       <c r="O40" t="n">
         <v>0.005245642658480248</v>
@@ -4570,7 +4570,7 @@
         <v>0.1451430127430058</v>
       </c>
       <c r="T40" t="n">
-        <v>0.07010990066164101</v>
+        <v>0.07566626543656089</v>
       </c>
       <c r="U40" t="n">
         <v>-0.004630048990826603</v>
@@ -4725,13 +4725,13 @@
         <v>-0.0003404891175879805</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.04082949521381195</v>
+        <v>-0.03706279316121912</v>
       </c>
       <c r="D42" t="n">
-        <v>0.03099449195681327</v>
+        <v>0.03238222429197905</v>
       </c>
       <c r="E42" t="n">
-        <v>0.01003243532016922</v>
+        <v>0.008567606744160889</v>
       </c>
       <c r="F42" t="n">
         <v>-0.01985398317717842</v>
@@ -4749,16 +4749,16 @@
         <v>0.1199091784393057</v>
       </c>
       <c r="K42" t="n">
-        <v>0.2265886259334638</v>
+        <v>0.2287858687974764</v>
       </c>
       <c r="L42" t="n">
         <v>0.05640104741773895</v>
       </c>
       <c r="M42" t="n">
-        <v>0.2257535882608454</v>
+        <v>0.2277818124430108</v>
       </c>
       <c r="N42" t="n">
-        <v>0.1297356934431868</v>
+        <v>0.1335023954957796</v>
       </c>
       <c r="O42" t="n">
         <v>0.04842558572662127</v>
@@ -4776,7 +4776,7 @@
         <v>0.0460511849512119</v>
       </c>
       <c r="T42" t="n">
-        <v>0.3425631229056075</v>
+        <v>0.3469576086336324</v>
       </c>
       <c r="U42" t="n">
         <v>-0</v>
@@ -4828,19 +4828,19 @@
         <v>-0.0002978358599740457</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.03142292375291122</v>
+        <v>-0.02287631873624403</v>
       </c>
       <c r="D43" t="n">
-        <v>0.05108461766930342</v>
+        <v>0.05423336688597028</v>
       </c>
       <c r="E43" t="n">
-        <v>-0.02074586251194761</v>
+        <v>-0.02408193360417671</v>
       </c>
       <c r="F43" t="n">
         <v>-0.005193481026755056</v>
       </c>
       <c r="G43" t="n">
-        <v>0.1580483457122288</v>
+        <v>0.1580802092184365</v>
       </c>
       <c r="H43" t="n">
         <v>-0.09542626207052035</v>
@@ -4852,16 +4852,16 @@
         <v>0.1527688808704114</v>
       </c>
       <c r="K43" t="n">
-        <v>0.2808136140543632</v>
+        <v>0.285799133647419</v>
       </c>
       <c r="L43" t="n">
         <v>0.1105601370907376</v>
       </c>
       <c r="M43" t="n">
-        <v>0.2525322735443741</v>
+        <v>0.2571514489028451</v>
       </c>
       <c r="N43" t="n">
-        <v>0.1623747402529843</v>
+        <v>0.1709213452696515</v>
       </c>
       <c r="O43" t="n">
         <v>0.06058721215682812</v>
@@ -4879,19 +4879,19 @@
         <v>0.07260184777581674</v>
       </c>
       <c r="T43" t="n">
-        <v>0.3619090372874325</v>
+        <v>0.3718800764735442</v>
       </c>
       <c r="U43" t="n">
         <v>-0.004159741412002104</v>
       </c>
       <c r="V43" t="n">
-        <v>-0.02706109099988337</v>
+        <v>-0.02706784992544257</v>
       </c>
       <c r="W43" t="n">
-        <v>-0.03734878351595795</v>
+        <v>-0.03733391387972772</v>
       </c>
       <c r="X43" t="n">
-        <v>0.2320076514361891</v>
+        <v>0.2320634125720525</v>
       </c>
       <c r="Y43" t="n">
         <v>-0.01222321468117648</v>
@@ -4931,13 +4931,13 @@
         <v>-0.001092625957297383</v>
       </c>
       <c r="C44" t="n">
-        <v>0.08665662072224718</v>
+        <v>0.08839479004908821</v>
       </c>
       <c r="D44" t="n">
-        <v>0.05710048094654326</v>
+        <v>0.05774085911958997</v>
       </c>
       <c r="E44" t="n">
-        <v>-0.02858766064458364</v>
+        <v>-0.02926361538279961</v>
       </c>
       <c r="F44" t="n">
         <v>-0.01067041380949188</v>
@@ -4955,16 +4955,16 @@
         <v>0.02153178893622207</v>
       </c>
       <c r="K44" t="n">
-        <v>0.1639294661608408</v>
+        <v>0.1649433982681648</v>
       </c>
       <c r="L44" t="n">
         <v>0.1469726820671141</v>
       </c>
       <c r="M44" t="n">
-        <v>0.2354099154748533</v>
+        <v>0.2363458528046907</v>
       </c>
       <c r="N44" t="n">
-        <v>0.2069645665824434</v>
+        <v>0.2087027359092844</v>
       </c>
       <c r="O44" t="n">
         <v>0.03729919329721947</v>
@@ -4982,7 +4982,7 @@
         <v>0.05693244587111397</v>
       </c>
       <c r="T44" t="n">
-        <v>0.4464945808505398</v>
+        <v>0.4485224450651876</v>
       </c>
       <c r="U44" t="n">
         <v>-0.1050372767942514</v>
@@ -5034,13 +5034,13 @@
         <v>-0</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.03266250107903376</v>
+        <v>-0.02188711115079714</v>
       </c>
       <c r="D45" t="n">
-        <v>0.02281315505587091</v>
+        <v>0.02678303555574755</v>
       </c>
       <c r="E45" t="n">
-        <v>-0.04278482131366071</v>
+        <v>-0.04697525073019717</v>
       </c>
       <c r="F45" t="n">
         <v>-0</v>
@@ -5058,16 +5058,16 @@
         <v>0.07725334078287674</v>
       </c>
       <c r="K45" t="n">
-        <v>0.2192966397290622</v>
+        <v>0.2255822838538669</v>
       </c>
       <c r="L45" t="n">
         <v>0.0643412900129712</v>
       </c>
       <c r="M45" t="n">
-        <v>0.2166769827223421</v>
+        <v>0.2224791157606233</v>
       </c>
       <c r="N45" t="n">
-        <v>0.1831594905976466</v>
+        <v>0.1939348805258832</v>
       </c>
       <c r="O45" t="n">
         <v>0.06480989698588382</v>
@@ -5085,7 +5085,7 @@
         <v>0.08423835827020872</v>
       </c>
       <c r="T45" t="n">
-        <v>0.2485239142528386</v>
+        <v>0.2610952025024481</v>
       </c>
       <c r="U45" t="n">
         <v>-0</v>
@@ -5137,19 +5137,19 @@
         <v>-0</v>
       </c>
       <c r="C46" t="n">
-        <v>-0.05722861821514813</v>
+        <v>-0.05122033994000155</v>
       </c>
       <c r="D46" t="n">
-        <v>0.02613216374762322</v>
+        <v>0.02834573995425617</v>
       </c>
       <c r="E46" t="n">
-        <v>-0.02109824893948189</v>
+        <v>-0.02346089889963027</v>
       </c>
       <c r="F46" t="n">
         <v>-0.001673454913916418</v>
       </c>
       <c r="G46" t="n">
-        <v>0.1240050571538722</v>
+        <v>0.1240721644905357</v>
       </c>
       <c r="H46" t="n">
         <v>-0.08661654582371947</v>
@@ -5161,16 +5161,16 @@
         <v>0.1008611401733707</v>
       </c>
       <c r="K46" t="n">
-        <v>0.2053853469602089</v>
+        <v>0.2088901759540444</v>
       </c>
       <c r="L46" t="n">
         <v>0.1336573376125102</v>
       </c>
       <c r="M46" t="n">
-        <v>0.2154410633036038</v>
+        <v>0.2187124247868862</v>
       </c>
       <c r="N46" t="n">
-        <v>0.1359474262453806</v>
+        <v>0.1419557045205272</v>
       </c>
       <c r="O46" t="n">
         <v>0.04977981773556808</v>
@@ -5188,19 +5188,19 @@
         <v>0.05607431741851939</v>
       </c>
       <c r="T46" t="n">
-        <v>0.3333728162785933</v>
+        <v>0.3403824742662643</v>
       </c>
       <c r="U46" t="n">
         <v>-0</v>
       </c>
       <c r="V46" t="n">
-        <v>-0.01372972855818582</v>
+        <v>-0.01374396344778112</v>
       </c>
       <c r="W46" t="n">
-        <v>-0.03807679499722744</v>
+        <v>-0.03804547824011779</v>
       </c>
       <c r="X46" t="n">
-        <v>0.1742537139585623</v>
+        <v>0.1743711517977235</v>
       </c>
       <c r="Y46" t="n">
         <v>0.05903284929897933</v>
@@ -5227,7 +5227,7 @@
         <v>2.395329167291155</v>
       </c>
       <c r="AG46" t="n">
-        <v>-9.671766722910995</v>
+        <v>-9.671766722910993</v>
       </c>
     </row>
     <row r="47">
@@ -5240,13 +5240,13 @@
         <v>-0</v>
       </c>
       <c r="C47" t="n">
-        <v>-0.03650585821857492</v>
+        <v>-0.03316331637101113</v>
       </c>
       <c r="D47" t="n">
-        <v>0.01751750232085277</v>
+        <v>0.01874896510679732</v>
       </c>
       <c r="E47" t="n">
-        <v>0.04570640439053901</v>
+        <v>0.04440652700537531</v>
       </c>
       <c r="F47" t="n">
         <v>-0.001910753585553961</v>
@@ -5264,16 +5264,16 @@
         <v>0.04512352229821234</v>
       </c>
       <c r="K47" t="n">
-        <v>0.1795350075130328</v>
+        <v>0.1814848235907782</v>
       </c>
       <c r="L47" t="n">
         <v>0.09690532827928623</v>
       </c>
       <c r="M47" t="n">
-        <v>0.1556759001912255</v>
+        <v>0.1574757304168367</v>
       </c>
       <c r="N47" t="n">
-        <v>0.1451337387474342</v>
+        <v>0.1484762805949979</v>
       </c>
       <c r="O47" t="n">
         <v>0.02356925832628494</v>
@@ -5291,7 +5291,7 @@
         <v>0.02668346104972013</v>
       </c>
       <c r="T47" t="n">
-        <v>0.3496628497965747</v>
+        <v>0.3535624819520657</v>
       </c>
       <c r="U47" t="n">
         <v>-0.001910753585553961</v>
@@ -5343,19 +5343,19 @@
         <v>-0</v>
       </c>
       <c r="C48" t="n">
-        <v>-0.1094326993937916</v>
+        <v>-0.06801046826135022</v>
       </c>
       <c r="D48" t="n">
-        <v>0.004344310034311324</v>
+        <v>0.01960513203047395</v>
       </c>
       <c r="E48" t="n">
-        <v>0.03387483330572818</v>
+        <v>0.01774699475068922</v>
       </c>
       <c r="F48" t="n">
         <v>-0.03117708177088227</v>
       </c>
       <c r="G48" t="n">
-        <v>0.1167808822790361</v>
+        <v>0.1168302360024091</v>
       </c>
       <c r="H48" t="n">
         <v>-0.09452932580947326</v>
@@ -5367,16 +5367,16 @@
         <v>0.07672744519499201</v>
       </c>
       <c r="K48" t="n">
-        <v>0.09221662790423284</v>
+        <v>0.1163795960648236</v>
       </c>
       <c r="L48" t="n">
         <v>0.02411405133442358</v>
       </c>
       <c r="M48" t="n">
-        <v>0.1516726230572087</v>
+        <v>0.1740034764411088</v>
       </c>
       <c r="N48" t="n">
-        <v>0.06187830393124399</v>
+        <v>0.1033005350636854</v>
       </c>
       <c r="O48" t="n">
         <v>0.03244730094620608</v>
@@ -5394,19 +5394,19 @@
         <v>0.04630897283395414</v>
       </c>
       <c r="T48" t="n">
-        <v>0.2563542449745604</v>
+        <v>0.3046801812957421</v>
       </c>
       <c r="U48" t="n">
         <v>-0.01302590339440693</v>
       </c>
       <c r="V48" t="n">
-        <v>-0.01681743715936198</v>
+        <v>-0.01682790613098656</v>
       </c>
       <c r="W48" t="n">
-        <v>-0.05511990689121224</v>
+        <v>-0.05509687515363815</v>
       </c>
       <c r="X48" t="n">
-        <v>0.1855298497960725</v>
+        <v>0.1856162188119753</v>
       </c>
       <c r="Y48" t="n">
         <v>0.01159992651582026</v>
@@ -5446,13 +5446,13 @@
         <v>-0.0002525940662116038</v>
       </c>
       <c r="C49" t="n">
-        <v>0.07194533081424266</v>
+        <v>0.0745664782403644</v>
       </c>
       <c r="D49" t="n">
-        <v>0.1029340095784494</v>
+        <v>0.1038996954722837</v>
       </c>
       <c r="E49" t="n">
-        <v>-0.1264450439973394</v>
+        <v>-0.1274643791074978</v>
       </c>
       <c r="F49" t="n">
         <v>-0</v>
@@ -5470,16 +5470,16 @@
         <v>0.2466322811665514</v>
       </c>
       <c r="K49" t="n">
-        <v>0.2142025198016358</v>
+        <v>0.2157315224668735</v>
       </c>
       <c r="L49" t="n">
         <v>0.1856200703571834</v>
       </c>
       <c r="M49" t="n">
-        <v>0.2294619643584633</v>
+        <v>0.2308733514340673</v>
       </c>
       <c r="N49" t="n">
-        <v>0.1643368792280026</v>
+        <v>0.1669580266541243</v>
       </c>
       <c r="O49" t="n">
         <v>0.009207675323295824</v>
@@ -5497,7 +5497,7 @@
         <v>0.1400849036995038</v>
       </c>
       <c r="T49" t="n">
-        <v>0.1477218821926766</v>
+        <v>0.1507798875231519</v>
       </c>
       <c r="U49" t="n">
         <v>-0</v>
@@ -5549,13 +5549,13 @@
         <v>-0.0004404538507627297</v>
       </c>
       <c r="C50" t="n">
-        <v>-0.1342485123916262</v>
+        <v>-0.1242707470443902</v>
       </c>
       <c r="D50" t="n">
-        <v>0.01445895034125077</v>
+        <v>0.01813496915339037</v>
       </c>
       <c r="E50" t="n">
-        <v>-0.08261354314515539</v>
+        <v>-0.08649378522463608</v>
       </c>
       <c r="F50" t="n">
         <v>-0.003083176955339108</v>
@@ -5573,16 +5573,16 @@
         <v>0.09767035013386045</v>
       </c>
       <c r="K50" t="n">
-        <v>0.1738941422812645</v>
+        <v>0.1797145054004856</v>
       </c>
       <c r="L50" t="n">
         <v>0.07778974077444505</v>
       </c>
       <c r="M50" t="n">
-        <v>0.1232266452952299</v>
+        <v>0.1285992881745108</v>
       </c>
       <c r="N50" t="n">
-        <v>0.238735827675628</v>
+        <v>0.2487135930228641</v>
       </c>
       <c r="O50" t="n">
         <v>0.04340671543523881</v>
@@ -5600,7 +5600,7 @@
         <v>0.1049841757279839</v>
       </c>
       <c r="T50" t="n">
-        <v>-0.002904742451408175</v>
+        <v>0.00873598378703389</v>
       </c>
       <c r="U50" t="n">
         <v>-0</v>
@@ -6373,13 +6373,13 @@
         <v>-0</v>
       </c>
       <c r="C58" t="n">
-        <v>0.1157368289622778</v>
+        <v>0.1164200997523462</v>
       </c>
       <c r="D58" t="n">
-        <v>0.03870641711147778</v>
+        <v>0.03895814845518717</v>
       </c>
       <c r="E58" t="n">
-        <v>-0.1560253155450369</v>
+        <v>-0.1562910319633968</v>
       </c>
       <c r="F58" t="n">
         <v>-0.5240189985562295</v>
@@ -6397,16 +6397,16 @@
         <v>0.07579441795708874</v>
       </c>
       <c r="K58" t="n">
-        <v>0.2709877466968532</v>
+        <v>0.2713863213243931</v>
       </c>
       <c r="L58" t="n">
         <v>0.2114885854786779</v>
       </c>
       <c r="M58" t="n">
-        <v>0.1688011267499412</v>
+        <v>0.1691690417907473</v>
       </c>
       <c r="N58" t="n">
-        <v>0.3164402787568517</v>
+        <v>0.3171235495469201</v>
       </c>
       <c r="O58" t="n">
         <v>0.02389585499335138</v>
@@ -6424,7 +6424,7 @@
         <v>0.1242860112542382</v>
       </c>
       <c r="T58" t="n">
-        <v>0.3858590288422067</v>
+        <v>0.3866561780972865</v>
       </c>
       <c r="U58" t="n">
         <v>-0.01009422287066674</v>
@@ -6579,13 +6579,13 @@
         <v>-0</v>
       </c>
       <c r="C60" t="n">
-        <v>-0.006120750108632969</v>
+        <v>-0.0008520986667326294</v>
       </c>
       <c r="D60" t="n">
-        <v>0.01198925762753875</v>
+        <v>0.01393033973771256</v>
       </c>
       <c r="E60" t="n">
-        <v>0.01972292547380142</v>
+        <v>0.01767400546861796</v>
       </c>
       <c r="F60" t="n">
         <v>-0.002315131458813684</v>
@@ -6603,16 +6603,16 @@
         <v>0.04869891395700206</v>
       </c>
       <c r="K60" t="n">
-        <v>0.09666354581038424</v>
+        <v>0.09973692581815945</v>
       </c>
       <c r="L60" t="n">
         <v>0.04575635720242476</v>
       </c>
       <c r="M60" t="n">
-        <v>0.1720250103374916</v>
+        <v>0.1748619764985149</v>
       </c>
       <c r="N60" t="n">
-        <v>0.09242246835815204</v>
+        <v>0.09769111980005239</v>
       </c>
       <c r="O60" t="n">
         <v>0.006034145144390417</v>
@@ -6630,7 +6630,7 @@
         <v>0.01531104388036279</v>
       </c>
       <c r="T60" t="n">
-        <v>0.3443724995301301</v>
+        <v>0.3505192595456805</v>
       </c>
       <c r="U60" t="n">
         <v>-0.01595258504324894</v>

</xml_diff>

<commit_message>
Update the code - EvaluatePercentileRank EBID type
</commit_message>
<xml_diff>
--- a/input/comp_mrs_cat.xlsx
+++ b/input/comp_mrs_cat.xlsx
@@ -662,7 +662,7 @@
         <v>-0.01071064103520192</v>
       </c>
       <c r="V2" t="n">
-        <v>-0.03412896898090094</v>
+        <v>-0.03627265887951114</v>
       </c>
       <c r="W2" t="n">
         <v>-0.01536020444654401</v>
@@ -765,7 +765,7 @@
         <v>-0.007189188363337521</v>
       </c>
       <c r="V3" t="n">
-        <v>-0.008816319945039496</v>
+        <v>-0.009385114780203334</v>
       </c>
       <c r="W3" t="n">
         <v>-0.0304735605759973</v>
@@ -868,7 +868,7 @@
         <v>-0.04886310065124592</v>
       </c>
       <c r="V4" t="n">
-        <v>-0.02379141666760547</v>
+        <v>-0.02400558613234823</v>
       </c>
       <c r="W4" t="n">
         <v>0.06030826676767691</v>
@@ -901,7 +901,7 @@
         <v>3.84770481406579</v>
       </c>
       <c r="AG4" t="n">
-        <v>-5.482663297224213</v>
+        <v>-5.482663297224214</v>
       </c>
     </row>
     <row r="5">
@@ -971,7 +971,7 @@
         <v>-0.01284754708782828</v>
       </c>
       <c r="V5" t="n">
-        <v>-0.03383147500015405</v>
+        <v>-0.0360141508066156</v>
       </c>
       <c r="W5" t="n">
         <v>-0.01924040092425374</v>
@@ -1074,7 +1074,7 @@
         <v>-0.003074228748897981</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.02378803527661036</v>
+        <v>-0.02532274722994006</v>
       </c>
       <c r="W6" t="n">
         <v>-0.02210813823482373</v>
@@ -1177,7 +1177,7 @@
         <v>-0.01434886773793887</v>
       </c>
       <c r="V7" t="n">
-        <v>-0.02796954126740608</v>
+        <v>-0.02977402780078712</v>
       </c>
       <c r="W7" t="n">
         <v>0.02889791874929446</v>
@@ -1280,7 +1280,7 @@
         <v>-0.005425457597809015</v>
       </c>
       <c r="V8" t="n">
-        <v>-0.01604657052499314</v>
+        <v>-0.01708183313950882</v>
       </c>
       <c r="W8" t="n">
         <v>-0.04328639151035411</v>
@@ -1383,7 +1383,7 @@
         <v>-0.004415955908644617</v>
       </c>
       <c r="V9" t="n">
-        <v>-0.0295004940177261</v>
+        <v>-0.03140375169628908</v>
       </c>
       <c r="W9" t="n">
         <v>-0.02963108672969265</v>
@@ -1486,7 +1486,7 @@
         <v>-0.002405492267089451</v>
       </c>
       <c r="V10" t="n">
-        <v>-0.02639820774602876</v>
+        <v>-0.02810131792319191</v>
       </c>
       <c r="W10" t="n">
         <v>-0.03429218526962157</v>
@@ -1589,7 +1589,7 @@
         <v>-0.00178183310199658</v>
       </c>
       <c r="V11" t="n">
-        <v>-0.00936865646858983</v>
+        <v>-0.009944317196613714</v>
       </c>
       <c r="W11" t="n">
         <v>-0.04829175851498334</v>
@@ -1692,7 +1692,7 @@
         <v>-0.00315088067895816</v>
       </c>
       <c r="V12" t="n">
-        <v>-0.009686465454185314</v>
+        <v>-0.01031139870929404</v>
       </c>
       <c r="W12" t="n">
         <v>-0.001553285430461922</v>
@@ -1795,7 +1795,7 @@
         <v>-0.004117112549703064</v>
       </c>
       <c r="V13" t="n">
-        <v>-0.01785194210075965</v>
+        <v>-0.01900368030080866</v>
       </c>
       <c r="W13" t="n">
         <v>-0.04745247097198309</v>
@@ -1898,7 +1898,7 @@
         <v>-1.379630375866064</v>
       </c>
       <c r="V14" t="n">
-        <v>-0.02050031588004539</v>
+        <v>-0.02182291690456445</v>
       </c>
       <c r="W14" t="n">
         <v>0.02256757433990903</v>
@@ -1931,7 +1931,7 @@
         <v>3.297158965890005</v>
       </c>
       <c r="AG14" t="n">
-        <v>-6.051455152389473</v>
+        <v>-6.051455152389472</v>
       </c>
     </row>
     <row r="15">
@@ -2001,7 +2001,7 @@
         <v>-0.007317276576014255</v>
       </c>
       <c r="V15" t="n">
-        <v>-0.02049106657626572</v>
+        <v>-0.02181307087150867</v>
       </c>
       <c r="W15" t="n">
         <v>-0.06060407089365231</v>
@@ -2104,7 +2104,7 @@
         <v>-0</v>
       </c>
       <c r="V16" t="n">
-        <v>-0.02160008946738107</v>
+        <v>-0.02299364362656695</v>
       </c>
       <c r="W16" t="n">
         <v>-0.02132240494236983</v>
@@ -2207,7 +2207,7 @@
         <v>-0.02487681866274705</v>
       </c>
       <c r="V17" t="n">
-        <v>-0.02528672036269618</v>
+        <v>-0.02691812167641852</v>
       </c>
       <c r="W17" t="n">
         <v>-0.01036219229424002</v>
@@ -2310,7 +2310,7 @@
         <v>-0.004715147321515603</v>
       </c>
       <c r="V18" t="n">
-        <v>-0.02825678703222972</v>
+        <v>-0.03007980555043809</v>
       </c>
       <c r="W18" t="n">
         <v>-0.02988238099641407</v>
@@ -2413,7 +2413,7 @@
         <v>-0.003300219966570374</v>
       </c>
       <c r="V19" t="n">
-        <v>-0.006134604002427083</v>
+        <v>-0.006530384905809475</v>
       </c>
       <c r="W19" t="n">
         <v>-0.05916328573754647</v>
@@ -2516,7 +2516,7 @@
         <v>-0.005181130545938043</v>
       </c>
       <c r="V20" t="n">
-        <v>-0.02121159430777428</v>
+        <v>-0.02258008426311456</v>
       </c>
       <c r="W20" t="n">
         <v>0.003798576830490822</v>
@@ -2619,7 +2619,7 @@
         <v>-0.00940176592196341</v>
       </c>
       <c r="V21" t="n">
-        <v>-0.02781557090439661</v>
+        <v>-0.02961012386597059</v>
       </c>
       <c r="W21" t="n">
         <v>0.01669973982278445</v>
@@ -2722,7 +2722,7 @@
         <v>-0.004680447088870762</v>
       </c>
       <c r="V22" t="n">
-        <v>-0.04934136108380265</v>
+        <v>-0.0525246747021125</v>
       </c>
       <c r="W22" t="n">
         <v>0.06034488210782132</v>
@@ -2825,7 +2825,7 @@
         <v>-0.004528265703097334</v>
       </c>
       <c r="V23" t="n">
-        <v>-0.02960454223534299</v>
+        <v>-0.03151451270213931</v>
       </c>
       <c r="W23" t="n">
         <v>0.01387218946199456</v>
@@ -2928,7 +2928,7 @@
         <v>-0.06618577597228457</v>
       </c>
       <c r="V24" t="n">
-        <v>-0.03159010703217852</v>
+        <v>-0.03362817845360939</v>
       </c>
       <c r="W24" t="n">
         <v>-0.06474090334131162</v>
@@ -3031,7 +3031,7 @@
         <v>-0.005137693971413827</v>
       </c>
       <c r="V25" t="n">
-        <v>-0.06886184540077024</v>
+        <v>-0.07330454510404574</v>
       </c>
       <c r="W25" t="n">
         <v>0.07705959095914858</v>
@@ -3134,7 +3134,7 @@
         <v>-0.001197096824273261</v>
       </c>
       <c r="V26" t="n">
-        <v>-0.02248894874789343</v>
+        <v>-0.02393984866711236</v>
       </c>
       <c r="W26" t="n">
         <v>0.007995156460562087</v>
@@ -3237,7 +3237,7 @@
         <v>-0.01020018127604768</v>
       </c>
       <c r="V27" t="n">
-        <v>-0.01838012833898668</v>
+        <v>-0.01956594307053421</v>
       </c>
       <c r="W27" t="n">
         <v>-0.05918194971373538</v>
@@ -3340,7 +3340,7 @@
         <v>-0.002131301729975717</v>
       </c>
       <c r="V28" t="n">
-        <v>-0.02307009171837146</v>
+        <v>-0.02455848473245995</v>
       </c>
       <c r="W28" t="n">
         <v>-0.07920542739232132</v>
@@ -3443,7 +3443,7 @@
         <v>-0.08440497192430108</v>
       </c>
       <c r="V29" t="n">
-        <v>-0.02288432042520977</v>
+        <v>-0.02425747755648504</v>
       </c>
       <c r="W29" t="n">
         <v>-0.03165683235147491</v>
@@ -3546,7 +3546,7 @@
         <v>-0.03992512136018329</v>
       </c>
       <c r="V30" t="n">
-        <v>-0.0157229186125985</v>
+        <v>-0.01673730045857259</v>
       </c>
       <c r="W30" t="n">
         <v>-0.03001580651365731</v>
@@ -3649,7 +3649,7 @@
         <v>-0.01177660231534626</v>
       </c>
       <c r="V31" t="n">
-        <v>-0.003161521691752886</v>
+        <v>-0.003255895504496828</v>
       </c>
       <c r="W31" t="n">
         <v>-0.02535938308364006</v>
@@ -3752,7 +3752,7 @@
         <v>-0.02903310428216221</v>
       </c>
       <c r="V32" t="n">
-        <v>-0.02542752858963314</v>
+        <v>-0.02706801430509334</v>
       </c>
       <c r="W32" t="n">
         <v>-0.02999020537277581</v>
@@ -3855,7 +3855,7 @@
         <v>-0.0156265996293639</v>
       </c>
       <c r="V33" t="n">
-        <v>-0.03685773209035448</v>
+        <v>-0.03923565028973219</v>
       </c>
       <c r="W33" t="n">
         <v>0.04324794225121848</v>
@@ -3958,7 +3958,7 @@
         <v>-0</v>
       </c>
       <c r="V34" t="n">
-        <v>-0.04399651183025172</v>
+        <v>-0.04683499646446151</v>
       </c>
       <c r="W34" t="n">
         <v>0.07650089851990881</v>
@@ -3991,7 +3991,7 @@
         <v>2.584924633664547</v>
       </c>
       <c r="AG34" t="n">
-        <v>-7.766735742086704</v>
+        <v>-7.766735742086705</v>
       </c>
     </row>
     <row r="35">
@@ -4061,7 +4061,7 @@
         <v>-0.0009382851204082873</v>
       </c>
       <c r="V35" t="n">
-        <v>-0.01273847796957286</v>
+        <v>-0.01356031525793239</v>
       </c>
       <c r="W35" t="n">
         <v>-0.02235778943724892</v>
@@ -4164,7 +4164,7 @@
         <v>-0.002583555994465855</v>
       </c>
       <c r="V36" t="n">
-        <v>-0.02323704289350942</v>
+        <v>-0.02396380221258047</v>
       </c>
       <c r="W36" t="n">
         <v>-0.04846202161789483</v>
@@ -4267,7 +4267,7 @@
         <v>-0.04134125182631532</v>
       </c>
       <c r="V37" t="n">
-        <v>-0.01554000883177202</v>
+        <v>-0.01654259004672505</v>
       </c>
       <c r="W37" t="n">
         <v>-0.03328775862919579</v>
@@ -4370,7 +4370,7 @@
         <v>-0.001505929182904178</v>
       </c>
       <c r="V38" t="n">
-        <v>-0.07878051562798098</v>
+        <v>-0.08347913895447956</v>
       </c>
       <c r="W38" t="n">
         <v>0.1114949428688813</v>
@@ -4473,7 +4473,7 @@
         <v>-0</v>
       </c>
       <c r="V39" t="n">
-        <v>-0.01100352315440931</v>
+        <v>-0.01171342787404863</v>
       </c>
       <c r="W39" t="n">
         <v>0.001404403801417163</v>
@@ -4576,7 +4576,7 @@
         <v>-0.004630048990826603</v>
       </c>
       <c r="V40" t="n">
-        <v>-0.02095699813811861</v>
+        <v>-0.02230906253412626</v>
       </c>
       <c r="W40" t="n">
         <v>-0.03981336546906516</v>
@@ -4679,7 +4679,7 @@
         <v>-0.004377784983794698</v>
       </c>
       <c r="V41" t="n">
-        <v>-0.001513509227653597</v>
+        <v>-0.00161115498427641</v>
       </c>
       <c r="W41" t="n">
         <v>-0.06912592366965621</v>
@@ -4782,7 +4782,7 @@
         <v>-0</v>
       </c>
       <c r="V42" t="n">
-        <v>-0.02025225766891607</v>
+        <v>-0.0215588549378784</v>
       </c>
       <c r="W42" t="n">
         <v>-0.07616286245590259</v>
@@ -4885,7 +4885,7 @@
         <v>-0.004159741412002104</v>
       </c>
       <c r="V43" t="n">
-        <v>-0.02706784992544257</v>
+        <v>-0.02881416282385822</v>
       </c>
       <c r="W43" t="n">
         <v>-0.03733391387972772</v>
@@ -4988,7 +4988,7 @@
         <v>-0.1050372767942514</v>
       </c>
       <c r="V44" t="n">
-        <v>-0.01079741463938554</v>
+        <v>-0.01149402203547493</v>
       </c>
       <c r="W44" t="n">
         <v>-0.05673327260908416</v>
@@ -5091,7 +5091,7 @@
         <v>-0</v>
       </c>
       <c r="V45" t="n">
-        <v>-0.02190581078201919</v>
+        <v>-0.02331908889698817</v>
       </c>
       <c r="W45" t="n">
         <v>-0.02141044117112621</v>
@@ -5194,7 +5194,7 @@
         <v>-0</v>
       </c>
       <c r="V46" t="n">
-        <v>-0.01374396344778112</v>
+        <v>-0.01457668835041486</v>
       </c>
       <c r="W46" t="n">
         <v>-0.03804547824011779</v>
@@ -5227,7 +5227,7 @@
         <v>2.395329167291155</v>
       </c>
       <c r="AG46" t="n">
-        <v>-9.671766722910993</v>
+        <v>-9.671766722910995</v>
       </c>
     </row>
     <row r="47">
@@ -5297,7 +5297,7 @@
         <v>-0.001910753585553961</v>
       </c>
       <c r="V47" t="n">
-        <v>-0.02113347325156888</v>
+        <v>-0.02249692313876687</v>
       </c>
       <c r="W47" t="n">
         <v>-0.08467070274294342</v>
@@ -5400,7 +5400,7 @@
         <v>-0.01302590339440693</v>
       </c>
       <c r="V48" t="n">
-        <v>-0.01682790613098656</v>
+        <v>-0.01791357749427602</v>
       </c>
       <c r="W48" t="n">
         <v>-0.05509687515363815</v>
@@ -5503,7 +5503,7 @@
         <v>-0</v>
       </c>
       <c r="V49" t="n">
-        <v>0.003260426692347203</v>
+        <v>0.003470776801530893</v>
       </c>
       <c r="W49" t="n">
         <v>-0.0197972358084675</v>
@@ -5606,7 +5606,7 @@
         <v>-0</v>
       </c>
       <c r="V50" t="n">
-        <v>-0.05331616686015751</v>
+        <v>-0.05675591956081284</v>
       </c>
       <c r="W50" t="n">
         <v>0.06141592511843775</v>
@@ -5709,7 +5709,7 @@
         <v>-0.02419824162144281</v>
       </c>
       <c r="V51" t="n">
-        <v>0.00682819889610726</v>
+        <v>0.007268727857146438</v>
       </c>
       <c r="W51" t="n">
         <v>-0.03918783135677703</v>
@@ -5812,7 +5812,7 @@
         <v>-0.007947055814867227</v>
       </c>
       <c r="V52" t="n">
-        <v>-0.02492192754559459</v>
+        <v>-0.02652979383885876</v>
       </c>
       <c r="W52" t="n">
         <v>0.01567749812016711</v>
@@ -5915,7 +5915,7 @@
         <v>-0.01216874793731972</v>
       </c>
       <c r="V53" t="n">
-        <v>0.01571235182759012</v>
+        <v>0.01672605194549916</v>
       </c>
       <c r="W53" t="n">
         <v>-0.06028722882779339</v>
@@ -6018,7 +6018,7 @@
         <v>-0.04872371123601588</v>
       </c>
       <c r="V54" t="n">
-        <v>-0.01159949735416566</v>
+        <v>-0.01234785202217635</v>
       </c>
       <c r="W54" t="n">
         <v>-0.01407887244322129</v>
@@ -6121,7 +6121,7 @@
         <v>-0.01160885251330833</v>
       </c>
       <c r="V55" t="n">
-        <v>-0.02466791610020921</v>
+        <v>-0.02625939455828722</v>
       </c>
       <c r="W55" t="n">
         <v>-0.04007872548350677</v>
@@ -6224,7 +6224,7 @@
         <v>-0.009858429928557443</v>
       </c>
       <c r="V56" t="n">
-        <v>-0.008653975433448155</v>
+        <v>-0.009212296429154488</v>
       </c>
       <c r="W56" t="n">
         <v>0.008496515441964999</v>
@@ -6327,7 +6327,7 @@
         <v>-0.004169525900134032</v>
       </c>
       <c r="V57" t="n">
-        <v>-0.03518055372705711</v>
+        <v>-0.03745026687073821</v>
       </c>
       <c r="W57" t="n">
         <v>-0.0186704196166897</v>
@@ -6430,7 +6430,7 @@
         <v>-0.01009422287066674</v>
       </c>
       <c r="V58" t="n">
-        <v>-0.0267898603190076</v>
+        <v>-0.02851823840410487</v>
       </c>
       <c r="W58" t="n">
         <v>0.03403071360061625</v>
@@ -6533,7 +6533,7 @@
         <v>-0.002149870643884635</v>
       </c>
       <c r="V59" t="n">
-        <v>-0.02140631466131048</v>
+        <v>-0.0227873672201047</v>
       </c>
       <c r="W59" t="n">
         <v>-0.04942109575554999</v>
@@ -6636,7 +6636,7 @@
         <v>-0.01595258504324894</v>
       </c>
       <c r="V60" t="n">
-        <v>-0.005718101105073843</v>
+        <v>-0.006087010853788285</v>
       </c>
       <c r="W60" t="n">
         <v>-0.05009775945084738</v>

</xml_diff>

<commit_message>
Update the phenotype_microbiome file
</commit_message>
<xml_diff>
--- a/input/comp_mrs_cat.xlsx
+++ b/input/comp_mrs_cat.xlsx
@@ -680,13 +680,13 @@
         <v>0.3217817741888539</v>
       </c>
       <c r="AB2" t="n">
-        <v>-0.07017307020429679</v>
+        <v>-0.166400372770544</v>
       </c>
       <c r="AC2" t="n">
         <v>-0.02253571108019671</v>
       </c>
       <c r="AD2" t="n">
-        <v>1.880354722814106</v>
+        <v>1.206763604850376</v>
       </c>
       <c r="AE2" t="n">
         <v>-10.71287134363504</v>
@@ -695,7 +695,7 @@
         <v>3.253217425700312</v>
       </c>
       <c r="AG2" t="n">
-        <v>-5.579299195120626</v>
+        <v>-6.252890313084356</v>
       </c>
     </row>
     <row r="3">
@@ -783,13 +783,13 @@
         <v>0.05218090395224684</v>
       </c>
       <c r="AB3" t="n">
-        <v>-0.03570594776254914</v>
+        <v>-0.295996312127685</v>
       </c>
       <c r="AC3" t="n">
         <v>0.05145483745961987</v>
       </c>
       <c r="AD3" t="n">
-        <v>1.160205198442633</v>
+        <v>-0.6618273521133181</v>
       </c>
       <c r="AE3" t="n">
         <v>-14.58010571514267</v>
@@ -798,7 +798,7 @@
         <v>1.848962917049874</v>
       </c>
       <c r="AG3" t="n">
-        <v>-11.57093759965016</v>
+        <v>-13.39297015020611</v>
       </c>
     </row>
     <row r="4">
@@ -886,13 +886,13 @@
         <v>0.1581203146599285</v>
       </c>
       <c r="AB4" t="n">
-        <v>-0.1612421228519281</v>
+        <v>-0.3074432006063255</v>
       </c>
       <c r="AC4" t="n">
         <v>-0.02311568454788574</v>
       </c>
       <c r="AD4" t="n">
-        <v>1.263719329021387</v>
+        <v>0.2403117847406054</v>
       </c>
       <c r="AE4" t="n">
         <v>-10.59408744031139</v>
@@ -901,7 +901,7 @@
         <v>3.84770481406579</v>
       </c>
       <c r="AG4" t="n">
-        <v>-5.482663297224214</v>
+        <v>-6.506070841504995</v>
       </c>
     </row>
     <row r="5">
@@ -989,13 +989,13 @@
         <v>0.2289954687923547</v>
       </c>
       <c r="AB5" t="n">
-        <v>-0.2013273141344778</v>
+        <v>-0.2902421723677454</v>
       </c>
       <c r="AC5" t="n">
         <v>-0.03391007751123196</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.2410808349646715</v>
+        <v>-0.3813231726682013</v>
       </c>
       <c r="AE5" t="n">
         <v>-10.19873570115378</v>
@@ -1004,7 +1004,7 @@
         <v>3.641193771392695</v>
       </c>
       <c r="AG5" t="n">
-        <v>-6.316461094796411</v>
+        <v>-6.938865102429284</v>
       </c>
     </row>
     <row r="6">
@@ -1092,13 +1092,13 @@
         <v>0.000256866576674956</v>
       </c>
       <c r="AB6" t="n">
-        <v>-0.1617026503197399</v>
+        <v>-0.3792063163659771</v>
       </c>
       <c r="AC6" t="n">
         <v>-0.1156702884233157</v>
       </c>
       <c r="AD6" t="n">
-        <v>-0.7893109803665219</v>
+        <v>-2.311836642690182</v>
       </c>
       <c r="AE6" t="n">
         <v>-14.38470400851906</v>
@@ -1107,7 +1107,7 @@
         <v>2.756894535999121</v>
       </c>
       <c r="AG6" t="n">
-        <v>-12.41712045288646</v>
+        <v>-13.93964611521012</v>
       </c>
     </row>
     <row r="7">
@@ -1195,13 +1195,13 @@
         <v>0.2617361715261289</v>
       </c>
       <c r="AB7" t="n">
-        <v>-0.233175306703107</v>
+        <v>-0.2372094180570924</v>
       </c>
       <c r="AC7" t="n">
         <v>0.01656407546583211</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.09176682659777449</v>
+        <v>0.06352804711987661</v>
       </c>
       <c r="AE7" t="n">
         <v>-12.52251865458284</v>
@@ -1210,7 +1210,7 @@
         <v>3.119152271531618</v>
       </c>
       <c r="AG7" t="n">
-        <v>-9.311599556453448</v>
+        <v>-9.339838335931347</v>
       </c>
     </row>
     <row r="8">
@@ -1298,13 +1298,13 @@
         <v>0.002572109935550683</v>
       </c>
       <c r="AB8" t="n">
-        <v>-0.09606169688343277</v>
+        <v>-0.354056202531341</v>
       </c>
       <c r="AC8" t="n">
         <v>0.03658320797548056</v>
       </c>
       <c r="AD8" t="n">
-        <v>-0.8071786683591793</v>
+        <v>-2.613140207894537</v>
       </c>
       <c r="AE8" t="n">
         <v>-15.0921182512653</v>
@@ -1313,7 +1313,7 @@
         <v>1.785537558360071</v>
       </c>
       <c r="AG8" t="n">
-        <v>-14.11375936126441</v>
+        <v>-15.91972090079977</v>
       </c>
     </row>
     <row r="9">
@@ -1401,13 +1401,13 @@
         <v>0.1063990140144021</v>
       </c>
       <c r="AB9" t="n">
-        <v>-0.138315192858073</v>
+        <v>-0.3666067631597452</v>
       </c>
       <c r="AC9" t="n">
         <v>-0.0257802155774243</v>
       </c>
       <c r="AD9" t="n">
-        <v>-0.8788573178155932</v>
+        <v>-2.476898309927298</v>
       </c>
       <c r="AE9" t="n">
         <v>-12.25232032141117</v>
@@ -1416,7 +1416,7 @@
         <v>3.004803121989122</v>
       </c>
       <c r="AG9" t="n">
-        <v>-10.12637451723764</v>
+        <v>-11.72441550934934</v>
       </c>
     </row>
     <row r="10">
@@ -1504,13 +1504,13 @@
         <v>0.1178200963918431</v>
       </c>
       <c r="AB10" t="n">
-        <v>-0.1151802791739185</v>
+        <v>-0.359883292689782</v>
       </c>
       <c r="AC10" t="n">
         <v>-0.02989159533577808</v>
       </c>
       <c r="AD10" t="n">
-        <v>-0.36756372605574</v>
+        <v>-2.080484820666785</v>
       </c>
       <c r="AE10" t="n">
         <v>-13.43421122439342</v>
@@ -1519,7 +1519,7 @@
         <v>2.468263610591526</v>
       </c>
       <c r="AG10" t="n">
-        <v>-11.33351133985763</v>
+        <v>-13.04643243446868</v>
       </c>
     </row>
     <row r="11">
@@ -1607,13 +1607,13 @@
         <v>0.02746085482650446</v>
       </c>
       <c r="AB11" t="n">
-        <v>-0.05422453157262382</v>
+        <v>-0.323263173420538</v>
       </c>
       <c r="AC11" t="n">
         <v>0.005491268636792317</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.01024056362713198</v>
+        <v>-1.873029929308267</v>
       </c>
       <c r="AE11" t="n">
         <v>-11.93731123504216</v>
@@ -1622,7 +1622,7 @@
         <v>1.21525785660293</v>
       </c>
       <c r="AG11" t="n">
-        <v>-10.7118128148121</v>
+        <v>-12.5950833077475</v>
       </c>
     </row>
     <row r="12">
@@ -1710,13 +1710,13 @@
         <v>0.01875854222731535</v>
       </c>
       <c r="AB12" t="n">
-        <v>-0.06051661563918916</v>
+        <v>-0.3288605364191713</v>
       </c>
       <c r="AC12" t="n">
         <v>0.0860694672710957</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.3365331903699944</v>
+        <v>-1.541874255089881</v>
       </c>
       <c r="AE12" t="n">
         <v>-11.69034257985</v>
@@ -1725,7 +1725,7 @@
         <v>1.398649254021426</v>
       </c>
       <c r="AG12" t="n">
-        <v>-9.955160135458577</v>
+        <v>-11.83356758091845</v>
       </c>
     </row>
     <row r="13">
@@ -1813,13 +1813,13 @@
         <v>0.1522226675145052</v>
       </c>
       <c r="AB13" t="n">
-        <v>-0.06138591613981749</v>
+        <v>-0.3114362264009238</v>
       </c>
       <c r="AC13" t="n">
         <v>-0.01425994787852184</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.8706559916903328</v>
+        <v>-0.8796961801374111</v>
       </c>
       <c r="AE13" t="n">
         <v>-12.74396681066839</v>
@@ -1828,7 +1828,7 @@
         <v>2.326473128727222</v>
       </c>
       <c r="AG13" t="n">
-        <v>-9.54683769025084</v>
+        <v>-11.29718986207859</v>
       </c>
     </row>
     <row r="14">
@@ -1916,13 +1916,13 @@
         <v>0.08365519128142866</v>
       </c>
       <c r="AB14" t="n">
-        <v>-0.1150521858683806</v>
+        <v>-0.2936119744798988</v>
       </c>
       <c r="AC14" t="n">
         <v>0.01950246349247608</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.5335503070264205</v>
+        <v>-0.7163682132542064</v>
       </c>
       <c r="AE14" t="n">
         <v>-9.882164425305898</v>
@@ -1931,7 +1931,7 @@
         <v>3.297158965890005</v>
       </c>
       <c r="AG14" t="n">
-        <v>-6.051455152389472</v>
+        <v>-7.301373672670099</v>
       </c>
     </row>
     <row r="15">
@@ -2019,13 +2019,13 @@
         <v>0.2522495684019206</v>
       </c>
       <c r="AB15" t="n">
-        <v>-0.1080074877997258</v>
+        <v>-0.336108560818545</v>
       </c>
       <c r="AC15" t="n">
         <v>-0.08801296918238558</v>
       </c>
       <c r="AD15" t="n">
-        <v>-0.3007246977056999</v>
+        <v>-1.897432208837434</v>
       </c>
       <c r="AE15" t="n">
         <v>-11.80059150596449</v>
@@ -2034,7 +2034,7 @@
         <v>2.713662913782229</v>
       </c>
       <c r="AG15" t="n">
-        <v>-9.387653289887957</v>
+        <v>-10.98436080101969</v>
       </c>
     </row>
     <row r="16">
@@ -2122,13 +2122,13 @@
         <v>0.03031446488649711</v>
       </c>
       <c r="AB16" t="n">
-        <v>-0.04219664885616636</v>
+        <v>-0.2825910882449856</v>
       </c>
       <c r="AC16" t="n">
         <v>0.02343061746642033</v>
       </c>
       <c r="AD16" t="n">
-        <v>0.4065876255219431</v>
+        <v>-1.276173450199792</v>
       </c>
       <c r="AE16" t="n">
         <v>-11.54009724639915</v>
@@ -2137,7 +2137,7 @@
         <v>2.176770978233852</v>
       </c>
       <c r="AG16" t="n">
-        <v>-8.956738642643352</v>
+        <v>-10.63949971836509</v>
       </c>
     </row>
     <row r="17">
@@ -2225,13 +2225,13 @@
         <v>0.1028599066275024</v>
       </c>
       <c r="AB17" t="n">
-        <v>-0.05404592228070815</v>
+        <v>-0.2822367851134115</v>
       </c>
       <c r="AC17" t="n">
         <v>0.01266755913370944</v>
       </c>
       <c r="AD17" t="n">
-        <v>-0.1609253440295031</v>
+        <v>-1.758261383858426</v>
       </c>
       <c r="AE17" t="n">
         <v>-15.37674820929016</v>
@@ -2240,7 +2240,7 @@
         <v>2.79833508502352</v>
       </c>
       <c r="AG17" t="n">
-        <v>-12.73933846829614</v>
+        <v>-14.33667450812506</v>
       </c>
     </row>
     <row r="18">
@@ -2328,13 +2328,13 @@
         <v>0.004657715238659752</v>
       </c>
       <c r="AB18" t="n">
-        <v>-0.1321892540934846</v>
+        <v>-0.3738842957307086</v>
       </c>
       <c r="AC18" t="n">
         <v>-0.1048208634132849</v>
       </c>
       <c r="AD18" t="n">
-        <v>-0.4853676978947175</v>
+        <v>-2.177232989355285</v>
       </c>
       <c r="AE18" t="n">
         <v>-13.42280115001057</v>
@@ -2343,7 +2343,7 @@
         <v>2.289331898834243</v>
       </c>
       <c r="AG18" t="n">
-        <v>-11.61883694907104</v>
+        <v>-13.31070224053161</v>
       </c>
     </row>
     <row r="19">
@@ -2431,13 +2431,13 @@
         <v>0.07890103011922783</v>
       </c>
       <c r="AB19" t="n">
-        <v>-0.03446330418885177</v>
+        <v>-0.3059633354622712</v>
       </c>
       <c r="AC19" t="n">
         <v>0.01469753701812776</v>
       </c>
       <c r="AD19" t="n">
-        <v>-0.3152810844358349</v>
+        <v>-2.215781303349771</v>
       </c>
       <c r="AE19" t="n">
         <v>-12.11501624570678</v>
@@ -2446,7 +2446,7 @@
         <v>1.034388269386078</v>
       </c>
       <c r="AG19" t="n">
-        <v>-11.39590906075654</v>
+        <v>-13.29640927967048</v>
       </c>
     </row>
     <row r="20">
@@ -2534,13 +2534,13 @@
         <v>0.05617141471529325</v>
       </c>
       <c r="AB20" t="n">
-        <v>-0.1596803015630923</v>
+        <v>-0.1714054313875508</v>
       </c>
       <c r="AC20" t="n">
         <v>0.07552317554046717</v>
       </c>
       <c r="AD20" t="n">
-        <v>2.569938285446573</v>
+        <v>2.487862376675363</v>
       </c>
       <c r="AE20" t="n">
         <v>-13.73356444982923</v>
@@ -2549,7 +2549,7 @@
         <v>2.367888785783177</v>
       </c>
       <c r="AG20" t="n">
-        <v>-8.79573737859948</v>
+        <v>-8.877813287370689</v>
       </c>
     </row>
     <row r="21">
@@ -2637,13 +2637,13 @@
         <v>0.02905311724059727</v>
       </c>
       <c r="AB21" t="n">
-        <v>-0.146702538617229</v>
+        <v>-0.388626272628939</v>
       </c>
       <c r="AC21" t="n">
         <v>0.06652481685425474</v>
       </c>
       <c r="AD21" t="n">
-        <v>1.201526142282055</v>
+        <v>-0.4919399957999145</v>
       </c>
       <c r="AE21" t="n">
         <v>-13.21489960443659</v>
@@ -2652,7 +2652,7 @@
         <v>2.496649824908592</v>
       </c>
       <c r="AG21" t="n">
-        <v>-9.516723637245937</v>
+        <v>-11.21018977532791</v>
       </c>
     </row>
     <row r="22">
@@ -2740,13 +2740,13 @@
         <v>0.001560149029623587</v>
       </c>
       <c r="AB22" t="n">
-        <v>-0.2002605397648755</v>
+        <v>-0.211315038441335</v>
       </c>
       <c r="AC22" t="n">
         <v>-0.01791581281148704</v>
       </c>
       <c r="AD22" t="n">
-        <v>2.353659535265955</v>
+        <v>2.276278044530738</v>
       </c>
       <c r="AE22" t="n">
         <v>-12.23345658516506</v>
@@ -2755,7 +2755,7 @@
         <v>3.276139743624471</v>
       </c>
       <c r="AG22" t="n">
-        <v>-6.603657306274636</v>
+        <v>-6.681038797009853</v>
       </c>
     </row>
     <row r="23">
@@ -2843,13 +2843,13 @@
         <v>0.07278670528648094</v>
       </c>
       <c r="AB23" t="n">
-        <v>-0.1773995312111843</v>
+        <v>-0.3911413300651606</v>
       </c>
       <c r="AC23" t="n">
         <v>-0.01723232483948973</v>
       </c>
       <c r="AD23" t="n">
-        <v>1.055292999703113</v>
+        <v>-0.4408995922747213</v>
       </c>
       <c r="AE23" t="n">
         <v>-11.5992000271969</v>
@@ -2858,7 +2858,7 @@
         <v>3.149142237757889</v>
       </c>
       <c r="AG23" t="n">
-        <v>-7.394764789735897</v>
+        <v>-8.890957381713731</v>
       </c>
     </row>
     <row r="24">
@@ -2946,13 +2946,13 @@
         <v>0.2974052605301021</v>
       </c>
       <c r="AB24" t="n">
-        <v>-0.0607841328736138</v>
+        <v>-0.2914807327057374</v>
       </c>
       <c r="AC24" t="n">
         <v>0.02140151786384475</v>
       </c>
       <c r="AD24" t="n">
-        <v>0.665569400006578</v>
+        <v>-0.9493067988182872</v>
       </c>
       <c r="AE24" t="n">
         <v>-11.46661957331528</v>
@@ -2961,7 +2961,7 @@
         <v>2.480869506725185</v>
       </c>
       <c r="AG24" t="n">
-        <v>-8.320180666583518</v>
+        <v>-9.935056865408384</v>
       </c>
     </row>
     <row r="25">
@@ -3049,13 +3049,13 @@
         <v>0.223989214557176</v>
       </c>
       <c r="AB25" t="n">
-        <v>-0.1733208992790237</v>
+        <v>-0.1952355654546289</v>
       </c>
       <c r="AC25" t="n">
         <v>-0.1252764488401676</v>
       </c>
       <c r="AD25" t="n">
-        <v>-1.17753979080433</v>
+        <v>-1.330942454033567</v>
       </c>
       <c r="AE25" t="n">
         <v>-9.98027283460573</v>
@@ -3064,7 +3064,7 @@
         <v>3.828349514488567</v>
       </c>
       <c r="AG25" t="n">
-        <v>-7.329463110921493</v>
+        <v>-7.48286577415073</v>
       </c>
     </row>
     <row r="26">
@@ -3152,13 +3152,13 @@
         <v>0.1428386930053857</v>
       </c>
       <c r="AB26" t="n">
-        <v>-0.1004406976427049</v>
+        <v>-0.3547353885848022</v>
       </c>
       <c r="AC26" t="n">
         <v>-0.005562017600533308</v>
       </c>
       <c r="AD26" t="n">
-        <v>1.707352774745438</v>
+        <v>-0.07271006184924378</v>
       </c>
       <c r="AE26" t="n">
         <v>-14.51851968851755</v>
@@ -3167,7 +3167,7 @@
         <v>1.907476798064713</v>
       </c>
       <c r="AG26" t="n">
-        <v>-10.9036901157074</v>
+        <v>-12.68375295230208</v>
       </c>
     </row>
     <row r="27">
@@ -3255,13 +3255,13 @@
         <v>0.2133597810137022</v>
       </c>
       <c r="AB27" t="n">
-        <v>-0.08901275588646708</v>
+        <v>-0.3453339062761586</v>
       </c>
       <c r="AC27" t="n">
         <v>-0.004944895094070909</v>
       </c>
       <c r="AD27" t="n">
-        <v>-0.01614545552741568</v>
+        <v>-1.810393508255256</v>
       </c>
       <c r="AE27" t="n">
         <v>-12.01886751273979</v>
@@ -3270,7 +3270,7 @@
         <v>2.030937895387919</v>
       </c>
       <c r="AG27" t="n">
-        <v>-10.00407507287928</v>
+        <v>-11.79832312560712</v>
       </c>
     </row>
     <row r="28">
@@ -3358,13 +3358,13 @@
         <v>0.2933569295274565</v>
       </c>
       <c r="AB28" t="n">
-        <v>-0.04566274694072794</v>
+        <v>-0.2726968453543164</v>
       </c>
       <c r="AC28" t="n">
         <v>-0.0566012107196378</v>
       </c>
       <c r="AD28" t="n">
-        <v>0.2968135463282928</v>
+        <v>-1.292425142566827</v>
       </c>
       <c r="AE28" t="n">
         <v>-15.37167225364937</v>
@@ -3373,7 +3373,7 @@
         <v>2.79206825249104</v>
       </c>
       <c r="AG28" t="n">
-        <v>-12.28279045483004</v>
+        <v>-13.87202914372516</v>
       </c>
     </row>
     <row r="29">
@@ -3461,13 +3461,13 @@
         <v>0.3364623363140553</v>
       </c>
       <c r="AB29" t="n">
-        <v>-0.2023950398392411</v>
+        <v>-0.3557734116958147</v>
       </c>
       <c r="AC29" t="n">
         <v>-0.1544274508518571</v>
       </c>
       <c r="AD29" t="n">
-        <v>-1.731324694150915</v>
+        <v>-2.804973297146931</v>
       </c>
       <c r="AE29" t="n">
         <v>-13.5241701207883</v>
@@ -3476,7 +3476,7 @@
         <v>3.83664770245198</v>
       </c>
       <c r="AG29" t="n">
-        <v>-11.41884711248723</v>
+        <v>-12.49249571548325</v>
       </c>
     </row>
     <row r="30">
@@ -3564,13 +3564,13 @@
         <v>0.1940060946409356</v>
       </c>
       <c r="AB30" t="n">
-        <v>-0.08221365193754618</v>
+        <v>-0.3330484021214341</v>
       </c>
       <c r="AC30" t="n">
         <v>-0.01375837472189369</v>
       </c>
       <c r="AD30" t="n">
-        <v>-2.888459615170522</v>
+        <v>-4.644302866457737</v>
       </c>
       <c r="AE30" t="n">
         <v>-11.49508205430502</v>
@@ -3579,7 +3579,7 @@
         <v>2.233250709367881</v>
       </c>
       <c r="AG30" t="n">
-        <v>-12.15029096010766</v>
+        <v>-13.90613421139488</v>
       </c>
     </row>
     <row r="31">
@@ -3667,13 +3667,13 @@
         <v>0.2506633533019865</v>
       </c>
       <c r="AB31" t="n">
-        <v>-0.1920288728395179</v>
+        <v>-0.4280826510776105</v>
       </c>
       <c r="AC31" t="n">
         <v>-0.09324834772141333</v>
       </c>
       <c r="AD31" t="n">
-        <v>0.4120992700091757</v>
+        <v>-1.240277177657472</v>
       </c>
       <c r="AE31" t="n">
         <v>-13.10995632210551</v>
@@ -3682,7 +3682,7 @@
         <v>3.068661166125489</v>
       </c>
       <c r="AG31" t="n">
-        <v>-9.62919588597085</v>
+        <v>-11.2815723336375</v>
       </c>
     </row>
     <row r="32">
@@ -3770,13 +3770,13 @@
         <v>0.216450839324619</v>
       </c>
       <c r="AB32" t="n">
-        <v>-0.07910358993796011</v>
+        <v>-0.3149096965297397</v>
       </c>
       <c r="AC32" t="n">
         <v>-0.03038792594645022</v>
       </c>
       <c r="AD32" t="n">
-        <v>-2.162919986593938</v>
+        <v>-3.813562732736394</v>
       </c>
       <c r="AE32" t="n">
         <v>-12.15714777458812</v>
@@ -3785,7 +3785,7 @@
         <v>2.843440208312904</v>
       </c>
       <c r="AG32" t="n">
-        <v>-11.47662755286915</v>
+        <v>-13.12727029901161</v>
       </c>
     </row>
     <row r="33">
@@ -3873,13 +3873,13 @@
         <v>0.05497114366317671</v>
       </c>
       <c r="AB33" t="n">
-        <v>-0.2441498820600434</v>
+        <v>-0.2600970374300035</v>
       </c>
       <c r="AC33" t="n">
         <v>0.01458613964633884</v>
       </c>
       <c r="AD33" t="n">
-        <v>-0.1628747295272073</v>
+        <v>-0.2745048171169281</v>
       </c>
       <c r="AE33" t="n">
         <v>-12.95483354674426</v>
@@ -3888,7 +3888,7 @@
         <v>3.343456731499479</v>
       </c>
       <c r="AG33" t="n">
-        <v>-9.774251544771984</v>
+        <v>-9.885881632361704</v>
       </c>
     </row>
     <row r="34">
@@ -3976,13 +3976,13 @@
         <v>-0.001138496900938303</v>
       </c>
       <c r="AB34" t="n">
-        <v>-0.1223463028689423</v>
+        <v>-0.12548761041987</v>
       </c>
       <c r="AC34" t="n">
         <v>-0.01172553878460611</v>
       </c>
       <c r="AD34" t="n">
-        <v>1.084240021166025</v>
+        <v>1.062250868309531</v>
       </c>
       <c r="AE34" t="n">
         <v>-11.43590039691728</v>
@@ -3991,7 +3991,7 @@
         <v>2.584924633664547</v>
       </c>
       <c r="AG34" t="n">
-        <v>-7.766735742086705</v>
+        <v>-7.788724894943198</v>
       </c>
     </row>
     <row r="35">
@@ -4079,13 +4079,13 @@
         <v>0.1620143090696582</v>
       </c>
       <c r="AB35" t="n">
-        <v>-0.1662318820686763</v>
+        <v>-0.360747391990778</v>
       </c>
       <c r="AC35" t="n">
         <v>-0.01210242488285608</v>
       </c>
       <c r="AD35" t="n">
-        <v>1.753225247087765</v>
+        <v>0.3916166776330529</v>
       </c>
       <c r="AE35" t="n">
         <v>-13.36936733974361</v>
@@ -4094,7 +4094,7 @@
         <v>2.633644577255411</v>
       </c>
       <c r="AG35" t="n">
-        <v>-8.982497515400432</v>
+        <v>-10.34410608485515</v>
       </c>
     </row>
     <row r="36">
@@ -4182,13 +4182,13 @@
         <v>0.1872980485485691</v>
       </c>
       <c r="AB36" t="n">
-        <v>-0.1127755515204362</v>
+        <v>-0.3396246821899999</v>
       </c>
       <c r="AC36" t="n">
         <v>-0.04310079228356984</v>
       </c>
       <c r="AD36" t="n">
-        <v>-0.628671139442126</v>
+        <v>-2.216615054129072</v>
       </c>
       <c r="AE36" t="n">
         <v>-15.49813795156405</v>
@@ -4197,7 +4197,7 @@
         <v>2.909579690590713</v>
       </c>
       <c r="AG36" t="n">
-        <v>-13.21722940041546</v>
+        <v>-14.80517331510241</v>
       </c>
     </row>
     <row r="37">
@@ -4285,13 +4285,13 @@
         <v>0.08465109450326329</v>
       </c>
       <c r="AB37" t="n">
-        <v>-0.09950743356071774</v>
+        <v>-0.3061277679427306</v>
       </c>
       <c r="AC37" t="n">
         <v>0.07903386814482644</v>
       </c>
       <c r="AD37" t="n">
-        <v>1.499145087651529</v>
+        <v>0.05280274697743949</v>
       </c>
       <c r="AE37" t="n">
         <v>-12.66543848325756</v>
@@ -4300,7 +4300,7 @@
         <v>3.157693416302038</v>
       </c>
       <c r="AG37" t="n">
-        <v>-8.008599979303989</v>
+        <v>-9.454942319978079</v>
       </c>
     </row>
     <row r="38">
@@ -4388,13 +4388,13 @@
         <v>-0.01868504957018772</v>
       </c>
       <c r="AB38" t="n">
-        <v>-0.2476512555869857</v>
+        <v>-0.2574029041840175</v>
       </c>
       <c r="AC38" t="n">
         <v>-0.1835343718749725</v>
       </c>
       <c r="AD38" t="n">
-        <v>-2.304652066047888</v>
+        <v>-2.37291360622711</v>
       </c>
       <c r="AE38" t="n">
         <v>-13.61467158714544</v>
@@ -4403,7 +4403,7 @@
         <v>3.432658560789324</v>
       </c>
       <c r="AG38" t="n">
-        <v>-12.486665092404</v>
+        <v>-12.55492663258322</v>
       </c>
     </row>
     <row r="39">
@@ -4491,13 +4491,13 @@
         <v>-0.004854780936305264</v>
       </c>
       <c r="AB39" t="n">
-        <v>-0.07321779553341845</v>
+        <v>-0.3255151247602819</v>
       </c>
       <c r="AC39" t="n">
         <v>0.1465525741500207</v>
       </c>
       <c r="AD39" t="n">
-        <v>1.060316433221241</v>
+        <v>-0.7057648713668029</v>
       </c>
       <c r="AE39" t="n">
         <v>-14.47207605144228</v>
@@ -4506,7 +4506,7 @@
         <v>1.700090545577031</v>
       </c>
       <c r="AG39" t="n">
-        <v>-11.71166907264401</v>
+        <v>-13.47775037723206</v>
       </c>
     </row>
     <row r="40">
@@ -4594,13 +4594,13 @@
         <v>0.3749577094189353</v>
       </c>
       <c r="AB40" t="n">
-        <v>-0.2403033457363206</v>
+        <v>-0.2787200484459515</v>
       </c>
       <c r="AC40" t="n">
         <v>0.05222368188633728</v>
       </c>
       <c r="AD40" t="n">
-        <v>1.328540635376679</v>
+        <v>1.059623716409263</v>
       </c>
       <c r="AE40" t="n">
         <v>-10.88123827321872</v>
@@ -4609,7 +4609,7 @@
         <v>3.031725283185861</v>
       </c>
       <c r="AG40" t="n">
-        <v>-6.520972354656181</v>
+        <v>-6.789889273623598</v>
       </c>
     </row>
     <row r="41">
@@ -4697,13 +4697,13 @@
         <v>0.01364078174187934</v>
       </c>
       <c r="AB41" t="n">
-        <v>-0.0478015526197952</v>
+        <v>-0.2927032072016966</v>
       </c>
       <c r="AC41" t="n">
         <v>0.1243715227320841</v>
       </c>
       <c r="AD41" t="n">
-        <v>1.200361501590282</v>
+        <v>-0.513950080483028</v>
       </c>
       <c r="AE41" t="n">
         <v>-14.66525189983984</v>
@@ -4712,7 +4712,7 @@
         <v>1.76104150121723</v>
       </c>
       <c r="AG41" t="n">
-        <v>-11.70384889703233</v>
+        <v>-13.41816047910564</v>
       </c>
     </row>
     <row r="42">
@@ -4800,13 +4800,13 @@
         <v>0.2253924869779931</v>
       </c>
       <c r="AB42" t="n">
-        <v>-0.1247325745368508</v>
+        <v>-0.364362594078273</v>
       </c>
       <c r="AC42" t="n">
         <v>-0.1240316426625881</v>
       </c>
       <c r="AD42" t="n">
-        <v>-0.1395944581824572</v>
+        <v>-1.817004594972412</v>
       </c>
       <c r="AE42" t="n">
         <v>-13.7896516881348</v>
@@ -4815,7 +4815,7 @@
         <v>2.407429868159737</v>
       </c>
       <c r="AG42" t="n">
-        <v>-11.52181627815752</v>
+        <v>-13.19922641494747</v>
       </c>
     </row>
     <row r="43">
@@ -4903,13 +4903,13 @@
         <v>0.3031319054320287</v>
       </c>
       <c r="AB43" t="n">
-        <v>-0.1730939102254399</v>
+        <v>-0.3814164375157714</v>
       </c>
       <c r="AC43" t="n">
         <v>-0.03817945356419498</v>
       </c>
       <c r="AD43" t="n">
-        <v>2.222951024299609</v>
+        <v>0.7646933332672882</v>
       </c>
       <c r="AE43" t="n">
         <v>-12.91365853710254</v>
@@ -4918,7 +4918,7 @@
         <v>2.816984400016397</v>
       </c>
       <c r="AG43" t="n">
-        <v>-7.87372311278653</v>
+        <v>-9.331980803818851</v>
       </c>
     </row>
     <row r="44">
@@ -5006,13 +5006,13 @@
         <v>0.04428380612626755</v>
       </c>
       <c r="AB44" t="n">
-        <v>-0.09511147720648441</v>
+        <v>-0.3325576634969708</v>
       </c>
       <c r="AC44" t="n">
         <v>0.03989310575973623</v>
       </c>
       <c r="AD44" t="n">
-        <v>0.7297410059872054</v>
+        <v>-0.9323822980461995</v>
       </c>
       <c r="AE44" t="n">
         <v>-12.58299944621622</v>
@@ -5021,7 +5021,7 @@
         <v>2.105639746971739</v>
       </c>
       <c r="AG44" t="n">
-        <v>-9.747618693257271</v>
+        <v>-11.40974199729068</v>
       </c>
     </row>
     <row r="45">
@@ -5109,13 +5109,13 @@
         <v>0.1678167311473384</v>
       </c>
       <c r="AB45" t="n">
-        <v>-0.1348847002901711</v>
+        <v>-0.33874534569127</v>
       </c>
       <c r="AC45" t="n">
         <v>0.003968274312813186</v>
       </c>
       <c r="AD45" t="n">
-        <v>1.169876004610023</v>
+        <v>-0.2571485131976691</v>
       </c>
       <c r="AE45" t="n">
         <v>-12.0595945518373</v>
@@ -5124,7 +5124,7 @@
         <v>3.293796111048356</v>
       </c>
       <c r="AG45" t="n">
-        <v>-7.595922436178923</v>
+        <v>-9.022946953986615</v>
       </c>
     </row>
     <row r="46">
@@ -5212,13 +5212,13 @@
         <v>0.1499860621409728</v>
       </c>
       <c r="AB46" t="n">
-        <v>-0.1421947695082295</v>
+        <v>-0.3821023360168416</v>
       </c>
       <c r="AC46" t="n">
         <v>0.04526844422307467</v>
       </c>
       <c r="AD46" t="n">
-        <v>1.953585008649281</v>
+        <v>0.2742320430889965</v>
       </c>
       <c r="AE46" t="n">
         <v>-14.02068089885143</v>
@@ -5227,7 +5227,7 @@
         <v>2.395329167291155</v>
       </c>
       <c r="AG46" t="n">
-        <v>-9.671766722910995</v>
+        <v>-11.35111968847128</v>
       </c>
     </row>
     <row r="47">
@@ -5315,13 +5315,13 @@
         <v>0.1076512542135793</v>
       </c>
       <c r="AB47" t="n">
-        <v>-0.1536516028968188</v>
+        <v>-0.3565462312341346</v>
       </c>
       <c r="AC47" t="n">
         <v>-0.08771332036010683</v>
       </c>
       <c r="AD47" t="n">
-        <v>-0.9808252429722474</v>
+        <v>-2.401087641333458</v>
       </c>
       <c r="AE47" t="n">
         <v>-13.76433087242771</v>
@@ -5330,7 +5330,7 @@
         <v>2.57710761741724</v>
       </c>
       <c r="AG47" t="n">
-        <v>-12.16804849798271</v>
+        <v>-13.58831089634392</v>
       </c>
     </row>
     <row r="48">
@@ -5418,13 +5418,13 @@
         <v>0.1015559042416925</v>
       </c>
       <c r="AB48" t="n">
-        <v>-0.0225485170932838</v>
+        <v>-0.2638665020039602</v>
       </c>
       <c r="AC48" t="n">
         <v>0.01171826334382941</v>
       </c>
       <c r="AD48" t="n">
-        <v>-0.3291890558271496</v>
+        <v>-2.018414950201884</v>
       </c>
       <c r="AE48" t="n">
         <v>-13.58696023262923</v>
@@ -5433,7 +5433,7 @@
         <v>2.375564778330544</v>
       </c>
       <c r="AG48" t="n">
-        <v>-11.54058451012583</v>
+        <v>-13.22981040450057</v>
       </c>
     </row>
     <row r="49">
@@ -5521,13 +5521,13 @@
         <v>0.4727449176712932</v>
       </c>
       <c r="AB49" t="n">
-        <v>-0.05476731098093935</v>
+        <v>-0.06033166280510745</v>
       </c>
       <c r="AC49" t="n">
         <v>-0.01100958685467849</v>
       </c>
       <c r="AD49" t="n">
-        <v>2.599782145581028</v>
+        <v>2.560831682811852</v>
       </c>
       <c r="AE49" t="n">
         <v>-11.44494132331521</v>
@@ -5536,7 +5536,7 @@
         <v>2.725849737383146</v>
       </c>
       <c r="AG49" t="n">
-        <v>-6.119309440351036</v>
+        <v>-6.158259903120213</v>
       </c>
     </row>
     <row r="50">
@@ -5624,13 +5624,13 @@
         <v>0.1339330134230141</v>
       </c>
       <c r="AB50" t="n">
-        <v>-0.248052521384538</v>
+        <v>-0.2531421791624721</v>
       </c>
       <c r="AC50" t="n">
         <v>-0.1035686816929112</v>
       </c>
       <c r="AD50" t="n">
-        <v>-1.421491056324024</v>
+        <v>-1.457118660769562</v>
       </c>
       <c r="AE50" t="n">
         <v>-11.06433018238832</v>
@@ -5639,7 +5639,7 @@
         <v>2.96434199520753</v>
       </c>
       <c r="AG50" t="n">
-        <v>-9.521479243504817</v>
+        <v>-9.557106847950354</v>
       </c>
     </row>
     <row r="51">
@@ -5727,13 +5727,13 @@
         <v>0.1038183791125062</v>
       </c>
       <c r="AB51" t="n">
-        <v>0.00957368520861855</v>
+        <v>-0.2598579162039645</v>
       </c>
       <c r="AC51" t="n">
         <v>0.01446724075091104</v>
       </c>
       <c r="AD51" t="n">
-        <v>-0.07401219719253563</v>
+        <v>-1.960033407080617</v>
       </c>
       <c r="AE51" t="n">
         <v>-9.811596911047625</v>
@@ -5742,7 +5742,7 @@
         <v>1.394942178171137</v>
       </c>
       <c r="AG51" t="n">
-        <v>-8.490666930069024</v>
+        <v>-10.37668813995711</v>
       </c>
     </row>
     <row r="52">
@@ -5830,13 +5830,13 @@
         <v>0.005788791873921934</v>
       </c>
       <c r="AB52" t="n">
-        <v>-0.2765634072932374</v>
+        <v>-0.2853614256819633</v>
       </c>
       <c r="AC52" t="n">
         <v>-0.05476918884983398</v>
       </c>
       <c r="AD52" t="n">
-        <v>-1.329361397044852</v>
+        <v>-1.390947525765934</v>
       </c>
       <c r="AE52" t="n">
         <v>-12.52304508827194</v>
@@ -5845,7 +5845,7 @@
         <v>1.618038913971178</v>
       </c>
       <c r="AG52" t="n">
-        <v>-12.23436757134561</v>
+        <v>-12.2959537000667</v>
       </c>
     </row>
     <row r="53">
@@ -5933,13 +5933,13 @@
         <v>0.1288691737888855</v>
       </c>
       <c r="AB53" t="n">
-        <v>-0.2325434165080062</v>
+        <v>-0.3338712546352632</v>
       </c>
       <c r="AC53" t="n">
         <v>-0.1476485834892379</v>
       </c>
       <c r="AD53" t="n">
-        <v>1.550463975336909</v>
+        <v>0.8411691084461106</v>
       </c>
       <c r="AE53" t="n">
         <v>-11.3042439117639</v>
@@ -5948,7 +5948,7 @@
         <v>3.654086850256318</v>
       </c>
       <c r="AG53" t="n">
-        <v>-6.099693086170669</v>
+        <v>-6.808987953061466</v>
       </c>
     </row>
     <row r="54">
@@ -6036,13 +6036,13 @@
         <v>0.01346263243114153</v>
       </c>
       <c r="AB54" t="n">
-        <v>-0.1267900032507412</v>
+        <v>-0.3526427880242517</v>
       </c>
       <c r="AC54" t="n">
         <v>0.07631202673319253</v>
       </c>
       <c r="AD54" t="n">
-        <v>1.806574869856693</v>
+        <v>0.2256053764421199</v>
       </c>
       <c r="AE54" t="n">
         <v>-10.95383022351939</v>
@@ -6051,7 +6051,7 @@
         <v>2.478154303234481</v>
       </c>
       <c r="AG54" t="n">
-        <v>-6.669101050428212</v>
+        <v>-8.250070543842785</v>
       </c>
     </row>
     <row r="55">
@@ -6139,13 +6139,13 @@
         <v>-0.001095090719234203</v>
       </c>
       <c r="AB55" t="n">
-        <v>-0.1896201388543599</v>
+        <v>-0.2464125002836758</v>
       </c>
       <c r="AC55" t="n">
         <v>-0.1023596181889312</v>
       </c>
       <c r="AD55" t="n">
-        <v>-2.199551322081558</v>
+        <v>-2.59709785208677</v>
       </c>
       <c r="AE55" t="n">
         <v>-12.69528876072049</v>
@@ -6154,7 +6154,7 @@
         <v>3.019378341784681</v>
       </c>
       <c r="AG55" t="n">
-        <v>-11.87546174101737</v>
+        <v>-12.27300827102258</v>
       </c>
     </row>
     <row r="56">
@@ -6242,13 +6242,13 @@
         <v>-0</v>
       </c>
       <c r="AB56" t="n">
-        <v>-0.1296495781779655</v>
+        <v>-0.3962041294550909</v>
       </c>
       <c r="AC56" t="n">
         <v>0.1065500901464023</v>
       </c>
       <c r="AD56" t="n">
-        <v>0.0660369882202221</v>
+        <v>-1.799844870719656</v>
       </c>
       <c r="AE56" t="n">
         <v>-11.47293217579436</v>
@@ -6257,7 +6257,7 @@
         <v>1.391759245545403</v>
       </c>
       <c r="AG56" t="n">
-        <v>-10.01513594202873</v>
+        <v>-11.88101780096861</v>
       </c>
     </row>
     <row r="57">
@@ -6345,13 +6345,13 @@
         <v>-0.00675583704793815</v>
       </c>
       <c r="AB57" t="n">
-        <v>-0.2647245741352404</v>
+        <v>-0.2746583752242959</v>
       </c>
       <c r="AC57" t="n">
         <v>-0.006678942190835382</v>
       </c>
       <c r="AD57" t="n">
-        <v>-2.272157707441588</v>
+        <v>-2.341694315064976</v>
       </c>
       <c r="AE57" t="n">
         <v>-11.13192123878857</v>
@@ -6360,7 +6360,7 @@
         <v>1.787457253412389</v>
       </c>
       <c r="AG57" t="n">
-        <v>-11.61662169281777</v>
+        <v>-11.68615830044116</v>
       </c>
     </row>
     <row r="58">
@@ -6448,13 +6448,13 @@
         <v>-0.003364740956888914</v>
       </c>
       <c r="AB58" t="n">
-        <v>-0.2171040137410161</v>
+        <v>-0.2597234112576138</v>
       </c>
       <c r="AC58" t="n">
         <v>0.07808724506113843</v>
       </c>
       <c r="AD58" t="n">
-        <v>1.910928805912604</v>
+        <v>1.61259302329642</v>
       </c>
       <c r="AE58" t="n">
         <v>-11.28390573792729</v>
@@ -6463,7 +6463,7 @@
         <v>3.426090643548985</v>
       </c>
       <c r="AG58" t="n">
-        <v>-5.946886288465697</v>
+        <v>-6.245222071081882</v>
       </c>
     </row>
     <row r="59">
@@ -6551,13 +6551,13 @@
         <v>0.02033884961310403</v>
       </c>
       <c r="AB59" t="n">
-        <v>-0.2067926779572891</v>
+        <v>-0.4200693917297115</v>
       </c>
       <c r="AC59" t="n">
         <v>-0.02650926173246486</v>
       </c>
       <c r="AD59" t="n">
-        <v>-1.457176037500283</v>
+        <v>-2.95011303390724</v>
       </c>
       <c r="AE59" t="n">
         <v>-13.60755576729628</v>
@@ -6566,7 +6566,7 @@
         <v>2.746127515958953</v>
       </c>
       <c r="AG59" t="n">
-        <v>-12.31860428883761</v>
+        <v>-13.81154128524457</v>
       </c>
     </row>
     <row r="60">
@@ -6654,13 +6654,13 @@
         <v>0.03819719000205478</v>
       </c>
       <c r="AB60" t="n">
-        <v>-0.02337881856957299</v>
+        <v>-0.2888850143619949</v>
       </c>
       <c r="AC60" t="n">
         <v>0.01581699255595311</v>
       </c>
       <c r="AD60" t="n">
-        <v>-0.6888531775598413</v>
+        <v>-2.547396548106795</v>
       </c>
       <c r="AE60" t="n">
         <v>-13.11686081229195</v>
@@ -6669,7 +6669,7 @@
         <v>1.450884836810187</v>
       </c>
       <c r="AG60" t="n">
-        <v>-12.3548291530416</v>
+        <v>-14.21337252358856</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the code - CalculateMicrobiomeRatio
</commit_message>
<xml_diff>
--- a/input/comp_mrs_cat.xlsx
+++ b/input/comp_mrs_cat.xlsx
@@ -686,7 +686,7 @@
         <v>-0.02253571108019671</v>
       </c>
       <c r="AD2" t="n">
-        <v>1.206763604850376</v>
+        <v>1.349324843968644</v>
       </c>
       <c r="AE2" t="n">
         <v>-10.71287134363504</v>
@@ -695,7 +695,7 @@
         <v>3.253217425700312</v>
       </c>
       <c r="AG2" t="n">
-        <v>-6.252890313084356</v>
+        <v>-6.110329073966087</v>
       </c>
     </row>
     <row r="3">
@@ -789,7 +789,7 @@
         <v>0.05145483745961987</v>
       </c>
       <c r="AD3" t="n">
-        <v>-0.6618273521133181</v>
+        <v>0.1790125063937677</v>
       </c>
       <c r="AE3" t="n">
         <v>-14.58010571514267</v>
@@ -798,7 +798,7 @@
         <v>1.848962917049874</v>
       </c>
       <c r="AG3" t="n">
-        <v>-13.39297015020611</v>
+        <v>-12.55213029169902</v>
       </c>
     </row>
     <row r="4">
@@ -892,7 +892,7 @@
         <v>-0.02311568454788574</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.2403117847406054</v>
+        <v>0.3251491368039667</v>
       </c>
       <c r="AE4" t="n">
         <v>-10.59408744031139</v>
@@ -901,7 +901,7 @@
         <v>3.84770481406579</v>
       </c>
       <c r="AG4" t="n">
-        <v>-6.506070841504995</v>
+        <v>-6.421233489441632</v>
       </c>
     </row>
     <row r="5">
@@ -995,7 +995,7 @@
         <v>-0.03391007751123196</v>
       </c>
       <c r="AD5" t="n">
-        <v>-0.3813231726682013</v>
+        <v>1.295364897130082</v>
       </c>
       <c r="AE5" t="n">
         <v>-10.19873570115378</v>
@@ -1004,7 +1004,7 @@
         <v>3.641193771392695</v>
       </c>
       <c r="AG5" t="n">
-        <v>-6.938865102429284</v>
+        <v>-5.262177032631001</v>
       </c>
     </row>
     <row r="6">
@@ -1098,7 +1098,7 @@
         <v>-0.1156702884233157</v>
       </c>
       <c r="AD6" t="n">
-        <v>-2.311836642690182</v>
+        <v>0.2573768658608793</v>
       </c>
       <c r="AE6" t="n">
         <v>-14.38470400851906</v>
@@ -1107,7 +1107,7 @@
         <v>2.756894535999121</v>
       </c>
       <c r="AG6" t="n">
-        <v>-13.93964611521012</v>
+        <v>-11.37043260665906</v>
       </c>
     </row>
     <row r="7">
@@ -1201,7 +1201,7 @@
         <v>0.01656407546583211</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.06352804711987661</v>
+        <v>0.6643901723454653</v>
       </c>
       <c r="AE7" t="n">
         <v>-12.52251865458284</v>
@@ -1210,7 +1210,7 @@
         <v>3.119152271531618</v>
       </c>
       <c r="AG7" t="n">
-        <v>-9.339838335931347</v>
+        <v>-8.738976210705758</v>
       </c>
     </row>
     <row r="8">
@@ -1304,7 +1304,7 @@
         <v>0.03658320797548056</v>
       </c>
       <c r="AD8" t="n">
-        <v>-2.613140207894537</v>
+        <v>0.0154326596133041</v>
       </c>
       <c r="AE8" t="n">
         <v>-15.0921182512653</v>
@@ -1313,7 +1313,7 @@
         <v>1.785537558360071</v>
       </c>
       <c r="AG8" t="n">
-        <v>-15.91972090079977</v>
+        <v>-13.29114803329192</v>
       </c>
     </row>
     <row r="9">
@@ -1407,7 +1407,7 @@
         <v>-0.0257802155774243</v>
       </c>
       <c r="AD9" t="n">
-        <v>-2.476898309927298</v>
+        <v>0.5184410162249959</v>
       </c>
       <c r="AE9" t="n">
         <v>-12.25232032141117</v>
@@ -1416,7 +1416,7 @@
         <v>3.004803121989122</v>
       </c>
       <c r="AG9" t="n">
-        <v>-11.72441550934934</v>
+        <v>-8.72907618319705</v>
       </c>
     </row>
     <row r="10">
@@ -1510,7 +1510,7 @@
         <v>-0.02989159533577808</v>
       </c>
       <c r="AD10" t="n">
-        <v>-2.080484820666785</v>
+        <v>0.3700482611681618</v>
       </c>
       <c r="AE10" t="n">
         <v>-13.43421122439342</v>
@@ -1519,7 +1519,7 @@
         <v>2.468263610591526</v>
       </c>
       <c r="AG10" t="n">
-        <v>-13.04643243446868</v>
+        <v>-10.59589935263373</v>
       </c>
     </row>
     <row r="11">
@@ -1613,7 +1613,7 @@
         <v>0.005491268636792317</v>
       </c>
       <c r="AD11" t="n">
-        <v>-1.873029929308267</v>
+        <v>0.2454642123782856</v>
       </c>
       <c r="AE11" t="n">
         <v>-11.93731123504216</v>
@@ -1622,7 +1622,7 @@
         <v>1.21525785660293</v>
       </c>
       <c r="AG11" t="n">
-        <v>-12.5950833077475</v>
+        <v>-10.47658916606095</v>
       </c>
     </row>
     <row r="12">
@@ -1716,7 +1716,7 @@
         <v>0.0860694672710957</v>
       </c>
       <c r="AD12" t="n">
-        <v>-1.541874255089881</v>
+        <v>0.05169514222383378</v>
       </c>
       <c r="AE12" t="n">
         <v>-11.69034257985</v>
@@ -1725,7 +1725,7 @@
         <v>1.398649254021426</v>
       </c>
       <c r="AG12" t="n">
-        <v>-11.83356758091845</v>
+        <v>-10.23999818360474</v>
       </c>
     </row>
     <row r="13">
@@ -1819,7 +1819,7 @@
         <v>-0.01425994787852184</v>
       </c>
       <c r="AD13" t="n">
-        <v>-0.8796961801374111</v>
+        <v>0.3448120709288106</v>
       </c>
       <c r="AE13" t="n">
         <v>-12.74396681066839</v>
@@ -1828,7 +1828,7 @@
         <v>2.326473128727222</v>
       </c>
       <c r="AG13" t="n">
-        <v>-11.29718986207859</v>
+        <v>-10.07268161101236</v>
       </c>
     </row>
     <row r="14">
@@ -1922,7 +1922,7 @@
         <v>0.01950246349247608</v>
       </c>
       <c r="AD14" t="n">
-        <v>-0.7163682132542064</v>
+        <v>-0.2355492703904264</v>
       </c>
       <c r="AE14" t="n">
         <v>-9.882164425305898</v>
@@ -1931,7 +1931,7 @@
         <v>3.297158965890005</v>
       </c>
       <c r="AG14" t="n">
-        <v>-7.301373672670099</v>
+        <v>-6.820554729806321</v>
       </c>
     </row>
     <row r="15">
@@ -2025,7 +2025,7 @@
         <v>-0.08801296918238558</v>
       </c>
       <c r="AD15" t="n">
-        <v>-1.897432208837434</v>
+        <v>0.9472263598682301</v>
       </c>
       <c r="AE15" t="n">
         <v>-11.80059150596449</v>
@@ -2034,7 +2034,7 @@
         <v>2.713662913782229</v>
       </c>
       <c r="AG15" t="n">
-        <v>-10.98436080101969</v>
+        <v>-8.139702232314026</v>
       </c>
     </row>
     <row r="16">
@@ -2128,7 +2128,7 @@
         <v>0.02343061746642033</v>
       </c>
       <c r="AD16" t="n">
-        <v>-1.276173450199792</v>
+        <v>0.2141670668851253</v>
       </c>
       <c r="AE16" t="n">
         <v>-11.54009724639915</v>
@@ -2137,7 +2137,7 @@
         <v>2.176770978233852</v>
       </c>
       <c r="AG16" t="n">
-        <v>-10.63949971836509</v>
+        <v>-9.14915920128017</v>
       </c>
     </row>
     <row r="17">
@@ -2231,7 +2231,7 @@
         <v>0.01266755913370944</v>
       </c>
       <c r="AD17" t="n">
-        <v>-1.758261383858426</v>
+        <v>0.5258243701171119</v>
       </c>
       <c r="AE17" t="n">
         <v>-15.37674820929016</v>
@@ -2240,7 +2240,7 @@
         <v>2.79833508502352</v>
       </c>
       <c r="AG17" t="n">
-        <v>-14.33667450812506</v>
+        <v>-12.05258875414952</v>
       </c>
     </row>
     <row r="18">
@@ -2334,7 +2334,7 @@
         <v>-0.1048208634132849</v>
       </c>
       <c r="AD18" t="n">
-        <v>-2.177232989355285</v>
+        <v>0.1833057836558002</v>
       </c>
       <c r="AE18" t="n">
         <v>-13.42280115001057</v>
@@ -2343,7 +2343,7 @@
         <v>2.289331898834243</v>
       </c>
       <c r="AG18" t="n">
-        <v>-13.31070224053161</v>
+        <v>-10.95016346752053</v>
       </c>
     </row>
     <row r="19">
@@ -2437,7 +2437,7 @@
         <v>0.01469753701812776</v>
       </c>
       <c r="AD19" t="n">
-        <v>-2.215781303349771</v>
+        <v>0.1283109762246061</v>
       </c>
       <c r="AE19" t="n">
         <v>-12.11501624570678</v>
@@ -2446,7 +2446,7 @@
         <v>1.034388269386078</v>
       </c>
       <c r="AG19" t="n">
-        <v>-13.29640927967048</v>
+        <v>-10.9523170000961</v>
       </c>
     </row>
     <row r="20">
@@ -2540,7 +2540,7 @@
         <v>0.07552317554046717</v>
       </c>
       <c r="AD20" t="n">
-        <v>2.487862376675363</v>
+        <v>0.2181686601032652</v>
       </c>
       <c r="AE20" t="n">
         <v>-13.73356444982923</v>
@@ -2549,7 +2549,7 @@
         <v>2.367888785783177</v>
       </c>
       <c r="AG20" t="n">
-        <v>-8.877813287370689</v>
+        <v>-11.14750700394278</v>
       </c>
     </row>
     <row r="21">
@@ -2643,7 +2643,7 @@
         <v>0.06652481685425474</v>
       </c>
       <c r="AD21" t="n">
-        <v>-0.4919399957999145</v>
+        <v>0.12262271326239</v>
       </c>
       <c r="AE21" t="n">
         <v>-13.21489960443659</v>
@@ -2652,7 +2652,7 @@
         <v>2.496649824908592</v>
       </c>
       <c r="AG21" t="n">
-        <v>-11.21018977532791</v>
+        <v>-10.5956270662656</v>
       </c>
     </row>
     <row r="22">
@@ -2746,7 +2746,7 @@
         <v>-0.01791581281148704</v>
       </c>
       <c r="AD22" t="n">
-        <v>2.276278044530738</v>
+        <v>0.08755629789200478</v>
       </c>
       <c r="AE22" t="n">
         <v>-12.23345658516506</v>
@@ -2755,7 +2755,7 @@
         <v>3.276139743624471</v>
       </c>
       <c r="AG22" t="n">
-        <v>-6.681038797009853</v>
+        <v>-8.869760543648585</v>
       </c>
     </row>
     <row r="23">
@@ -2849,7 +2849,7 @@
         <v>-0.01723232483948973</v>
       </c>
       <c r="AD23" t="n">
-        <v>-0.4408995922747213</v>
+        <v>0.2539916717785259</v>
       </c>
       <c r="AE23" t="n">
         <v>-11.5992000271969</v>
@@ -2858,7 +2858,7 @@
         <v>3.149142237757889</v>
       </c>
       <c r="AG23" t="n">
-        <v>-8.890957381713731</v>
+        <v>-8.196066117660484</v>
       </c>
     </row>
     <row r="24">
@@ -2952,7 +2952,7 @@
         <v>0.02140151786384475</v>
       </c>
       <c r="AD24" t="n">
-        <v>-0.9493067988182872</v>
+        <v>0.9667243371685512</v>
       </c>
       <c r="AE24" t="n">
         <v>-11.46661957331528</v>
@@ -2961,7 +2961,7 @@
         <v>2.480869506725185</v>
       </c>
       <c r="AG24" t="n">
-        <v>-9.935056865408384</v>
+        <v>-8.019025729421545</v>
       </c>
     </row>
     <row r="25">
@@ -3055,7 +3055,7 @@
         <v>-0.1252764488401676</v>
       </c>
       <c r="AD25" t="n">
-        <v>-1.330942454033567</v>
+        <v>0.8735024107446513</v>
       </c>
       <c r="AE25" t="n">
         <v>-9.98027283460573</v>
@@ -3064,7 +3064,7 @@
         <v>3.828349514488567</v>
       </c>
       <c r="AG25" t="n">
-        <v>-7.48286577415073</v>
+        <v>-5.278420909372512</v>
       </c>
     </row>
     <row r="26">
@@ -3158,7 +3158,7 @@
         <v>-0.005562017600533308</v>
       </c>
       <c r="AD26" t="n">
-        <v>-0.07271006184924378</v>
+        <v>0.6485321294332147</v>
       </c>
       <c r="AE26" t="n">
         <v>-14.51851968851755</v>
@@ -3167,7 +3167,7 @@
         <v>1.907476798064713</v>
       </c>
       <c r="AG26" t="n">
-        <v>-12.68375295230208</v>
+        <v>-11.96251076101962</v>
       </c>
     </row>
     <row r="27">
@@ -3261,7 +3261,7 @@
         <v>-0.004944895094070909</v>
       </c>
       <c r="AD27" t="n">
-        <v>-1.810393508255256</v>
+        <v>0.7147900127387261</v>
       </c>
       <c r="AE27" t="n">
         <v>-12.01886751273979</v>
@@ -3270,7 +3270,7 @@
         <v>2.030937895387919</v>
       </c>
       <c r="AG27" t="n">
-        <v>-11.79832312560712</v>
+        <v>-9.273139604613139</v>
       </c>
     </row>
     <row r="28">
@@ -3364,7 +3364,7 @@
         <v>-0.0566012107196378</v>
       </c>
       <c r="AD28" t="n">
-        <v>-1.292425142566827</v>
+        <v>1.21651060392319</v>
       </c>
       <c r="AE28" t="n">
         <v>-15.37167225364937</v>
@@ -3373,7 +3373,7 @@
         <v>2.79206825249104</v>
       </c>
       <c r="AG28" t="n">
-        <v>-13.87202914372516</v>
+        <v>-11.36309339723514</v>
       </c>
     </row>
     <row r="29">
@@ -3467,7 +3467,7 @@
         <v>-0.1544274508518571</v>
       </c>
       <c r="AD29" t="n">
-        <v>-2.804973297146931</v>
+        <v>-0.1278783053910493</v>
       </c>
       <c r="AE29" t="n">
         <v>-13.5241701207883</v>
@@ -3476,7 +3476,7 @@
         <v>3.83664770245198</v>
       </c>
       <c r="AG29" t="n">
-        <v>-12.49249571548325</v>
+        <v>-9.815400723727365</v>
       </c>
     </row>
     <row r="30">
@@ -3570,7 +3570,7 @@
         <v>-0.01375837472189369</v>
       </c>
       <c r="AD30" t="n">
-        <v>-4.644302866457737</v>
+        <v>-1.28158685972077</v>
       </c>
       <c r="AE30" t="n">
         <v>-11.49508205430502</v>
@@ -3579,7 +3579,7 @@
         <v>2.233250709367881</v>
       </c>
       <c r="AG30" t="n">
-        <v>-13.90613421139488</v>
+        <v>-10.54341820465791</v>
       </c>
     </row>
     <row r="31">
@@ -3673,7 +3673,7 @@
         <v>-0.09324834772141333</v>
       </c>
       <c r="AD31" t="n">
-        <v>-1.240277177657472</v>
+        <v>0.7622049139410226</v>
       </c>
       <c r="AE31" t="n">
         <v>-13.10995632210551</v>
@@ -3682,7 +3682,7 @@
         <v>3.068661166125489</v>
       </c>
       <c r="AG31" t="n">
-        <v>-11.2815723336375</v>
+        <v>-9.279090242039002</v>
       </c>
     </row>
     <row r="32">
@@ -3776,7 +3776,7 @@
         <v>-0.03038792594645022</v>
       </c>
       <c r="AD32" t="n">
-        <v>-3.813562732736394</v>
+        <v>-0.7800801661261121</v>
       </c>
       <c r="AE32" t="n">
         <v>-12.15714777458812</v>
@@ -3785,7 +3785,7 @@
         <v>2.843440208312904</v>
       </c>
       <c r="AG32" t="n">
-        <v>-13.12727029901161</v>
+        <v>-10.09378773240133</v>
       </c>
     </row>
     <row r="33">
@@ -3879,7 +3879,7 @@
         <v>0.01458613964633884</v>
       </c>
       <c r="AD33" t="n">
-        <v>-0.2745048171169281</v>
+        <v>0.6516771192456889</v>
       </c>
       <c r="AE33" t="n">
         <v>-12.95483354674426</v>
@@ -3888,7 +3888,7 @@
         <v>3.343456731499479</v>
       </c>
       <c r="AG33" t="n">
-        <v>-9.885881632361704</v>
+        <v>-8.959699695999088</v>
       </c>
     </row>
     <row r="34">
@@ -3982,7 +3982,7 @@
         <v>-0.01172553878460611</v>
       </c>
       <c r="AD34" t="n">
-        <v>1.062250868309531</v>
+        <v>0.2036337351286908</v>
       </c>
       <c r="AE34" t="n">
         <v>-11.43590039691728</v>
@@ -3991,7 +3991,7 @@
         <v>2.584924633664547</v>
       </c>
       <c r="AG34" t="n">
-        <v>-7.788724894943198</v>
+        <v>-8.647342028124038</v>
       </c>
     </row>
     <row r="35">
@@ -4085,7 +4085,7 @@
         <v>-0.01210242488285608</v>
       </c>
       <c r="AD35" t="n">
-        <v>0.3916166776330529</v>
+        <v>0.7926442020663729</v>
       </c>
       <c r="AE35" t="n">
         <v>-13.36936733974361</v>
@@ -4094,7 +4094,7 @@
         <v>2.633644577255411</v>
       </c>
       <c r="AG35" t="n">
-        <v>-10.34410608485515</v>
+        <v>-9.943078560421824</v>
       </c>
     </row>
     <row r="36">
@@ -4188,7 +4188,7 @@
         <v>-0.04310079228356984</v>
       </c>
       <c r="AD36" t="n">
-        <v>-2.216615054129072</v>
+        <v>0.6496091768848999</v>
       </c>
       <c r="AE36" t="n">
         <v>-15.49813795156405</v>
@@ -4197,7 +4197,7 @@
         <v>2.909579690590713</v>
       </c>
       <c r="AG36" t="n">
-        <v>-14.80517331510241</v>
+        <v>-11.93894908408843</v>
       </c>
     </row>
     <row r="37">
@@ -4291,7 +4291,7 @@
         <v>0.07903386814482644</v>
       </c>
       <c r="AD37" t="n">
-        <v>0.05280274697743949</v>
+        <v>0.05582418165583897</v>
       </c>
       <c r="AE37" t="n">
         <v>-12.66543848325756</v>
@@ -4300,7 +4300,7 @@
         <v>3.157693416302038</v>
       </c>
       <c r="AG37" t="n">
-        <v>-9.454942319978079</v>
+        <v>-9.45192088529968</v>
       </c>
     </row>
     <row r="38">
@@ -4394,7 +4394,7 @@
         <v>-0.1835343718749725</v>
       </c>
       <c r="AD38" t="n">
-        <v>-2.37291360622711</v>
+        <v>0.2055341294371552</v>
       </c>
       <c r="AE38" t="n">
         <v>-13.61467158714544</v>
@@ -4403,7 +4403,7 @@
         <v>3.432658560789324</v>
       </c>
       <c r="AG38" t="n">
-        <v>-12.55492663258322</v>
+        <v>-9.976478896918959</v>
       </c>
     </row>
     <row r="39">
@@ -4497,7 +4497,7 @@
         <v>0.1465525741500207</v>
       </c>
       <c r="AD39" t="n">
-        <v>-0.7057648713668029</v>
+        <v>0.04042874502368653</v>
       </c>
       <c r="AE39" t="n">
         <v>-14.47207605144228</v>
@@ -4506,7 +4506,7 @@
         <v>1.700090545577031</v>
       </c>
       <c r="AG39" t="n">
-        <v>-13.47775037723206</v>
+        <v>-12.73155676084157</v>
       </c>
     </row>
     <row r="40">
@@ -4600,7 +4600,7 @@
         <v>0.05222368188633728</v>
       </c>
       <c r="AD40" t="n">
-        <v>1.059623716409263</v>
+        <v>1.581307269299106</v>
       </c>
       <c r="AE40" t="n">
         <v>-10.88123827321872</v>
@@ -4609,7 +4609,7 @@
         <v>3.031725283185861</v>
       </c>
       <c r="AG40" t="n">
-        <v>-6.789889273623598</v>
+        <v>-6.268205720733754</v>
       </c>
     </row>
     <row r="41">
@@ -4703,7 +4703,7 @@
         <v>0.1243715227320841</v>
       </c>
       <c r="AD41" t="n">
-        <v>-0.513950080483028</v>
+        <v>0.05606475215748565</v>
       </c>
       <c r="AE41" t="n">
         <v>-14.66525189983984</v>
@@ -4712,7 +4712,7 @@
         <v>1.76104150121723</v>
       </c>
       <c r="AG41" t="n">
-        <v>-13.41816047910564</v>
+        <v>-12.84814564646513</v>
       </c>
     </row>
     <row r="42">
@@ -4806,7 +4806,7 @@
         <v>-0.1240316426625881</v>
       </c>
       <c r="AD42" t="n">
-        <v>-1.817004594972412</v>
+        <v>0.5120571413802395</v>
       </c>
       <c r="AE42" t="n">
         <v>-13.7896516881348</v>
@@ -4815,7 +4815,7 @@
         <v>2.407429868159737</v>
       </c>
       <c r="AG42" t="n">
-        <v>-13.19922641494747</v>
+        <v>-10.87016467859482</v>
       </c>
     </row>
     <row r="43">
@@ -4909,7 +4909,7 @@
         <v>-0.03817945356419498</v>
       </c>
       <c r="AD43" t="n">
-        <v>0.7646933332672882</v>
+        <v>1.171238522772072</v>
       </c>
       <c r="AE43" t="n">
         <v>-12.91365853710254</v>
@@ -4918,7 +4918,7 @@
         <v>2.816984400016397</v>
       </c>
       <c r="AG43" t="n">
-        <v>-9.331980803818851</v>
+        <v>-8.925435614314068</v>
       </c>
     </row>
     <row r="44">
@@ -5012,7 +5012,7 @@
         <v>0.03989310575973623</v>
       </c>
       <c r="AD44" t="n">
-        <v>-0.9323822980461995</v>
+        <v>0.04952614163671054</v>
       </c>
       <c r="AE44" t="n">
         <v>-12.58299944621622</v>
@@ -5021,7 +5021,7 @@
         <v>2.105639746971739</v>
       </c>
       <c r="AG44" t="n">
-        <v>-11.40974199729068</v>
+        <v>-10.42783355760777</v>
       </c>
     </row>
     <row r="45">
@@ -5115,7 +5115,7 @@
         <v>0.003968274312813186</v>
       </c>
       <c r="AD45" t="n">
-        <v>-0.2571485131976691</v>
+        <v>0.7465755421807339</v>
       </c>
       <c r="AE45" t="n">
         <v>-12.0595945518373</v>
@@ -5124,7 +5124,7 @@
         <v>3.293796111048356</v>
       </c>
       <c r="AG45" t="n">
-        <v>-9.022946953986615</v>
+        <v>-8.019222898608213</v>
       </c>
     </row>
     <row r="46">
@@ -5218,7 +5218,7 @@
         <v>0.04526844422307467</v>
       </c>
       <c r="AD46" t="n">
-        <v>0.2742320430889965</v>
+        <v>0.6797772062528168</v>
       </c>
       <c r="AE46" t="n">
         <v>-14.02068089885143</v>
@@ -5227,7 +5227,7 @@
         <v>2.395329167291155</v>
       </c>
       <c r="AG46" t="n">
-        <v>-11.35111968847128</v>
+        <v>-10.94557452530746</v>
       </c>
     </row>
     <row r="47">
@@ -5321,7 +5321,7 @@
         <v>-0.08771332036010683</v>
       </c>
       <c r="AD47" t="n">
-        <v>-2.401087641333458</v>
+        <v>0.3458254045777432</v>
       </c>
       <c r="AE47" t="n">
         <v>-13.76433087242771</v>
@@ -5330,7 +5330,7 @@
         <v>2.57710761741724</v>
       </c>
       <c r="AG47" t="n">
-        <v>-13.58831089634392</v>
+        <v>-10.84139785043272</v>
       </c>
     </row>
     <row r="48">
@@ -5424,7 +5424,7 @@
         <v>0.01171826334382941</v>
       </c>
       <c r="AD48" t="n">
-        <v>-2.018414950201884</v>
+        <v>0.02688030345492576</v>
       </c>
       <c r="AE48" t="n">
         <v>-13.58696023262923</v>
@@ -5433,7 +5433,7 @@
         <v>2.375564778330544</v>
       </c>
       <c r="AG48" t="n">
-        <v>-13.22981040450057</v>
+        <v>-11.18451515084376</v>
       </c>
     </row>
     <row r="49">
@@ -5527,7 +5527,7 @@
         <v>-0.01100958685467849</v>
       </c>
       <c r="AD49" t="n">
-        <v>2.560831682811852</v>
+        <v>0.04137663367350292</v>
       </c>
       <c r="AE49" t="n">
         <v>-11.44494132331521</v>
@@ -5536,7 +5536,7 @@
         <v>2.725849737383146</v>
       </c>
       <c r="AG49" t="n">
-        <v>-6.158259903120213</v>
+        <v>-8.677714952258562</v>
       </c>
     </row>
     <row r="50">
@@ -5630,7 +5630,7 @@
         <v>-0.1035686816929112</v>
       </c>
       <c r="AD50" t="n">
-        <v>-1.457118660769562</v>
+        <v>0.6863028741057466</v>
       </c>
       <c r="AE50" t="n">
         <v>-11.06433018238832</v>
@@ -5639,7 +5639,7 @@
         <v>2.96434199520753</v>
       </c>
       <c r="AG50" t="n">
-        <v>-9.557106847950354</v>
+        <v>-7.413685313075046</v>
       </c>
     </row>
     <row r="51">
@@ -5733,7 +5733,7 @@
         <v>0.01446724075091104</v>
       </c>
       <c r="AD51" t="n">
-        <v>-1.960033407080617</v>
+        <v>0.1862437341284388</v>
       </c>
       <c r="AE51" t="n">
         <v>-9.811596911047625</v>
@@ -5742,7 +5742,7 @@
         <v>1.394942178171137</v>
       </c>
       <c r="AG51" t="n">
-        <v>-10.37668813995711</v>
+        <v>-8.230410998748049</v>
       </c>
     </row>
     <row r="52">
@@ -5836,7 +5836,7 @@
         <v>-0.05476918884983398</v>
       </c>
       <c r="AD52" t="n">
-        <v>-1.390947525765934</v>
+        <v>0.4312064758209718</v>
       </c>
       <c r="AE52" t="n">
         <v>-12.52304508827194</v>
@@ -5845,7 +5845,7 @@
         <v>1.618038913971178</v>
       </c>
       <c r="AG52" t="n">
-        <v>-12.2959537000667</v>
+        <v>-10.47379969847979</v>
       </c>
     </row>
     <row r="53">
@@ -5939,7 +5939,7 @@
         <v>-0.1476485834892379</v>
       </c>
       <c r="AD53" t="n">
-        <v>0.8411691084461106</v>
+        <v>-0.1669175544610551</v>
       </c>
       <c r="AE53" t="n">
         <v>-11.3042439117639</v>
@@ -5948,7 +5948,7 @@
         <v>3.654086850256318</v>
       </c>
       <c r="AG53" t="n">
-        <v>-6.808987953061466</v>
+        <v>-7.817074615968632</v>
       </c>
     </row>
     <row r="54">
@@ -6042,7 +6042,7 @@
         <v>0.07631202673319253</v>
       </c>
       <c r="AD54" t="n">
-        <v>0.2256053764421199</v>
+        <v>0.04286757755881693</v>
       </c>
       <c r="AE54" t="n">
         <v>-10.95383022351939</v>
@@ -6051,7 +6051,7 @@
         <v>2.478154303234481</v>
       </c>
       <c r="AG54" t="n">
-        <v>-8.250070543842785</v>
+        <v>-8.432808342726089</v>
       </c>
     </row>
     <row r="55">
@@ -6145,7 +6145,7 @@
         <v>-0.1023596181889312</v>
       </c>
       <c r="AD55" t="n">
-        <v>-2.59709785208677</v>
+        <v>0.06375664783978777</v>
       </c>
       <c r="AE55" t="n">
         <v>-12.69528876072049</v>
@@ -6154,7 +6154,7 @@
         <v>3.019378341784681</v>
       </c>
       <c r="AG55" t="n">
-        <v>-12.27300827102258</v>
+        <v>-9.612153771096022</v>
       </c>
     </row>
     <row r="56">
@@ -6248,7 +6248,7 @@
         <v>0.1065500901464023</v>
       </c>
       <c r="AD56" t="n">
-        <v>-1.799844870719656</v>
+        <v>-0.02842617464579093</v>
       </c>
       <c r="AE56" t="n">
         <v>-11.47293217579436</v>
@@ -6257,7 +6257,7 @@
         <v>1.391759245545403</v>
       </c>
       <c r="AG56" t="n">
-        <v>-11.88101780096861</v>
+        <v>-10.10959910489474</v>
       </c>
     </row>
     <row r="57">
@@ -6351,7 +6351,7 @@
         <v>-0.006678942190835382</v>
       </c>
       <c r="AD57" t="n">
-        <v>-2.341694315064976</v>
+        <v>0.1535286260219229</v>
       </c>
       <c r="AE57" t="n">
         <v>-11.13192123878857</v>
@@ -6360,7 +6360,7 @@
         <v>1.787457253412389</v>
       </c>
       <c r="AG57" t="n">
-        <v>-11.68615830044116</v>
+        <v>-9.190935359354258</v>
       </c>
     </row>
     <row r="58">
@@ -6454,7 +6454,7 @@
         <v>0.07808724506113843</v>
       </c>
       <c r="AD58" t="n">
-        <v>1.61259302329642</v>
+        <v>-0.002499888651234683</v>
       </c>
       <c r="AE58" t="n">
         <v>-11.28390573792729</v>
@@ -6463,7 +6463,7 @@
         <v>3.426090643548985</v>
       </c>
       <c r="AG58" t="n">
-        <v>-6.245222071081882</v>
+        <v>-7.860314983029536</v>
       </c>
     </row>
     <row r="59">
@@ -6557,7 +6557,7 @@
         <v>-0.02650926173246486</v>
       </c>
       <c r="AD59" t="n">
-        <v>-2.95011303390724</v>
+        <v>-0.651592177382373</v>
       </c>
       <c r="AE59" t="n">
         <v>-13.60755576729628</v>
@@ -6566,7 +6566,7 @@
         <v>2.746127515958953</v>
       </c>
       <c r="AG59" t="n">
-        <v>-13.81154128524457</v>
+        <v>-11.5130204287197</v>
       </c>
     </row>
     <row r="60">
@@ -6660,7 +6660,7 @@
         <v>0.01581699255595311</v>
       </c>
       <c r="AD60" t="n">
-        <v>-2.547396548106795</v>
+        <v>0.1918172034293323</v>
       </c>
       <c r="AE60" t="n">
         <v>-13.11686081229195</v>
@@ -6669,7 +6669,7 @@
         <v>1.450884836810187</v>
       </c>
       <c r="AG60" t="n">
-        <v>-14.21337252358856</v>
+        <v>-11.47415877205243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>